<commit_message>
Ithink e R estão alinhados até o tempo 4.37 - Variável Value of Backlog
</commit_message>
<xml_diff>
--- a/models/dissertation-model/modelo-ithink/dados_ithink_excel_checks.xlsx
+++ b/models/dissertation-model/modelo-ithink/dados_ithink_excel_checks.xlsx
@@ -470,7 +470,7 @@
         <v>101904</v>
       </c>
       <c r="H2" s="3">
-        <v>765.92250000000001</v>
+        <v>1051.875</v>
       </c>
       <c r="I2">
         <v>181.81818200000001</v>
@@ -489,13 +489,13 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>171864.18927900001</v>
       </c>
       <c r="C3">
         <v>100000</v>
       </c>
       <c r="D3">
-        <v>7198.8</v>
+        <v>179062.989279</v>
       </c>
       <c r="E3">
         <v>101904</v>
@@ -504,10 +504,10 @@
         <v>101904</v>
       </c>
       <c r="G3">
-        <v>7198.8</v>
+        <v>179062.989279</v>
       </c>
       <c r="H3">
-        <v>765.671604</v>
+        <v>1062.151953</v>
       </c>
       <c r="I3">
         <v>181.758623</v>
@@ -524,25 +524,25 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>193290.18431400001</v>
       </c>
       <c r="C4">
         <v>100000</v>
       </c>
       <c r="D4">
-        <v>8382.6149999999998</v>
+        <v>201672.799314</v>
       </c>
       <c r="E4">
-        <v>54551.4</v>
+        <v>101904</v>
       </c>
       <c r="F4">
         <v>101904</v>
       </c>
       <c r="G4">
-        <v>8382.6149999999998</v>
+        <v>201672.799314</v>
       </c>
       <c r="H4">
-        <v>758.02695100000005</v>
+        <v>1180.0350989999999</v>
       </c>
       <c r="I4">
         <v>181.69912199999999</v>
@@ -559,31 +559,31 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>217376.29083000001</v>
       </c>
       <c r="C5">
         <v>100000</v>
       </c>
       <c r="D5">
-        <v>8959.7248130000007</v>
+        <v>226927.92314299999</v>
       </c>
       <c r="E5">
-        <v>31467.0075</v>
+        <v>107077.03125</v>
       </c>
       <c r="F5">
         <v>101904</v>
       </c>
       <c r="G5">
-        <v>8959.7248130000007</v>
+        <v>226927.92314299999</v>
       </c>
       <c r="H5">
-        <v>754.29022199999997</v>
+        <v>1304.2992400000001</v>
       </c>
       <c r="I5">
-        <v>181.667293</v>
+        <v>181.63967700000001</v>
       </c>
       <c r="J5">
-        <v>605.55764199999999</v>
+        <v>605.46559100000002</v>
       </c>
       <c r="AP5" s="1"/>
       <c r="AQ5" s="1"/>
@@ -594,31 +594,31 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>0</v>
+        <v>244449.84577099999</v>
       </c>
       <c r="C6">
         <v>100000</v>
       </c>
       <c r="D6">
-        <v>9241.0658459999995</v>
+        <v>255220.54556999999</v>
       </c>
       <c r="E6">
-        <v>20213.366156</v>
+        <v>116776.464844</v>
       </c>
       <c r="F6">
         <v>101904</v>
       </c>
       <c r="G6">
-        <v>9241.0658459999995</v>
+        <v>255220.54556999999</v>
       </c>
       <c r="H6">
-        <v>752.45727699999998</v>
+        <v>1417.917027</v>
       </c>
       <c r="I6">
-        <v>181.64894000000001</v>
+        <v>181.57727700000001</v>
       </c>
       <c r="J6">
-        <v>605.49646700000005</v>
+        <v>605.25759100000005</v>
       </c>
       <c r="AP6" s="1"/>
       <c r="AQ6" s="1"/>
@@ -629,31 +629,31 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>0</v>
+        <v>274877.68993699999</v>
       </c>
       <c r="C7">
         <v>100000</v>
       </c>
       <c r="D7">
-        <v>9378.2196000000004</v>
+        <v>286973.46179899998</v>
       </c>
       <c r="E7">
-        <v>14727.216001000001</v>
+        <v>128900.756836</v>
       </c>
       <c r="F7">
         <v>101904</v>
       </c>
       <c r="G7">
-        <v>9378.2196000000004</v>
+        <v>286973.46179899998</v>
       </c>
       <c r="H7">
-        <v>751.552097</v>
+        <v>1522.025627</v>
       </c>
       <c r="I7">
-        <v>181.63715400000001</v>
+        <v>181.509297</v>
       </c>
       <c r="J7">
-        <v>605.45717999999999</v>
+        <v>605.03098799999998</v>
       </c>
       <c r="AP7" s="1"/>
       <c r="AQ7" s="1"/>
@@ -664,31 +664,31 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>0</v>
+        <v>309070.72880400001</v>
       </c>
       <c r="C8">
         <v>100000</v>
       </c>
       <c r="D8">
-        <v>9445.0820550000008</v>
+        <v>322626.56297799997</v>
       </c>
       <c r="E8">
-        <v>12052.717801000001</v>
+        <v>141530.22766100001</v>
       </c>
       <c r="F8">
         <v>101904</v>
       </c>
       <c r="G8">
-        <v>9445.0820550000008</v>
+        <v>322626.56297799997</v>
       </c>
       <c r="H8">
-        <v>751.09911699999998</v>
+        <v>1626.5646549999999</v>
       </c>
       <c r="I8">
-        <v>181.628568</v>
+        <v>181.43434500000001</v>
       </c>
       <c r="J8">
-        <v>605.42856099999995</v>
+        <v>604.78114900000003</v>
       </c>
       <c r="AP8" s="1"/>
       <c r="AQ8" s="1"/>
@@ -699,31 +699,31 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>0</v>
+        <v>347488.964331</v>
       </c>
       <c r="C9">
-        <v>100000</v>
+        <v>109760.10640800001</v>
       </c>
       <c r="D9">
-        <v>9477.6775020000005</v>
+        <v>362644.47842399997</v>
       </c>
       <c r="E9">
-        <v>10748.899928000001</v>
+        <v>153370.35655999999</v>
       </c>
       <c r="F9">
         <v>101904</v>
       </c>
       <c r="G9">
-        <v>9477.6775020000005</v>
+        <v>362644.47842399997</v>
       </c>
       <c r="H9">
-        <v>750.86656200000004</v>
+        <v>1737.869731</v>
       </c>
       <c r="I9">
-        <v>181.621543</v>
+        <v>181.35215400000001</v>
       </c>
       <c r="J9">
-        <v>605.40514199999996</v>
+        <v>604.50717999999995</v>
       </c>
       <c r="AP9" s="1"/>
       <c r="AQ9" s="1"/>
@@ -734,31 +734,31 @@
         <v>1000</v>
       </c>
       <c r="B10">
-        <v>0</v>
+        <v>390647.03099900001</v>
       </c>
       <c r="C10">
-        <v>100000</v>
+        <v>142685.32686599999</v>
       </c>
       <c r="D10">
-        <v>9493.5677820000001</v>
+        <v>407530.23062300001</v>
       </c>
       <c r="E10">
-        <v>10113.288715000001</v>
+        <v>163730.469346</v>
       </c>
       <c r="F10">
         <v>101904</v>
       </c>
       <c r="G10">
-        <v>9493.5677820000001</v>
+        <v>407530.23062300001</v>
       </c>
       <c r="H10">
-        <v>750.74145799999997</v>
+        <v>1863.0536480000001</v>
       </c>
       <c r="I10">
-        <v>181.61527799999999</v>
+        <v>181.26321100000001</v>
       </c>
       <c r="J10">
-        <v>605.38425800000005</v>
+        <v>604.21070299999997</v>
       </c>
       <c r="AP10" s="1"/>
       <c r="AQ10" s="1"/>
@@ -769,31 +769,31 @@
         <v>1125</v>
       </c>
       <c r="B11">
-        <v>0</v>
+        <v>439120.26697400003</v>
       </c>
       <c r="C11">
-        <v>100000</v>
+        <v>162970.581913</v>
       </c>
       <c r="D11">
-        <v>9501.3142939999998</v>
+        <v>457839.05746899999</v>
       </c>
       <c r="E11">
-        <v>9803.4282480000002</v>
+        <v>172363.896668</v>
       </c>
       <c r="F11">
         <v>101904</v>
       </c>
       <c r="G11">
-        <v>9501.3142939999998</v>
+        <v>457839.05746899999</v>
       </c>
       <c r="H11">
-        <v>750.66873399999997</v>
+        <v>2026.1708799999999</v>
       </c>
       <c r="I11">
-        <v>181.60938400000001</v>
+        <v>181.16840099999999</v>
       </c>
       <c r="J11">
-        <v>605.36461199999997</v>
+        <v>603.89467200000001</v>
       </c>
       <c r="AP11" s="1"/>
       <c r="AQ11" s="1"/>
@@ -804,31 +804,31 @@
         <v>1250</v>
       </c>
       <c r="B12">
-        <v>0</v>
+        <v>493551.347067</v>
       </c>
       <c r="C12">
-        <v>100000</v>
+        <v>181048.50354800001</v>
       </c>
       <c r="D12">
-        <v>9505.0907179999995</v>
+        <v>514190.70138899999</v>
       </c>
       <c r="E12">
-        <v>9652.371271</v>
+        <v>180330.85841700001</v>
       </c>
       <c r="F12">
         <v>101904</v>
       </c>
       <c r="G12">
-        <v>9505.0907179999995</v>
+        <v>514190.70138899999</v>
       </c>
       <c r="H12">
-        <v>750.62154499999997</v>
+        <v>2215.3209029999998</v>
       </c>
       <c r="I12">
-        <v>181.60367099999999</v>
+        <v>181.06874999999999</v>
       </c>
       <c r="J12">
-        <v>605.34556899999995</v>
+        <v>603.562501</v>
       </c>
       <c r="AP12" s="1"/>
       <c r="AQ12" s="1"/>
@@ -839,31 +839,31 @@
         <v>1375</v>
       </c>
       <c r="B13">
-        <v>0</v>
+        <v>554657.49748500006</v>
       </c>
       <c r="C13">
-        <v>100000</v>
+        <v>198485.382859</v>
       </c>
       <c r="D13">
-        <v>9506.9317250000004</v>
+        <v>577292.99560899998</v>
       </c>
       <c r="E13">
-        <v>9578.7309949999999</v>
+        <v>191153.52030999999</v>
       </c>
       <c r="F13">
-        <v>60052.334032999999</v>
+        <v>101904</v>
       </c>
       <c r="G13">
-        <v>9506.9317250000004</v>
+        <v>577292.99560899998</v>
       </c>
       <c r="H13">
-        <v>750.58680600000002</v>
+        <v>2402.6394329999998</v>
       </c>
       <c r="I13">
-        <v>181.59804600000001</v>
+        <v>180.964665</v>
       </c>
       <c r="J13">
-        <v>605.326821</v>
+        <v>603.215552</v>
       </c>
       <c r="AP13" s="1"/>
       <c r="AQ13" s="1"/>
@@ -874,31 +874,31 @@
         <v>1500</v>
       </c>
       <c r="B14">
-        <v>0</v>
+        <v>623238.30241600005</v>
       </c>
       <c r="C14">
-        <v>100000</v>
+        <v>212936.272616</v>
       </c>
       <c r="D14">
-        <v>9507.8292160000001</v>
+        <v>647980.27581699996</v>
       </c>
       <c r="E14">
-        <v>9542.8313600000001</v>
+        <v>206356.95889499999</v>
       </c>
       <c r="F14">
-        <v>29520.256451000001</v>
+        <v>107142.681893</v>
       </c>
       <c r="G14">
-        <v>9507.8292160000001</v>
+        <v>647980.27581699996</v>
       </c>
       <c r="H14">
-        <v>750.55813599999999</v>
+        <v>2570.611868</v>
       </c>
       <c r="I14">
-        <v>181.592465</v>
+        <v>180.85452599999999</v>
       </c>
       <c r="J14">
-        <v>605.30821800000001</v>
+        <v>602.84842000000003</v>
       </c>
       <c r="AP14" s="1"/>
       <c r="AQ14" s="1"/>
@@ -909,31 +909,31 @@
         <v>1625</v>
       </c>
       <c r="B15">
-        <v>0</v>
+        <v>700184.09840899997</v>
       </c>
       <c r="C15">
-        <v>100000</v>
+        <v>227874.70408900001</v>
       </c>
       <c r="D15">
-        <v>9508.2667430000001</v>
+        <v>727196.25912800001</v>
       </c>
       <c r="E15">
-        <v>9525.3302879999992</v>
+        <v>226032.31415399999</v>
       </c>
       <c r="F15">
-        <v>13822.106279</v>
+        <v>120110.78231900001</v>
       </c>
       <c r="G15">
-        <v>9508.2667430000001</v>
+        <v>727196.25912800001</v>
       </c>
       <c r="H15">
-        <v>750.53242699999998</v>
+        <v>2713.4104950000001</v>
       </c>
       <c r="I15">
-        <v>181.586906</v>
+        <v>180.735848</v>
       </c>
       <c r="J15">
-        <v>605.28968699999996</v>
+        <v>602.45282599999996</v>
       </c>
       <c r="AP15" s="1"/>
       <c r="AQ15" s="1"/>
@@ -944,31 +944,31 @@
         <v>1750</v>
       </c>
       <c r="B16">
-        <v>0</v>
+        <v>786484.93315499998</v>
       </c>
       <c r="C16">
-        <v>100000</v>
+        <v>247722.50809600001</v>
       </c>
       <c r="D16">
-        <v>9508.4800369999994</v>
+        <v>815984.84579199995</v>
       </c>
       <c r="E16">
-        <v>9516.7985150000004</v>
+        <v>249588.37297699999</v>
       </c>
       <c r="F16">
-        <v>6699.5756899999997</v>
+        <v>140761.53909400001</v>
       </c>
       <c r="G16">
-        <v>9508.4800369999994</v>
+        <v>815984.84579199995</v>
       </c>
       <c r="H16">
-        <v>750.50816099999997</v>
+        <v>2835.6150299999999</v>
       </c>
       <c r="I16">
-        <v>181.581357</v>
+        <v>180.60611700000001</v>
       </c>
       <c r="J16">
-        <v>605.27119100000004</v>
+        <v>602.02038900000002</v>
       </c>
       <c r="AP16" s="1"/>
       <c r="AQ16" s="1"/>
@@ -979,31 +979,31 @@
         <v>1875</v>
       </c>
       <c r="B17">
-        <v>0</v>
+        <v>883240.039185</v>
       </c>
       <c r="C17">
-        <v>100000</v>
+        <v>275088.38520600001</v>
       </c>
       <c r="D17">
-        <v>9508.5840179999996</v>
+        <v>915491.057577</v>
       </c>
       <c r="E17">
-        <v>9512.6392759999999</v>
+        <v>275934.82060199999</v>
       </c>
       <c r="F17">
-        <v>3576.472424</v>
+        <v>167501.53512700001</v>
       </c>
       <c r="G17">
-        <v>9508.5840179999996</v>
+        <v>915491.057577</v>
       </c>
       <c r="H17">
-        <v>750.484601</v>
+        <v>2948.9450470000002</v>
       </c>
       <c r="I17">
-        <v>181.57581400000001</v>
+        <v>180.46318400000001</v>
       </c>
       <c r="J17">
-        <v>605.25271299999997</v>
+        <v>601.54394600000001</v>
       </c>
       <c r="AP17" s="1"/>
       <c r="AQ17" s="1"/>
@@ -1014,31 +1014,31 @@
         <v>2000</v>
       </c>
       <c r="B18">
-        <v>0</v>
+        <v>991667.73864</v>
       </c>
       <c r="C18">
-        <v>100000</v>
+        <v>310206.039254</v>
       </c>
       <c r="D18">
-        <v>9508.6347089999999</v>
+        <v>1026964.804559</v>
       </c>
       <c r="E18">
-        <v>9510.6116469999997</v>
+        <v>304108.74469199998</v>
       </c>
       <c r="F18">
-        <v>2184.4208279999998</v>
+        <v>197899.02905700001</v>
       </c>
       <c r="G18">
-        <v>9508.6347089999999</v>
+        <v>1026964.804559</v>
       </c>
       <c r="H18">
-        <v>750.46138499999995</v>
+        <v>3064.3852489999999</v>
       </c>
       <c r="I18">
-        <v>181.57027299999999</v>
+        <v>180.30555000000001</v>
       </c>
       <c r="J18">
-        <v>605.23424499999999</v>
+        <v>601.01849900000002</v>
       </c>
       <c r="AP18" s="1"/>
       <c r="AQ18" s="1"/>
@@ -1049,31 +1049,31 @@
         <v>2125</v>
       </c>
       <c r="B19">
-        <v>0</v>
+        <v>1113115.650563</v>
       </c>
       <c r="C19">
-        <v>100000</v>
+        <v>352746.44090500002</v>
       </c>
       <c r="D19">
-        <v>9508.6594210000003</v>
+        <v>1151772.862467</v>
       </c>
       <c r="E19">
-        <v>9509.6231779999998</v>
+        <v>333904.42305099999</v>
       </c>
       <c r="F19">
-        <v>1537.370596</v>
+        <v>229325.98005899999</v>
       </c>
       <c r="G19">
-        <v>9508.6594210000003</v>
+        <v>1151772.862467</v>
       </c>
       <c r="H19">
-        <v>750.43833800000004</v>
+        <v>3186.011512</v>
       </c>
       <c r="I19">
-        <v>181.56473500000001</v>
+        <v>180.13228899999999</v>
       </c>
       <c r="J19">
-        <v>605.21578199999999</v>
+        <v>600.44096300000001</v>
       </c>
       <c r="AP19" s="1"/>
       <c r="AQ19" s="1"/>
@@ -1084,31 +1084,31 @@
         <v>2250</v>
       </c>
       <c r="B20">
-        <v>0</v>
+        <v>1249071.0148769999</v>
       </c>
       <c r="C20">
-        <v>100000</v>
+        <v>403600.15466900001</v>
       </c>
       <c r="D20">
-        <v>9508.6714680000005</v>
+        <v>1291418.8169199999</v>
       </c>
       <c r="E20">
-        <v>9509.1412990000008</v>
+        <v>366073.48572300002</v>
       </c>
       <c r="F20">
-        <v>1222.1840319999999</v>
+        <v>259501.79286799999</v>
       </c>
       <c r="G20">
-        <v>9508.6714680000005</v>
+        <v>1291418.8169199999</v>
       </c>
       <c r="H20">
-        <v>750.41537500000004</v>
+        <v>3310.1269010000001</v>
       </c>
       <c r="I20">
-        <v>181.55919700000001</v>
+        <v>179.94261599999999</v>
       </c>
       <c r="J20">
-        <v>605.19732399999998</v>
+        <v>599.80872099999999</v>
       </c>
       <c r="AP20" s="1"/>
       <c r="AQ20" s="1"/>
@@ -1119,31 +1119,31 @@
         <v>2375</v>
       </c>
       <c r="B21">
-        <v>0</v>
+        <v>1401170.874693</v>
       </c>
       <c r="C21">
-        <v>100000</v>
+        <v>463301.49364599999</v>
       </c>
       <c r="D21">
-        <v>9508.6773400000002</v>
+        <v>1447565.2477820001</v>
       </c>
       <c r="E21">
-        <v>9508.9063829999996</v>
+        <v>402055.88216699997</v>
       </c>
       <c r="F21">
-        <v>1384.2746959999999</v>
+        <v>288539.20272100001</v>
       </c>
       <c r="G21">
-        <v>9508.6773400000002</v>
+        <v>1447565.2477820001</v>
       </c>
       <c r="H21">
-        <v>750.39245300000005</v>
+        <v>3428.875822</v>
       </c>
       <c r="I21">
-        <v>181.55366000000001</v>
+        <v>179.735344</v>
       </c>
       <c r="J21">
-        <v>605.17886699999997</v>
+        <v>599.11781299999996</v>
       </c>
       <c r="AP21" s="1"/>
       <c r="AQ21" s="1"/>
@@ -1154,31 +1154,31 @@
         <v>2500</v>
       </c>
       <c r="B22">
-        <v>0</v>
+        <v>1571211.7679000001</v>
       </c>
       <c r="C22">
-        <v>100000</v>
+        <v>527374.90674600005</v>
       </c>
       <c r="D22">
-        <v>9508.6802029999999</v>
+        <v>1622051.909853</v>
       </c>
       <c r="E22">
-        <v>9508.791862</v>
+        <v>443585.773705</v>
       </c>
       <c r="F22">
-        <v>1820.4923470000001</v>
+        <v>314618.61945400003</v>
       </c>
       <c r="G22">
-        <v>9508.6802029999999</v>
+        <v>1622051.909853</v>
       </c>
       <c r="H22">
-        <v>750.369553</v>
+        <v>3534.4978059999999</v>
       </c>
       <c r="I22">
-        <v>181.548124</v>
+        <v>179.50850600000001</v>
       </c>
       <c r="J22">
-        <v>605.16041299999995</v>
+        <v>598.36168699999996</v>
       </c>
       <c r="AP22" s="1"/>
       <c r="AQ22" s="1"/>
@@ -1189,31 +1189,31 @@
         <v>2625</v>
       </c>
       <c r="B23">
-        <v>0</v>
+        <v>1761158.466946</v>
       </c>
       <c r="C23">
-        <v>100000</v>
+        <v>595175.55753700004</v>
       </c>
       <c r="D23">
-        <v>9508.6815989999996</v>
+        <v>1816907.9292959999</v>
       </c>
       <c r="E23">
-        <v>9508.7360329999992</v>
+        <v>492504.70219600003</v>
       </c>
       <c r="F23">
-        <v>2542.125055</v>
+        <v>339609.07299800002</v>
       </c>
       <c r="G23">
-        <v>9508.6815989999996</v>
+        <v>1816907.9292959999</v>
       </c>
       <c r="H23">
-        <v>750.34666500000003</v>
+        <v>3619.2750820000001</v>
       </c>
       <c r="I23">
-        <v>181.54258799999999</v>
+        <v>179.25921199999999</v>
       </c>
       <c r="J23">
-        <v>605.14196100000004</v>
+        <v>597.53070700000001</v>
       </c>
       <c r="AP23" s="1"/>
       <c r="AQ23" s="1"/>
@@ -1224,31 +1224,31 @@
         <v>2750</v>
       </c>
       <c r="B24">
-        <v>0</v>
+        <v>1973151.169037</v>
       </c>
       <c r="C24">
-        <v>100000</v>
+        <v>670258.055192</v>
       </c>
       <c r="D24">
-        <v>9508.6822800000009</v>
+        <v>2034360.071885</v>
       </c>
       <c r="E24">
-        <v>9508.7088160000003</v>
+        <v>550641.241821</v>
       </c>
       <c r="F24">
-        <v>3561.3865369999999</v>
+        <v>367982.542976</v>
       </c>
       <c r="G24">
-        <v>9508.6822800000009</v>
+        <v>2034360.071885</v>
       </c>
       <c r="H24">
-        <v>750.32378300000005</v>
+        <v>3678.049344</v>
       </c>
       <c r="I24">
-        <v>181.53705299999999</v>
+        <v>178.98361600000001</v>
       </c>
       <c r="J24">
-        <v>605.12351100000001</v>
+        <v>596.61205500000005</v>
       </c>
       <c r="AP24" s="1"/>
       <c r="AQ24" s="1"/>
@@ -1259,31 +1259,31 @@
         <v>2875</v>
       </c>
       <c r="B25">
-        <v>0</v>
+        <v>2209510.374485</v>
       </c>
       <c r="C25">
-        <v>100000</v>
+        <v>758959.60954500001</v>
       </c>
       <c r="D25">
-        <v>9508.6826110000002</v>
+        <v>2276837.1815709998</v>
       </c>
       <c r="E25">
-        <v>9508.6955479999997</v>
+        <v>619217.26075899997</v>
       </c>
       <c r="F25">
-        <v>4809.0234899999996</v>
+        <v>404061.97965300002</v>
       </c>
       <c r="G25">
-        <v>9508.6826110000002</v>
+        <v>2276837.1815709998</v>
       </c>
       <c r="H25">
-        <v>750.30090499999994</v>
+        <v>3711.8561399999999</v>
       </c>
       <c r="I25">
-        <v>181.531519</v>
+        <v>178.67696000000001</v>
       </c>
       <c r="J25">
-        <v>605.10506199999998</v>
+        <v>595.58986800000002</v>
       </c>
       <c r="AP25" s="1"/>
       <c r="AQ25" s="1"/>
@@ -1294,31 +1294,31 @@
         <v>3000</v>
       </c>
       <c r="B26">
-        <v>0</v>
+        <v>2472738.4960309998</v>
       </c>
       <c r="C26">
-        <v>100000</v>
+        <v>868119.83534300001</v>
       </c>
       <c r="D26">
-        <v>9508.6827730000005</v>
+        <v>2546963.9337869999</v>
       </c>
       <c r="E26">
-        <v>9508.6890800000001</v>
+        <v>698762.48655699997</v>
       </c>
       <c r="F26">
-        <v>6109.1798040000003</v>
+        <v>450195.82123</v>
       </c>
       <c r="G26">
-        <v>9508.6827730000005</v>
+        <v>2546963.9337869999</v>
       </c>
       <c r="H26">
-        <v>750.27803100000006</v>
+        <v>3726.6646300000002</v>
       </c>
       <c r="I26">
-        <v>181.52598399999999</v>
+        <v>178.33395400000001</v>
       </c>
       <c r="J26">
-        <v>605.08661500000005</v>
+        <v>594.44651499999998</v>
       </c>
       <c r="AP26" s="1"/>
       <c r="AQ26" s="1"/>
@@ -1329,31 +1329,31 @@
         <v>3125</v>
       </c>
       <c r="B27">
-        <v>0</v>
+        <v>2765517.0149369999</v>
       </c>
       <c r="C27">
-        <v>100000</v>
+        <v>1002868.1386909999</v>
       </c>
       <c r="D27">
-        <v>9508.6828519999999</v>
+        <v>2847549.1658029999</v>
       </c>
       <c r="E27">
-        <v>9508.6859260000001</v>
+        <v>789659.61103000003</v>
       </c>
       <c r="F27">
-        <v>7254.3496080000004</v>
+        <v>507295.06333899999</v>
       </c>
       <c r="G27">
-        <v>9508.6828519999999</v>
+        <v>2847549.1658029999</v>
       </c>
       <c r="H27">
-        <v>750.25515900000005</v>
+        <v>3728.9358179999999</v>
       </c>
       <c r="I27">
-        <v>181.52045100000001</v>
+        <v>177.94920400000001</v>
       </c>
       <c r="J27">
-        <v>605.06816900000001</v>
+        <v>593.16401199999996</v>
       </c>
       <c r="AP27" s="1"/>
       <c r="AQ27" s="1"/>
@@ -1364,31 +1364,31 @@
         <v>3250</v>
       </c>
       <c r="B28">
-        <v>0</v>
+        <v>3090697.740925</v>
       </c>
       <c r="C28">
-        <v>100000</v>
+        <v>1166122.773509</v>
       </c>
       <c r="D28">
-        <v>9508.68289</v>
+        <v>3181575.235043</v>
       </c>
       <c r="E28">
-        <v>9508.684389</v>
+        <v>892972.09211900004</v>
       </c>
       <c r="F28">
-        <v>8119.728822</v>
+        <v>576527.65540499997</v>
       </c>
       <c r="G28">
-        <v>9508.68289</v>
+        <v>3181575.235043</v>
       </c>
       <c r="H28">
-        <v>750.23228900000004</v>
+        <v>3721.791737</v>
       </c>
       <c r="I28">
-        <v>181.51491799999999</v>
+        <v>177.51732999999999</v>
       </c>
       <c r="J28">
-        <v>605.04972599999996</v>
+        <v>591.72443499999997</v>
       </c>
       <c r="AP28" s="1"/>
       <c r="AQ28" s="1"/>
@@ -1399,31 +1399,31 @@
         <v>3375</v>
       </c>
       <c r="B29">
-        <v>0</v>
+        <v>3451286.445632</v>
       </c>
       <c r="C29">
-        <v>100000</v>
+        <v>1359844.6740649999</v>
       </c>
       <c r="D29">
-        <v>9508.6829089999992</v>
+        <v>3552190.1222250001</v>
       </c>
       <c r="E29">
-        <v>9508.6836399999993</v>
+        <v>1011096.140126</v>
       </c>
       <c r="F29">
-        <v>8698.6673719999999</v>
+        <v>658905.02261900005</v>
       </c>
       <c r="G29">
-        <v>9508.6829089999992</v>
+        <v>3552190.1222250001</v>
       </c>
       <c r="H29">
-        <v>750.20942200000002</v>
+        <v>3704.002086</v>
       </c>
       <c r="I29">
-        <v>181.50938500000001</v>
+        <v>177.03265200000001</v>
       </c>
       <c r="J29">
-        <v>605.03128400000003</v>
+        <v>590.10883999999999</v>
       </c>
       <c r="AP29" s="1"/>
       <c r="AQ29" s="1"/>
@@ -1434,31 +1434,31 @@
         <v>3500</v>
       </c>
       <c r="B30">
-        <v>0</v>
+        <v>3850416.8310890002</v>
       </c>
       <c r="C30">
-        <v>100000</v>
+        <v>1587229.2235719999</v>
       </c>
       <c r="D30">
-        <v>9508.6829180000004</v>
+        <v>3962697.9134760001</v>
       </c>
       <c r="E30">
-        <v>9508.6832740000009</v>
+        <v>1147912.8322600001</v>
       </c>
       <c r="F30">
-        <v>9053.7898499999992</v>
+        <v>751352.43670700002</v>
       </c>
       <c r="G30">
-        <v>9508.6829180000004</v>
+        <v>3962697.9134760001</v>
       </c>
       <c r="H30">
-        <v>750.18655699999999</v>
+        <v>3671.6601730000002</v>
       </c>
       <c r="I30">
-        <v>181.50385299999999</v>
+        <v>176.48853399999999</v>
       </c>
       <c r="J30">
-        <v>605.01284299999998</v>
+        <v>588.29511200000002</v>
       </c>
       <c r="AP30" s="1"/>
       <c r="AQ30" s="1"/>
@@ -1469,31 +1469,31 @@
         <v>3625</v>
       </c>
       <c r="B31">
-        <v>0</v>
+        <v>4291312.4795639999</v>
       </c>
       <c r="C31">
-        <v>100000</v>
+        <v>1854389.282107</v>
       </c>
       <c r="D31">
-        <v>9508.6829230000003</v>
+        <v>4416538.9588249996</v>
       </c>
       <c r="E31">
-        <v>9508.6830960000007</v>
+        <v>1308458.5472240001</v>
       </c>
       <c r="F31">
-        <v>9259.4857769999999</v>
+        <v>851816.664383</v>
       </c>
       <c r="G31">
-        <v>9508.6829230000003</v>
+        <v>4416538.9588249996</v>
       </c>
       <c r="H31">
-        <v>750.16369299999997</v>
+        <v>3620.95514</v>
       </c>
       <c r="I31">
-        <v>181.498321</v>
+        <v>175.87671499999999</v>
       </c>
       <c r="J31">
-        <v>604.99440400000003</v>
+        <v>586.255717</v>
       </c>
       <c r="AP31" s="1"/>
       <c r="AQ31" s="1"/>
@@ -1504,31 +1504,31 @@
         <v>3750</v>
       </c>
       <c r="B32">
-        <v>0</v>
+        <v>4777234.1318239998</v>
       </c>
       <c r="C32">
-        <v>100000</v>
+        <v>2170325.1464470001</v>
       </c>
       <c r="D32">
-        <v>9508.6829249999992</v>
+        <v>4917251.0119340001</v>
       </c>
       <c r="E32">
-        <v>9508.6830090000003</v>
+        <v>1498420.1872940001</v>
       </c>
       <c r="F32">
-        <v>9374.3669539999992</v>
+        <v>962114.77634500002</v>
       </c>
       <c r="G32">
-        <v>9508.6829249999992</v>
+        <v>4917251.0119340001</v>
       </c>
       <c r="H32">
-        <v>750.14083200000005</v>
+        <v>3550.2490969999999</v>
       </c>
       <c r="I32">
-        <v>181.49279000000001</v>
+        <v>175.18688499999999</v>
       </c>
       <c r="J32">
-        <v>604.97596699999997</v>
+        <v>583.95628199999999</v>
       </c>
       <c r="AP32" s="1"/>
       <c r="AQ32" s="1"/>
@@ -1541,31 +1541,31 @@
         <v>3875</v>
       </c>
       <c r="B33">
-        <v>0</v>
+        <v>5311409.3914069999</v>
       </c>
       <c r="C33">
-        <v>100000</v>
+        <v>2546127.8416240001</v>
       </c>
       <c r="D33">
-        <v>9508.6829259999995</v>
+        <v>5468406.3128570002</v>
       </c>
       <c r="E33">
-        <v>9508.6829670000006</v>
+        <v>1723843.229634</v>
       </c>
       <c r="F33">
-        <v>9437.069227</v>
+        <v>1088225.0758080001</v>
       </c>
       <c r="G33">
-        <v>9508.6829259999995</v>
+        <v>5468406.3128570002</v>
       </c>
       <c r="H33">
-        <v>750.11797300000001</v>
+        <v>3460.4371540000002</v>
       </c>
       <c r="I33">
-        <v>181.48725999999999</v>
+        <v>174.40660399999999</v>
       </c>
       <c r="J33">
-        <v>604.95753200000001</v>
+        <v>581.35534700000005</v>
       </c>
       <c r="AP33" s="1"/>
       <c r="AQ33" s="1"/>
@@ -1574,26 +1574,35 @@
       <c r="FV33" s="1"/>
     </row>
     <row r="34" spans="1:178" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>9</v>
+      <c r="A34" s="2">
+        <v>4000</v>
+      </c>
+      <c r="B34">
+        <v>5896941.8013220001</v>
       </c>
       <c r="C34">
-        <v>100000</v>
+        <v>2996983.0990769998</v>
+      </c>
+      <c r="D34">
+        <v>6073524.3016240001</v>
       </c>
       <c r="E34">
-        <v>9508.6829460000008</v>
+        <v>1991272.9056830001</v>
       </c>
       <c r="F34">
-        <v>9470.7890370000005</v>
+        <v>1238608.4061779999</v>
+      </c>
+      <c r="G34">
+        <v>6073524.3016240001</v>
       </c>
       <c r="H34">
-        <v>750.09511599999996</v>
+        <v>3353.882736</v>
       </c>
       <c r="I34">
-        <v>181.481729</v>
+        <v>173.521469</v>
       </c>
       <c r="J34">
-        <v>604.93909799999994</v>
+        <v>578.40489700000001</v>
       </c>
       <c r="AP34" s="1"/>
       <c r="AQ34" s="1"/>
@@ -1602,6 +1611,36 @@
       <c r="FV34" s="1"/>
     </row>
     <row r="35" spans="1:178" x14ac:dyDescent="0.25">
+      <c r="A35" s="2">
+        <v>4125</v>
+      </c>
+      <c r="B35">
+        <v>6536696.2520690002</v>
+      </c>
+      <c r="C35">
+        <v>3543871.7677859999</v>
+      </c>
+      <c r="D35">
+        <v>6735962.3824380003</v>
+      </c>
+      <c r="E35">
+        <v>2308234.634755</v>
+      </c>
+      <c r="F35">
+        <v>1421598.714042</v>
+      </c>
+      <c r="G35">
+        <v>6735962.3824380003</v>
+      </c>
+      <c r="H35">
+        <v>3233.2687289999999</v>
+      </c>
+      <c r="I35">
+        <v>172.51529500000001</v>
+      </c>
+      <c r="J35">
+        <v>575.05098199999998</v>
+      </c>
       <c r="AP35" s="1"/>
       <c r="AQ35" s="1"/>
       <c r="CA35" s="1"/>
@@ -1609,6 +1648,36 @@
       <c r="FV35" s="1"/>
     </row>
     <row r="36" spans="1:178" x14ac:dyDescent="0.25">
+      <c r="A36" s="2">
+        <v>4250</v>
+      </c>
+      <c r="B36">
+        <v>7233157.9406859996</v>
+      </c>
+      <c r="C36">
+        <v>4213487.4231470004</v>
+      </c>
+      <c r="D36">
+        <v>7458786.1773600001</v>
+      </c>
+      <c r="E36">
+        <v>2683814.0880999998</v>
+      </c>
+      <c r="F36">
+        <v>1643697.575828</v>
+      </c>
+      <c r="G36">
+        <v>7458786.1773600001</v>
+      </c>
+      <c r="H36">
+        <v>3101.0016599999999</v>
+      </c>
+      <c r="I36">
+        <v>171.370181</v>
+      </c>
+      <c r="J36">
+        <v>571.23393799999997</v>
+      </c>
       <c r="AP36" s="1"/>
       <c r="AQ36" s="1"/>
       <c r="CA36" s="1"/>
@@ -1616,6 +1685,36 @@
       <c r="FV36" s="1"/>
     </row>
     <row r="37" spans="1:178" x14ac:dyDescent="0.25">
+      <c r="A37" s="2">
+        <v>4375</v>
+      </c>
+      <c r="B37">
+        <v>7988262.7134159999</v>
+      </c>
+      <c r="C37">
+        <v>5036624.9804419996</v>
+      </c>
+      <c r="D37">
+        <v>8244618.2732330002</v>
+      </c>
+      <c r="E37">
+        <v>3129427.625554</v>
+      </c>
+      <c r="F37">
+        <v>1909724.5271660001</v>
+      </c>
+      <c r="G37">
+        <v>8244618.2732330002</v>
+      </c>
+      <c r="H37">
+        <v>2958.9345939999998</v>
+      </c>
+      <c r="I37">
+        <v>170.06646599999999</v>
+      </c>
+      <c r="J37">
+        <v>566.88822100000004</v>
+      </c>
       <c r="AP37" s="1"/>
       <c r="AQ37" s="1"/>
       <c r="CA37" s="1"/>
@@ -1623,6 +1722,36 @@
       <c r="FV37" s="1"/>
     </row>
     <row r="38" spans="1:178" x14ac:dyDescent="0.25">
+      <c r="A38" s="2">
+        <v>4500</v>
+      </c>
+      <c r="B38">
+        <v>8803197.7100699991</v>
+      </c>
+      <c r="C38">
+        <v>6047295.29954</v>
+      </c>
+      <c r="D38">
+        <v>9095466.6707090009</v>
+      </c>
+      <c r="E38">
+        <v>3659883.7353050001</v>
+      </c>
+      <c r="F38">
+        <v>2224645.6424400001</v>
+      </c>
+      <c r="G38">
+        <v>9095466.6707090009</v>
+      </c>
+      <c r="H38">
+        <v>2808.2765479999998</v>
+      </c>
+      <c r="I38">
+        <v>168.58254099999999</v>
+      </c>
+      <c r="J38">
+        <v>561.94180400000005</v>
+      </c>
       <c r="W38" s="1"/>
       <c r="X38" s="1"/>
       <c r="AP38" s="1"/>
@@ -1632,6 +1761,36 @@
       <c r="FV38" s="1"/>
     </row>
     <row r="39" spans="1:178" x14ac:dyDescent="0.25">
+      <c r="A39" s="2">
+        <v>4625</v>
+      </c>
+      <c r="B39">
+        <v>9678172.9151549991</v>
+      </c>
+      <c r="C39">
+        <v>7284899.6886710003</v>
+      </c>
+      <c r="D39">
+        <v>10012537.060477</v>
+      </c>
+      <c r="E39">
+        <v>4294603.3055140004</v>
+      </c>
+      <c r="F39">
+        <v>2595834.2469049999</v>
+      </c>
+      <c r="G39">
+        <v>10012537.060477</v>
+      </c>
+      <c r="H39">
+        <v>2649.777607</v>
+      </c>
+      <c r="I39">
+        <v>166.89451299999999</v>
+      </c>
+      <c r="J39">
+        <v>556.31504199999995</v>
+      </c>
       <c r="W39" s="1"/>
       <c r="X39" s="1"/>
       <c r="AP39" s="1"/>
@@ -1641,6 +1800,36 @@
       <c r="FV39" s="1"/>
     </row>
     <row r="40" spans="1:178" x14ac:dyDescent="0.25">
+      <c r="A40" s="2">
+        <v>4750</v>
+      </c>
+      <c r="B40">
+        <v>10612166.631957</v>
+      </c>
+      <c r="C40">
+        <v>8800079.3590479996</v>
+      </c>
+      <c r="D40">
+        <v>10996033.766782001</v>
+      </c>
+      <c r="E40">
+        <v>5058681.9028289998</v>
+      </c>
+      <c r="F40">
+        <v>3034177.2406100002</v>
+      </c>
+      <c r="G40">
+        <v>10996033.766782001</v>
+      </c>
+      <c r="H40">
+        <v>2484.1832199999999</v>
+      </c>
+      <c r="I40">
+        <v>164.97579400000001</v>
+      </c>
+      <c r="J40">
+        <v>549.91931299999999</v>
+      </c>
       <c r="S40" s="1"/>
       <c r="T40" s="1"/>
       <c r="W40" s="1"/>
@@ -1654,6 +1843,36 @@
       <c r="FV40" s="1"/>
     </row>
     <row r="41" spans="1:178" x14ac:dyDescent="0.25">
+      <c r="A41" s="2">
+        <v>4875</v>
+      </c>
+      <c r="B41">
+        <v>11602651.123087</v>
+      </c>
+      <c r="C41">
+        <v>10662530.328777</v>
+      </c>
+      <c r="D41">
+        <v>12044953.442511</v>
+      </c>
+      <c r="E41">
+        <v>5983617.2978440002</v>
+      </c>
+      <c r="F41">
+        <v>3553990.8936040001</v>
+      </c>
+      <c r="G41">
+        <v>12044953.442511</v>
+      </c>
+      <c r="H41">
+        <v>2312.704698</v>
+      </c>
+      <c r="I41">
+        <v>162.79690400000001</v>
+      </c>
+      <c r="J41">
+        <v>542.65634599999998</v>
+      </c>
       <c r="S41" s="1"/>
       <c r="T41" s="1"/>
       <c r="W41" s="1"/>
@@ -1667,6 +1886,36 @@
       <c r="FV41" s="1"/>
     </row>
     <row r="42" spans="1:178" x14ac:dyDescent="0.25">
+      <c r="A42" s="2">
+        <v>5000</v>
+      </c>
+      <c r="B42">
+        <v>12645308.730520001</v>
+      </c>
+      <c r="C42">
+        <v>12967815.108165</v>
+      </c>
+      <c r="D42">
+        <v>13156877.487175001</v>
+      </c>
+      <c r="E42">
+        <v>7107955.9777539996</v>
+      </c>
+      <c r="F42">
+        <v>4174581.9260630002</v>
+      </c>
+      <c r="G42">
+        <v>13156877.487175001</v>
+      </c>
+      <c r="H42">
+        <v>2137.2014450000001</v>
+      </c>
+      <c r="I42">
+        <v>160.32583099999999</v>
+      </c>
+      <c r="J42">
+        <v>534.41943700000002</v>
+      </c>
       <c r="S42" s="1"/>
       <c r="T42" s="1"/>
       <c r="W42" s="1"/>
@@ -1680,6 +1929,36 @@
       <c r="FV42" s="1"/>
     </row>
     <row r="43" spans="1:178" x14ac:dyDescent="0.25">
+      <c r="A43" s="2">
+        <v>5125</v>
+      </c>
+      <c r="B43">
+        <v>13733753.614492999</v>
+      </c>
+      <c r="C43">
+        <v>15841719.997556999</v>
+      </c>
+      <c r="D43">
+        <v>14327777.211412</v>
+      </c>
+      <c r="E43">
+        <v>8478529.0687099993</v>
+      </c>
+      <c r="F43">
+        <v>4922388.3772600004</v>
+      </c>
+      <c r="G43">
+        <v>14327777.211412</v>
+      </c>
+      <c r="H43">
+        <v>1959.987652</v>
+      </c>
+      <c r="I43">
+        <v>157.52917299999999</v>
+      </c>
+      <c r="J43">
+        <v>525.09724200000005</v>
+      </c>
       <c r="S43" s="1"/>
       <c r="T43" s="1"/>
       <c r="W43" s="1"/>
@@ -1693,6 +1972,36 @@
       <c r="FV43" s="1"/>
     </row>
     <row r="44" spans="1:178" x14ac:dyDescent="0.25">
+      <c r="A44" s="2">
+        <v>5250</v>
+      </c>
+      <c r="B44">
+        <v>14859279.582691001</v>
+      </c>
+      <c r="C44">
+        <v>19444594.949331999</v>
+      </c>
+      <c r="D44">
+        <v>15551859.498006999</v>
+      </c>
+      <c r="E44">
+        <v>10153013.904871</v>
+      </c>
+      <c r="F44">
+        <v>5831984.1271479996</v>
+      </c>
+      <c r="G44">
+        <v>15551859.498006999</v>
+      </c>
+      <c r="H44">
+        <v>1783.45146</v>
+      </c>
+      <c r="I44">
+        <v>154.373941</v>
+      </c>
+      <c r="J44">
+        <v>514.57980299999997</v>
+      </c>
       <c r="S44" s="1"/>
       <c r="T44" s="1"/>
       <c r="W44" s="1"/>
@@ -1706,6 +2015,36 @@
       <c r="FV44" s="1"/>
     </row>
     <row r="45" spans="1:178" x14ac:dyDescent="0.25">
+      <c r="A45" s="2">
+        <v>5375</v>
+      </c>
+      <c r="B45">
+        <v>16010659.849990999</v>
+      </c>
+      <c r="C45">
+        <v>23980597.849227</v>
+      </c>
+      <c r="D45">
+        <v>16821495.190177001</v>
+      </c>
+      <c r="E45">
+        <v>12204164.883809</v>
+      </c>
+      <c r="F45">
+        <v>6945292.0479269996</v>
+      </c>
+      <c r="G45">
+        <v>16821495.190177001</v>
+      </c>
+      <c r="H45">
+        <v>1609.764226</v>
+      </c>
+      <c r="I45">
+        <v>150.82970599999999</v>
+      </c>
+      <c r="J45">
+        <v>502.76568500000002</v>
+      </c>
       <c r="S45" s="1"/>
       <c r="T45" s="1"/>
       <c r="W45" s="1"/>
@@ -1719,6 +2058,36 @@
       <c r="FV45" s="1"/>
     </row>
     <row r="46" spans="1:178" x14ac:dyDescent="0.25">
+      <c r="A46" s="2">
+        <v>5500</v>
+      </c>
+      <c r="B46">
+        <v>17174029.248206999</v>
+      </c>
+      <c r="C46">
+        <v>29713438.8211</v>
+      </c>
+      <c r="D46">
+        <v>18127281.207688</v>
+      </c>
+      <c r="E46">
+        <v>14725505.779278999</v>
+      </c>
+      <c r="F46">
+        <v>8310482.2635960001</v>
+      </c>
+      <c r="G46">
+        <v>18127281.207688</v>
+      </c>
+      <c r="H46">
+        <v>1440.8149980000001</v>
+      </c>
+      <c r="I46">
+        <v>146.87073799999999</v>
+      </c>
+      <c r="J46">
+        <v>489.56912599999998</v>
+      </c>
       <c r="S46" s="1"/>
       <c r="T46" s="1"/>
       <c r="W46" s="1"/>
@@ -1732,6 +2101,36 @@
       <c r="FV46" s="1"/>
     </row>
     <row r="47" spans="1:178" x14ac:dyDescent="0.25">
+      <c r="A47" s="2">
+        <v>5625</v>
+      </c>
+      <c r="B47">
+        <v>18332882.408622999</v>
+      </c>
+      <c r="C47">
+        <v>36987339.769784003</v>
+      </c>
+      <c r="D47">
+        <v>19458287.540851001</v>
+      </c>
+      <c r="E47">
+        <v>17838127.896866001</v>
+      </c>
+      <c r="F47">
+        <v>9983160.8827350009</v>
+      </c>
+      <c r="G47">
+        <v>19458287.540851001</v>
+      </c>
+      <c r="H47">
+        <v>1278.292308</v>
+      </c>
+      <c r="I47">
+        <v>142.47809599999999</v>
+      </c>
+      <c r="J47">
+        <v>474.926987</v>
+      </c>
       <c r="S47" s="1"/>
       <c r="T47" s="1"/>
       <c r="W47" s="1"/>
@@ -1745,6 +2144,36 @@
       <c r="FV47" s="1"/>
     </row>
     <row r="48" spans="1:178" x14ac:dyDescent="0.25">
+      <c r="A48" s="2">
+        <v>5750</v>
+      </c>
+      <c r="B48">
+        <v>19468221.578322001</v>
+      </c>
+      <c r="C48">
+        <v>46252722.117463</v>
+      </c>
+      <c r="D48">
+        <v>20802535.745108001</v>
+      </c>
+      <c r="E48">
+        <v>21698773.843277</v>
+      </c>
+      <c r="F48">
+        <v>12031643.928606</v>
+      </c>
+      <c r="G48">
+        <v>20802535.745108001</v>
+      </c>
+      <c r="H48">
+        <v>1123.7610999999999</v>
+      </c>
+      <c r="I48">
+        <v>137.64180899999999</v>
+      </c>
+      <c r="J48">
+        <v>458.80602900000002</v>
+      </c>
       <c r="S48" s="1"/>
       <c r="T48" s="1"/>
       <c r="W48" s="1"/>
@@ -1757,7 +2186,37 @@
       <c r="CF48" s="1"/>
       <c r="FV48" s="1"/>
     </row>
-    <row r="49" spans="19:178" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:178" x14ac:dyDescent="0.25">
+      <c r="A49" s="2">
+        <v>5875</v>
+      </c>
+      <c r="B49">
+        <v>20558883.755279001</v>
+      </c>
+      <c r="C49">
+        <v>58100971.275187001</v>
+      </c>
+      <c r="D49">
+        <v>22147753.668021999</v>
+      </c>
+      <c r="E49">
+        <v>26510078.262063</v>
+      </c>
+      <c r="F49">
+        <v>14545846.227325</v>
+      </c>
+      <c r="G49">
+        <v>22147753.668021999</v>
+      </c>
+      <c r="H49">
+        <v>978.65978099999995</v>
+      </c>
+      <c r="I49">
+        <v>132.36324500000001</v>
+      </c>
+      <c r="J49">
+        <v>441.21081600000002</v>
+      </c>
       <c r="S49" s="1"/>
       <c r="T49" s="1"/>
       <c r="W49" s="1"/>
@@ -1770,7 +2229,37 @@
       <c r="CF49" s="1"/>
       <c r="FV49" s="1"/>
     </row>
-    <row r="50" spans="19:178" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:178" x14ac:dyDescent="0.25">
+      <c r="A50" s="2">
+        <v>6000</v>
+      </c>
+      <c r="B50">
+        <v>21582067.668582998</v>
+      </c>
+      <c r="C50">
+        <v>73316774.230162993</v>
+      </c>
+      <c r="D50">
+        <v>23482452.685692001</v>
+      </c>
+      <c r="E50">
+        <v>32534166.328692</v>
+      </c>
+      <c r="F50">
+        <v>17647175.200194001</v>
+      </c>
+      <c r="G50">
+        <v>23482452.685692001</v>
+      </c>
+      <c r="H50">
+        <v>844.23630200000002</v>
+      </c>
+      <c r="I50">
+        <v>126.657472</v>
+      </c>
+      <c r="J50">
+        <v>422.19157200000001</v>
+      </c>
       <c r="S50" s="1"/>
       <c r="T50" s="1"/>
       <c r="W50" s="1"/>
@@ -1783,7 +2272,37 @@
       <c r="CF50" s="1"/>
       <c r="FV50" s="1"/>
     </row>
-    <row r="51" spans="19:178" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:178" x14ac:dyDescent="0.25">
+      <c r="A51" s="2">
+        <v>6125</v>
+      </c>
+      <c r="B51">
+        <v>0</v>
+      </c>
+      <c r="C51">
+        <v>92955788.459819004</v>
+      </c>
+      <c r="D51">
+        <v>2283307.2835039999</v>
+      </c>
+      <c r="E51">
+        <v>40110832.896600999</v>
+      </c>
+      <c r="F51">
+        <v>21496963.598143</v>
+      </c>
+      <c r="G51">
+        <v>2283307.2835039999</v>
+      </c>
+      <c r="H51">
+        <v>721.47010299999999</v>
+      </c>
+      <c r="I51">
+        <v>120.55515</v>
+      </c>
+      <c r="J51">
+        <v>401.85050200000001</v>
+      </c>
       <c r="S51" s="1"/>
       <c r="T51" s="1"/>
       <c r="W51" s="1"/>
@@ -1796,7 +2315,37 @@
       <c r="CF51" s="1"/>
       <c r="FV51" s="1"/>
     </row>
-    <row r="52" spans="19:178" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:178" x14ac:dyDescent="0.25">
+      <c r="A52" s="2">
+        <v>6250</v>
+      </c>
+      <c r="B52">
+        <v>0</v>
+      </c>
+      <c r="C52">
+        <v>118450753.690322</v>
+      </c>
+      <c r="D52">
+        <v>2756151.3536669998</v>
+      </c>
+      <c r="E52">
+        <v>25957074.114291999</v>
+      </c>
+      <c r="F52">
+        <v>26304157.758536998</v>
+      </c>
+      <c r="G52">
+        <v>2756151.3536669998</v>
+      </c>
+      <c r="H52">
+        <v>567.04440099999999</v>
+      </c>
+      <c r="I52">
+        <v>114.103461</v>
+      </c>
+      <c r="J52">
+        <v>380.34487100000001</v>
+      </c>
       <c r="S52" s="1"/>
       <c r="T52" s="1"/>
       <c r="AP52" s="1"/>
@@ -1807,7 +2356,37 @@
       <c r="CF52" s="1"/>
       <c r="FV52" s="1"/>
     </row>
-    <row r="53" spans="19:178" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:178" x14ac:dyDescent="0.25">
+      <c r="A53" s="2">
+        <v>6375</v>
+      </c>
+      <c r="B53">
+        <v>0</v>
+      </c>
+      <c r="C53">
+        <v>63905657.705907002</v>
+      </c>
+      <c r="D53">
+        <v>3046162.888175</v>
+      </c>
+      <c r="E53">
+        <v>14356612.733979</v>
+      </c>
+      <c r="F53">
+        <v>32336557.158651002</v>
+      </c>
+      <c r="G53">
+        <v>3046162.888175</v>
+      </c>
+      <c r="H53">
+        <v>499.61269800000002</v>
+      </c>
+      <c r="I53">
+        <v>110.433053</v>
+      </c>
+      <c r="J53">
+        <v>368.11017700000002</v>
+      </c>
       <c r="S53" s="1"/>
       <c r="T53" s="1"/>
       <c r="AP53" s="1"/>
@@ -1818,7 +2397,37 @@
       <c r="CF53" s="1"/>
       <c r="FV53" s="1"/>
     </row>
-    <row r="54" spans="19:178" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:178" x14ac:dyDescent="0.25">
+      <c r="A54" s="2">
+        <v>6500</v>
+      </c>
+      <c r="B54">
+        <v>0</v>
+      </c>
+      <c r="C54">
+        <v>29211113.261381</v>
+      </c>
+      <c r="D54">
+        <v>3187543.511248</v>
+      </c>
+      <c r="E54">
+        <v>8701387.8110770006</v>
+      </c>
+      <c r="F54">
+        <v>39939029.636205003</v>
+      </c>
+      <c r="G54">
+        <v>3187543.511248</v>
+      </c>
+      <c r="H54">
+        <v>468.756844</v>
+      </c>
+      <c r="I54">
+        <v>108.546627</v>
+      </c>
+      <c r="J54">
+        <v>361.822091</v>
+      </c>
       <c r="S54" s="1"/>
       <c r="T54" s="1"/>
       <c r="AP54" s="1"/>
@@ -1829,7 +2438,37 @@
       <c r="CF54" s="1"/>
       <c r="FV54" s="1"/>
     </row>
-    <row r="55" spans="19:178" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:178" x14ac:dyDescent="0.25">
+      <c r="A55" s="2">
+        <v>6625</v>
+      </c>
+      <c r="B55">
+        <v>0</v>
+      </c>
+      <c r="C55">
+        <v>11782859.601066001</v>
+      </c>
+      <c r="D55">
+        <v>3256466.5649959999</v>
+      </c>
+      <c r="E55">
+        <v>5944465.6611630004</v>
+      </c>
+      <c r="F55">
+        <v>49559386.633928999</v>
+      </c>
+      <c r="G55">
+        <v>3256466.5649959999</v>
+      </c>
+      <c r="H55">
+        <v>454.53053899999998</v>
+      </c>
+      <c r="I55">
+        <v>107.44844399999999</v>
+      </c>
+      <c r="J55">
+        <v>358.16148199999998</v>
+      </c>
       <c r="S55" s="1"/>
       <c r="T55" s="1"/>
       <c r="AP55" s="1"/>
@@ -1840,7 +2479,37 @@
       <c r="CF55" s="1"/>
       <c r="FV55" s="1"/>
     </row>
-    <row r="56" spans="19:178" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:178" x14ac:dyDescent="0.25">
+      <c r="A56" s="2">
+        <v>6750</v>
+      </c>
+      <c r="B56">
+        <v>0</v>
+      </c>
+      <c r="C56">
+        <v>4682507.2004340002</v>
+      </c>
+      <c r="D56">
+        <v>3290066.553698</v>
+      </c>
+      <c r="E56">
+        <v>4600466.1130790003</v>
+      </c>
+      <c r="F56">
+        <v>61781871.010935001</v>
+      </c>
+      <c r="G56">
+        <v>3290066.553698</v>
+      </c>
+      <c r="H56">
+        <v>447.65293400000002</v>
+      </c>
+      <c r="I56">
+        <v>106.716741</v>
+      </c>
+      <c r="J56">
+        <v>355.72246999999999</v>
+      </c>
       <c r="S56" s="1"/>
       <c r="T56" s="1"/>
       <c r="AP56" s="1"/>
@@ -1851,7 +2520,37 @@
       <c r="CF56" s="1"/>
       <c r="FV56" s="1"/>
     </row>
-    <row r="57" spans="19:178" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:178" x14ac:dyDescent="0.25">
+      <c r="A57" s="2">
+        <v>6875</v>
+      </c>
+      <c r="B57">
+        <v>0</v>
+      </c>
+      <c r="C57">
+        <v>1975907.4847860001</v>
+      </c>
+      <c r="D57">
+        <v>3306446.54819</v>
+      </c>
+      <c r="E57">
+        <v>3945266.3333879998</v>
+      </c>
+      <c r="F57">
+        <v>77371712.525617003</v>
+      </c>
+      <c r="G57">
+        <v>3306446.54819</v>
+      </c>
+      <c r="H57">
+        <v>443.74280599999997</v>
+      </c>
+      <c r="I57">
+        <v>106.16043000000001</v>
+      </c>
+      <c r="J57">
+        <v>353.86810100000002</v>
+      </c>
       <c r="S57" s="1"/>
       <c r="T57" s="1"/>
       <c r="AP57" s="1"/>
@@ -1862,7 +2561,37 @@
       <c r="CF57" s="1"/>
       <c r="FV57" s="1"/>
     </row>
-    <row r="58" spans="19:178" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:178" x14ac:dyDescent="0.25">
+      <c r="A58" s="2">
+        <v>7000</v>
+      </c>
+      <c r="B58">
+        <v>0</v>
+      </c>
+      <c r="C58">
+        <v>932573.21671299997</v>
+      </c>
+      <c r="D58">
+        <v>3314431.7955049998</v>
+      </c>
+      <c r="E58">
+        <v>3625856.4407890001</v>
+      </c>
+      <c r="F58">
+        <v>97339275.646938995</v>
+      </c>
+      <c r="G58">
+        <v>3314431.7955049998</v>
+      </c>
+      <c r="H58">
+        <v>441.04642200000001</v>
+      </c>
+      <c r="I58">
+        <v>105.690088</v>
+      </c>
+      <c r="J58">
+        <v>352.30029500000001</v>
+      </c>
       <c r="AP58" s="1"/>
       <c r="AQ58" s="1"/>
       <c r="CA58" s="1"/>
@@ -1871,7 +2600,37 @@
       <c r="CF58" s="1"/>
       <c r="FV58" s="1"/>
     </row>
-    <row r="59" spans="19:178" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:178" x14ac:dyDescent="0.25">
+      <c r="A59" s="2">
+        <v>7125</v>
+      </c>
+      <c r="B59">
+        <v>0</v>
+      </c>
+      <c r="C59">
+        <v>503802.80989799998</v>
+      </c>
+      <c r="D59">
+        <v>3318324.603571</v>
+      </c>
+      <c r="E59">
+        <v>3470144.1181470002</v>
+      </c>
+      <c r="F59">
+        <v>123034268.591325</v>
+      </c>
+      <c r="G59">
+        <v>3318324.603571</v>
+      </c>
+      <c r="H59">
+        <v>438.90472399999999</v>
+      </c>
+      <c r="I59">
+        <v>105.26319100000001</v>
+      </c>
+      <c r="J59">
+        <v>350.87730399999998</v>
+      </c>
       <c r="AP59" s="1"/>
       <c r="AQ59" s="1"/>
       <c r="CA59" s="1"/>
@@ -1880,7 +2639,37 @@
       <c r="CF59" s="1"/>
       <c r="FV59" s="1"/>
     </row>
-    <row r="60" spans="19:178" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:178" x14ac:dyDescent="0.25">
+      <c r="A60" s="2">
+        <v>7250</v>
+      </c>
+      <c r="B60">
+        <v>0</v>
+      </c>
+      <c r="C60">
+        <v>309165.42629899998</v>
+      </c>
+      <c r="D60">
+        <v>3320222.3475029999</v>
+      </c>
+      <c r="E60">
+        <v>3394234.3608590001</v>
+      </c>
+      <c r="F60">
+        <v>156277737.24792001</v>
+      </c>
+      <c r="G60">
+        <v>3320222.3475029999</v>
+      </c>
+      <c r="H60">
+        <v>437.03547600000002</v>
+      </c>
+      <c r="I60">
+        <v>104.859345</v>
+      </c>
+      <c r="J60">
+        <v>349.53114799999997</v>
+      </c>
       <c r="AP60" s="1"/>
       <c r="AQ60" s="1"/>
       <c r="CA60" s="1"/>
@@ -1889,7 +2678,37 @@
       <c r="CF60" s="1"/>
       <c r="FV60" s="1"/>
     </row>
-    <row r="61" spans="19:178" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:178" x14ac:dyDescent="0.25">
+      <c r="A61" s="2">
+        <v>7375</v>
+      </c>
+      <c r="B61">
+        <v>0</v>
+      </c>
+      <c r="C61">
+        <v>292841.96062500001</v>
+      </c>
+      <c r="D61">
+        <v>3321147.49767</v>
+      </c>
+      <c r="E61">
+        <v>3357228.354181</v>
+      </c>
+      <c r="F61">
+        <v>102249052.32945099</v>
+      </c>
+      <c r="G61">
+        <v>3321147.49767</v>
+      </c>
+      <c r="H61">
+        <v>435.30893300000002</v>
+      </c>
+      <c r="I61">
+        <v>104.468712</v>
+      </c>
+      <c r="J61">
+        <v>348.229039</v>
+      </c>
       <c r="AP61" s="1"/>
       <c r="AQ61" s="1"/>
       <c r="CA61" s="1"/>
@@ -1898,7 +2717,37 @@
       <c r="CF61" s="1"/>
       <c r="FV61" s="1"/>
     </row>
-    <row r="62" spans="19:178" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:178" x14ac:dyDescent="0.25">
+      <c r="A62" s="2">
+        <v>7500</v>
+      </c>
+      <c r="B62">
+        <v>0</v>
+      </c>
+      <c r="C62">
+        <v>355995.07162200002</v>
+      </c>
+      <c r="D62">
+        <v>3321598.5083770002</v>
+      </c>
+      <c r="E62">
+        <v>3339187.9259259999</v>
+      </c>
+      <c r="F62">
+        <v>46737781.218209997</v>
+      </c>
+      <c r="G62">
+        <v>3321598.5083770002</v>
+      </c>
+      <c r="H62">
+        <v>433.66275300000001</v>
+      </c>
+      <c r="I62">
+        <v>104.086521</v>
+      </c>
+      <c r="J62">
+        <v>346.95507099999998</v>
+      </c>
       <c r="AP62" s="1"/>
       <c r="AQ62" s="1"/>
       <c r="CA62" s="1"/>
@@ -1907,7 +2756,37 @@
       <c r="CF62" s="1"/>
       <c r="FV62" s="1"/>
     </row>
-    <row r="63" spans="19:178" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:178" x14ac:dyDescent="0.25">
+      <c r="A63" s="2">
+        <v>7625</v>
+      </c>
+      <c r="B63">
+        <v>0</v>
+      </c>
+      <c r="C63">
+        <v>481147.405509</v>
+      </c>
+      <c r="D63">
+        <v>3321818.376096</v>
+      </c>
+      <c r="E63">
+        <v>3330393.2171510002</v>
+      </c>
+      <c r="F63">
+        <v>18852575.361706</v>
+      </c>
+      <c r="G63">
+        <v>3321818.376096</v>
+      </c>
+      <c r="H63">
+        <v>432.06600100000003</v>
+      </c>
+      <c r="I63">
+        <v>103.710438</v>
+      </c>
+      <c r="J63">
+        <v>345.70146099999999</v>
+      </c>
       <c r="AP63" s="1"/>
       <c r="AQ63" s="1"/>
       <c r="CA63" s="1"/>
@@ -1916,7 +2795,37 @@
       <c r="CF63" s="1"/>
       <c r="FV63" s="1"/>
     </row>
-    <row r="64" spans="19:178" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:178" x14ac:dyDescent="0.25">
+      <c r="A64" s="2">
+        <v>7750</v>
+      </c>
+      <c r="B64">
+        <v>0</v>
+      </c>
+      <c r="C64">
+        <v>763297.36378200003</v>
+      </c>
+      <c r="D64">
+        <v>3321925.561609</v>
+      </c>
+      <c r="E64">
+        <v>3326105.7966240002</v>
+      </c>
+      <c r="F64">
+        <v>7492011.520695</v>
+      </c>
+      <c r="G64">
+        <v>3321925.561609</v>
+      </c>
+      <c r="H64">
+        <v>427.56534699999997</v>
+      </c>
+      <c r="I64">
+        <v>103.339302</v>
+      </c>
+      <c r="J64">
+        <v>344.464339</v>
+      </c>
       <c r="AP64" s="1"/>
       <c r="AQ64" s="1"/>
       <c r="CA64" s="1"/>
@@ -1925,7 +2834,37 @@
       <c r="CF64" s="1"/>
       <c r="FV64" s="1"/>
     </row>
-    <row r="65" spans="42:178" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:178" x14ac:dyDescent="0.25">
+      <c r="A65" s="2">
+        <v>7875</v>
+      </c>
+      <c r="B65">
+        <v>0</v>
+      </c>
+      <c r="C65">
+        <v>1172138.909338</v>
+      </c>
+      <c r="D65">
+        <v>3321977.814547</v>
+      </c>
+      <c r="E65">
+        <v>3324015.679116</v>
+      </c>
+      <c r="F65">
+        <v>3161451.975658</v>
+      </c>
+      <c r="G65">
+        <v>3321977.814547</v>
+      </c>
+      <c r="H65">
+        <v>423.142944</v>
+      </c>
+      <c r="I65">
+        <v>102.97251799999999</v>
+      </c>
+      <c r="J65">
+        <v>343.24172600000003</v>
+      </c>
       <c r="AP65" s="1"/>
       <c r="AQ65" s="1"/>
       <c r="CA65" s="1"/>
@@ -1934,501 +2873,1081 @@
       <c r="CF65" s="1"/>
       <c r="FV65" s="1"/>
     </row>
-    <row r="66" spans="42:178" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:178" x14ac:dyDescent="0.25">
+      <c r="A66" s="2">
+        <v>8000</v>
+      </c>
+      <c r="B66">
+        <v>0</v>
+      </c>
+      <c r="C66">
+        <v>1486142.796419</v>
+      </c>
+      <c r="D66">
+        <v>3322003.287854</v>
+      </c>
+      <c r="E66">
+        <v>3322996.7468320001</v>
+      </c>
+      <c r="F66">
+        <v>1492117.146741</v>
+      </c>
+      <c r="G66">
+        <v>3322003.287854</v>
+      </c>
+      <c r="H66">
+        <v>422.44028400000002</v>
+      </c>
+      <c r="I66">
+        <v>102.60976599999999</v>
+      </c>
+      <c r="J66">
+        <v>342.032555</v>
+      </c>
       <c r="AP66" s="1"/>
       <c r="AQ66" s="1"/>
       <c r="CE66" s="1"/>
       <c r="CF66" s="1"/>
       <c r="FV66" s="1"/>
     </row>
-    <row r="67" spans="42:178" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:178" x14ac:dyDescent="0.25">
+      <c r="A67" s="2">
+        <v>8125</v>
+      </c>
+      <c r="B67">
+        <v>0</v>
+      </c>
+      <c r="C67">
+        <v>1742507.5485680001</v>
+      </c>
+      <c r="D67">
+        <v>3322015.7060909998</v>
+      </c>
+      <c r="E67">
+        <v>3322500.017343</v>
+      </c>
+      <c r="F67">
+        <v>806084.49583699997</v>
+      </c>
+      <c r="G67">
+        <v>3322015.7060909998</v>
+      </c>
+      <c r="H67">
+        <v>422.05759999999998</v>
+      </c>
+      <c r="I67">
+        <v>102.25086</v>
+      </c>
+      <c r="J67">
+        <v>340.83620000000002</v>
+      </c>
       <c r="AP67" s="1"/>
       <c r="AQ67" s="1"/>
       <c r="CE67" s="1"/>
       <c r="CF67" s="1"/>
       <c r="FV67" s="1"/>
     </row>
-    <row r="68" spans="42:178" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:178" x14ac:dyDescent="0.25">
+      <c r="A68" s="2">
+        <v>8250</v>
+      </c>
+      <c r="B68">
+        <v>0</v>
+      </c>
+      <c r="C68">
+        <v>1910207.5443839999</v>
+      </c>
+      <c r="D68">
+        <v>3322021.7599820001</v>
+      </c>
+      <c r="E68">
+        <v>3322257.8617170001</v>
+      </c>
+      <c r="F68">
+        <v>494664.68207899999</v>
+      </c>
+      <c r="G68">
+        <v>3322021.7599820001</v>
+      </c>
+      <c r="H68">
+        <v>421.727395</v>
+      </c>
+      <c r="I68">
+        <v>101.89567700000001</v>
+      </c>
+      <c r="J68">
+        <v>339.65225600000002</v>
+      </c>
       <c r="AP68" s="1"/>
       <c r="AQ68" s="1"/>
       <c r="CE68" s="1"/>
       <c r="CF68" s="1"/>
       <c r="FV68" s="1"/>
     </row>
-    <row r="69" spans="42:178" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:178" x14ac:dyDescent="0.25">
+      <c r="A69" s="2">
+        <v>8375</v>
+      </c>
+      <c r="B69">
+        <v>0</v>
+      </c>
+      <c r="C69">
+        <v>2000727.646432</v>
+      </c>
+      <c r="D69">
+        <v>3322024.711253</v>
+      </c>
+      <c r="E69">
+        <v>3322139.8108489998</v>
+      </c>
+      <c r="F69">
+        <v>468547.13699899998</v>
+      </c>
+      <c r="G69">
+        <v>3322024.711253</v>
+      </c>
+      <c r="H69">
+        <v>421.23266100000001</v>
+      </c>
+      <c r="I69">
+        <v>101.54412600000001</v>
+      </c>
+      <c r="J69">
+        <v>338.48041999999998</v>
+      </c>
       <c r="AP69" s="1"/>
       <c r="AQ69" s="1"/>
       <c r="CE69" s="1"/>
       <c r="CF69" s="1"/>
       <c r="FV69" s="1"/>
     </row>
-    <row r="70" spans="42:178" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:178" x14ac:dyDescent="0.25">
+      <c r="A70" s="2">
+        <v>8500</v>
+      </c>
+      <c r="B70">
+        <v>0</v>
+      </c>
+      <c r="C70">
+        <v>2043342.9852479999</v>
+      </c>
+      <c r="D70">
+        <v>3322026.1499979999</v>
+      </c>
+      <c r="E70">
+        <v>3322082.2610510001</v>
+      </c>
+      <c r="F70">
+        <v>569592.11459500005</v>
+      </c>
+      <c r="G70">
+        <v>3322026.1499979999</v>
+      </c>
+      <c r="H70">
+        <v>420.48403500000001</v>
+      </c>
+      <c r="I70">
+        <v>101.196134</v>
+      </c>
+      <c r="J70">
+        <v>337.320446</v>
+      </c>
       <c r="AP70" s="1"/>
       <c r="AQ70" s="1"/>
       <c r="CE70" s="1"/>
       <c r="CF70" s="1"/>
       <c r="FV70" s="1"/>
     </row>
-    <row r="71" spans="42:178" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:178" x14ac:dyDescent="0.25">
+      <c r="A71" s="2">
+        <v>8625</v>
+      </c>
+      <c r="B71">
+        <v>0</v>
+      </c>
+      <c r="C71">
+        <v>2061973.439515</v>
+      </c>
+      <c r="D71">
+        <v>3322026.8513870002</v>
+      </c>
+      <c r="E71">
+        <v>3322054.2055250001</v>
+      </c>
+      <c r="F71">
+        <v>769835.84881500003</v>
+      </c>
+      <c r="G71">
+        <v>3322026.8513870002</v>
+      </c>
+      <c r="H71">
+        <v>419.502298</v>
+      </c>
+      <c r="I71">
+        <v>100.851635</v>
+      </c>
+      <c r="J71">
+        <v>336.17211500000002</v>
+      </c>
       <c r="AP71" s="1"/>
       <c r="AQ71" s="1"/>
       <c r="CE71" s="1"/>
       <c r="CF71" s="1"/>
       <c r="FV71" s="1"/>
     </row>
-    <row r="72" spans="42:178" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:178" x14ac:dyDescent="0.25">
+      <c r="A72" s="2">
+        <v>8750</v>
+      </c>
+      <c r="B72">
+        <v>0</v>
+      </c>
+      <c r="C72">
+        <v>2069945.88592</v>
+      </c>
+      <c r="D72">
+        <v>3322027.1933129998</v>
+      </c>
+      <c r="E72">
+        <v>3322040.5284560001</v>
+      </c>
+      <c r="F72">
+        <v>1074621.6195169999</v>
+      </c>
+      <c r="G72">
+        <v>3322027.1933129998</v>
+      </c>
+      <c r="H72">
+        <v>418.35349300000001</v>
+      </c>
+      <c r="I72">
+        <v>100.51056699999999</v>
+      </c>
+      <c r="J72">
+        <v>335.03522400000003</v>
+      </c>
       <c r="AP72" s="1"/>
       <c r="AQ72" s="1"/>
       <c r="CE72" s="1"/>
       <c r="CF72" s="1"/>
       <c r="FV72" s="1"/>
     </row>
-    <row r="73" spans="42:178" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:178" x14ac:dyDescent="0.25">
+      <c r="A73" s="2">
+        <v>8875</v>
+      </c>
+      <c r="B73">
+        <v>0</v>
+      </c>
+      <c r="C73">
+        <v>2073399.2221949999</v>
+      </c>
+      <c r="D73">
+        <v>3322027.3600030001</v>
+      </c>
+      <c r="E73">
+        <v>3322033.8608849999</v>
+      </c>
+      <c r="F73">
+        <v>1475021.937229</v>
+      </c>
+      <c r="G73">
+        <v>3322027.3600030001</v>
+      </c>
+      <c r="H73">
+        <v>417.10222599999997</v>
+      </c>
+      <c r="I73">
+        <v>100.17287399999999</v>
+      </c>
+      <c r="J73">
+        <v>333.909581</v>
+      </c>
       <c r="AP73" s="1"/>
       <c r="AQ73" s="1"/>
       <c r="FV73" s="1"/>
     </row>
-    <row r="74" spans="42:178" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:178" x14ac:dyDescent="0.25">
+      <c r="A74" s="2">
+        <v>9000</v>
+      </c>
+      <c r="B74">
+        <v>0</v>
+      </c>
+      <c r="C74">
+        <v>2074935.269319</v>
+      </c>
+      <c r="D74">
+        <v>3322027.4412639998</v>
+      </c>
+      <c r="E74">
+        <v>3322030.610444</v>
+      </c>
+      <c r="F74">
+        <v>1926425.20575</v>
+      </c>
+      <c r="G74">
+        <v>3322027.4412639998</v>
+      </c>
+      <c r="H74">
+        <v>415.79549200000002</v>
+      </c>
+      <c r="I74">
+        <v>99.838499999999996</v>
+      </c>
+      <c r="J74">
+        <v>332.79499900000002</v>
+      </c>
       <c r="AP74" s="1"/>
       <c r="AQ74" s="1"/>
       <c r="FV74" s="1"/>
     </row>
-    <row r="75" spans="42:178" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:178" x14ac:dyDescent="0.25">
+      <c r="A75" s="2">
+        <v>9125</v>
+      </c>
+      <c r="B75">
+        <v>0</v>
+      </c>
+      <c r="C75">
+        <v>2075637.602433</v>
+      </c>
+      <c r="D75">
+        <v>3322027.4808780001</v>
+      </c>
+      <c r="E75">
+        <v>3322029.0258539999</v>
+      </c>
+      <c r="F75">
+        <v>2357218.641729</v>
+      </c>
+      <c r="G75">
+        <v>3322027.4808780001</v>
+      </c>
+      <c r="H75">
+        <v>414.46301599999998</v>
+      </c>
+      <c r="I75">
+        <v>99.507389000000003</v>
+      </c>
+      <c r="J75">
+        <v>331.69129800000002</v>
+      </c>
       <c r="AP75" s="1"/>
       <c r="AQ75" s="1"/>
       <c r="FV75" s="1"/>
     </row>
-    <row r="76" spans="42:178" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:178" x14ac:dyDescent="0.25">
+      <c r="A76" s="2">
+        <v>9250</v>
+      </c>
+      <c r="B76">
+        <v>0</v>
+      </c>
+      <c r="C76">
+        <v>2075965.992483</v>
+      </c>
+      <c r="D76">
+        <v>3322027.5001909998</v>
+      </c>
+      <c r="E76">
+        <v>3322028.253366</v>
+      </c>
+      <c r="F76">
+        <v>2706775.3563720002</v>
+      </c>
+      <c r="G76">
+        <v>3322027.5001909998</v>
+      </c>
+      <c r="H76">
+        <v>413.122208</v>
+      </c>
+      <c r="I76">
+        <v>99.179490999999999</v>
+      </c>
+      <c r="J76">
+        <v>330.59830199999999</v>
+      </c>
       <c r="AP76" s="1"/>
       <c r="AQ76" s="1"/>
       <c r="FV76" s="1"/>
     </row>
-    <row r="77" spans="42:178" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:178" x14ac:dyDescent="0.25">
+      <c r="A77" s="2">
+        <v>9375</v>
+      </c>
+      <c r="B77">
+        <v>0</v>
+      </c>
+      <c r="C77">
+        <v>2076121.9911179999</v>
+      </c>
+      <c r="D77">
+        <v>3322027.5096049998</v>
+      </c>
+      <c r="E77">
+        <v>3322027.876778</v>
+      </c>
+      <c r="F77">
+        <v>2953969.7953320001</v>
+      </c>
+      <c r="G77">
+        <v>3322027.5096049998</v>
+      </c>
+      <c r="H77">
+        <v>411.78279600000002</v>
+      </c>
+      <c r="I77">
+        <v>98.854752000000005</v>
+      </c>
+      <c r="J77">
+        <v>329.51584100000002</v>
+      </c>
       <c r="AP77" s="1"/>
       <c r="AQ77" s="1"/>
       <c r="FV77" s="1"/>
     </row>
-    <row r="78" spans="42:178" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:178" x14ac:dyDescent="0.25">
+      <c r="A78" s="2">
+        <v>9500</v>
+      </c>
+      <c r="B78">
+        <v>0</v>
+      </c>
+      <c r="C78">
+        <v>2076196.868456</v>
+      </c>
+      <c r="D78">
+        <v>3322027.5141949998</v>
+      </c>
+      <c r="E78">
+        <v>3322027.693192</v>
+      </c>
+      <c r="F78">
+        <v>3111659.2858640002</v>
+      </c>
+      <c r="G78">
+        <v>3322027.5141949998</v>
+      </c>
+      <c r="H78">
+        <v>410.45003800000001</v>
+      </c>
+      <c r="I78">
+        <v>98.533124000000001</v>
+      </c>
+      <c r="J78">
+        <v>328.44374499999998</v>
+      </c>
       <c r="AP78" s="1"/>
       <c r="AQ78" s="1"/>
       <c r="FV78" s="1"/>
     </row>
-    <row r="79" spans="42:178" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:178" x14ac:dyDescent="0.25">
+      <c r="A79" s="2">
+        <v>9625</v>
+      </c>
+      <c r="B79">
+        <v>0</v>
+      </c>
+      <c r="C79">
+        <v>2076233.040364</v>
+      </c>
+      <c r="D79">
+        <v>3322027.5164319999</v>
+      </c>
+      <c r="E79">
+        <v>3322027.603693</v>
+      </c>
+      <c r="F79">
+        <v>3205408.3945439998</v>
+      </c>
+      <c r="G79">
+        <v>3322027.5164319999</v>
+      </c>
+      <c r="H79">
+        <v>409.12668300000001</v>
+      </c>
+      <c r="I79">
+        <v>98.214556000000002</v>
+      </c>
+      <c r="J79">
+        <v>327.38185199999998</v>
+      </c>
       <c r="AP79" s="1"/>
       <c r="AQ79" s="1"/>
       <c r="FV79" s="1"/>
     </row>
-    <row r="80" spans="42:178" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:178" x14ac:dyDescent="0.25">
+      <c r="A80" s="2">
+        <v>9750</v>
+      </c>
+      <c r="B80">
+        <v>0</v>
+      </c>
+      <c r="C80">
+        <v>2076250.58186</v>
+      </c>
+      <c r="D80">
+        <v>3322027.517523</v>
+      </c>
+      <c r="E80">
+        <v>3322027.5600629998</v>
+      </c>
+      <c r="F80">
+        <v>3258660.906008</v>
+      </c>
+      <c r="G80">
+        <v>3322027.517523</v>
+      </c>
+      <c r="H80">
+        <v>407.81411400000002</v>
+      </c>
+      <c r="I80">
+        <v>97.899000000000001</v>
+      </c>
+      <c r="J80">
+        <v>326.33000099999998</v>
+      </c>
       <c r="AP80" s="1"/>
       <c r="AQ80" s="1"/>
       <c r="FV80" s="1"/>
     </row>
-    <row r="81" spans="42:178" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:178" x14ac:dyDescent="0.25">
+      <c r="A81" s="2">
+        <v>9875</v>
+      </c>
+      <c r="B81">
+        <v>0</v>
+      </c>
+      <c r="C81">
+        <v>2076259.107815</v>
+      </c>
+      <c r="D81">
+        <v>3322027.5180549999</v>
+      </c>
+      <c r="E81">
+        <v>3322027.5387929999</v>
+      </c>
+      <c r="F81">
+        <v>3288049.8307599998</v>
+      </c>
+      <c r="G81">
+        <v>3322027.5180549999</v>
+      </c>
+      <c r="H81">
+        <v>406.51297099999999</v>
+      </c>
+      <c r="I81">
+        <v>97.586410999999998</v>
+      </c>
+      <c r="J81">
+        <v>325.28803499999998</v>
+      </c>
       <c r="AP81" s="1"/>
       <c r="AQ81" s="1"/>
       <c r="FV81" s="1"/>
     </row>
-    <row r="82" spans="42:178" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:178" x14ac:dyDescent="0.25">
+      <c r="A82" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C82">
+        <v>2076263.257216</v>
+      </c>
+      <c r="E82">
+        <v>3322027.5284239999</v>
+      </c>
+      <c r="F82">
+        <v>3303973.130835</v>
+      </c>
+      <c r="H82">
+        <v>405.22350699999998</v>
+      </c>
+      <c r="I82">
+        <v>97.276741000000001</v>
+      </c>
+      <c r="J82">
+        <v>324.25580200000002</v>
+      </c>
       <c r="AP82" s="1"/>
       <c r="AQ82" s="1"/>
       <c r="FV82" s="1"/>
     </row>
-    <row r="83" spans="42:178" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:178" x14ac:dyDescent="0.25">
+      <c r="A83" s="2"/>
       <c r="AP83" s="1"/>
       <c r="AQ83" s="1"/>
       <c r="FV83" s="1"/>
     </row>
-    <row r="84" spans="42:178" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:178" x14ac:dyDescent="0.25">
+      <c r="A84" s="2"/>
       <c r="AP84" s="1"/>
       <c r="AQ84" s="1"/>
       <c r="FV84" s="1"/>
     </row>
-    <row r="85" spans="42:178" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:178" x14ac:dyDescent="0.25">
+      <c r="A85" s="2"/>
       <c r="AP85" s="1"/>
       <c r="AQ85" s="1"/>
       <c r="FV85" s="1"/>
     </row>
-    <row r="86" spans="42:178" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:178" x14ac:dyDescent="0.25">
+      <c r="A86" s="2"/>
       <c r="AP86" s="1"/>
       <c r="AQ86" s="1"/>
       <c r="FV86" s="1"/>
     </row>
-    <row r="87" spans="42:178" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:178" x14ac:dyDescent="0.25">
+      <c r="A87" s="2"/>
       <c r="AP87" s="1"/>
       <c r="AQ87" s="1"/>
       <c r="FV87" s="1"/>
     </row>
-    <row r="88" spans="42:178" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:178" x14ac:dyDescent="0.25">
+      <c r="A88" s="2"/>
       <c r="AP88" s="1"/>
       <c r="AQ88" s="1"/>
       <c r="FV88" s="1"/>
     </row>
-    <row r="89" spans="42:178" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:178" x14ac:dyDescent="0.25">
+      <c r="A89" s="2"/>
       <c r="AP89" s="1"/>
       <c r="AQ89" s="1"/>
       <c r="FV89" s="1"/>
     </row>
-    <row r="90" spans="42:178" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:178" x14ac:dyDescent="0.25">
+      <c r="A90" s="2"/>
       <c r="AP90" s="1"/>
       <c r="AQ90" s="1"/>
       <c r="FV90" s="1"/>
     </row>
-    <row r="91" spans="42:178" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:178" x14ac:dyDescent="0.25">
+      <c r="A91" s="2"/>
       <c r="AP91" s="1"/>
       <c r="AQ91" s="1"/>
       <c r="FV91" s="1"/>
     </row>
-    <row r="92" spans="42:178" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:178" x14ac:dyDescent="0.25">
+      <c r="A92" s="2"/>
       <c r="AP92" s="1"/>
       <c r="AQ92" s="1"/>
       <c r="FV92" s="1"/>
     </row>
-    <row r="93" spans="42:178" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:178" x14ac:dyDescent="0.25">
+      <c r="A93" s="2"/>
       <c r="AP93" s="1"/>
       <c r="AQ93" s="1"/>
       <c r="FV93" s="1"/>
     </row>
-    <row r="94" spans="42:178" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:178" x14ac:dyDescent="0.25">
+      <c r="A94" s="2"/>
       <c r="AP94" s="1"/>
       <c r="AQ94" s="1"/>
       <c r="FV94" s="1"/>
     </row>
-    <row r="95" spans="42:178" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:178" x14ac:dyDescent="0.25">
+      <c r="A95" s="2"/>
       <c r="AP95" s="1"/>
       <c r="AQ95" s="1"/>
       <c r="FV95" s="1"/>
     </row>
-    <row r="96" spans="42:178" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:178" x14ac:dyDescent="0.25">
+      <c r="A96" s="2"/>
       <c r="AP96" s="1"/>
       <c r="AQ96" s="1"/>
       <c r="FV96" s="1"/>
     </row>
-    <row r="97" spans="42:178" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:178" x14ac:dyDescent="0.25">
+      <c r="A97" s="2"/>
       <c r="AP97" s="1"/>
       <c r="AQ97" s="1"/>
       <c r="FV97" s="1"/>
     </row>
-    <row r="98" spans="42:178" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:178" x14ac:dyDescent="0.25">
+      <c r="A98" s="2"/>
       <c r="AP98" s="1"/>
       <c r="AQ98" s="1"/>
       <c r="FV98" s="1"/>
     </row>
-    <row r="99" spans="42:178" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:178" x14ac:dyDescent="0.25">
+      <c r="A99" s="2"/>
       <c r="AP99" s="1"/>
       <c r="AQ99" s="1"/>
       <c r="FV99" s="1"/>
     </row>
-    <row r="100" spans="42:178" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:178" x14ac:dyDescent="0.25">
+      <c r="A100" s="2"/>
       <c r="AP100" s="1"/>
       <c r="AQ100" s="1"/>
       <c r="FV100" s="1"/>
     </row>
-    <row r="101" spans="42:178" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:178" x14ac:dyDescent="0.25">
+      <c r="A101" s="2"/>
       <c r="AP101" s="1"/>
       <c r="AQ101" s="1"/>
       <c r="FV101" s="1"/>
     </row>
-    <row r="102" spans="42:178" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:178" x14ac:dyDescent="0.25">
+      <c r="A102" s="2"/>
       <c r="AP102" s="1"/>
       <c r="AQ102" s="1"/>
       <c r="FV102" s="1"/>
     </row>
-    <row r="103" spans="42:178" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:178" x14ac:dyDescent="0.25">
+      <c r="A103" s="2"/>
       <c r="AP103" s="1"/>
       <c r="AQ103" s="1"/>
       <c r="FV103" s="1"/>
     </row>
-    <row r="104" spans="42:178" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:178" x14ac:dyDescent="0.25">
+      <c r="A104" s="2"/>
       <c r="AP104" s="1"/>
       <c r="AQ104" s="1"/>
       <c r="FV104" s="1"/>
     </row>
-    <row r="105" spans="42:178" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:178" x14ac:dyDescent="0.25">
+      <c r="A105" s="2"/>
       <c r="AP105" s="1"/>
       <c r="AQ105" s="1"/>
       <c r="FV105" s="1"/>
     </row>
-    <row r="106" spans="42:178" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:178" x14ac:dyDescent="0.25">
+      <c r="A106" s="2"/>
       <c r="AP106" s="1"/>
       <c r="AQ106" s="1"/>
       <c r="FV106" s="1"/>
     </row>
-    <row r="107" spans="42:178" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:178" x14ac:dyDescent="0.25">
+      <c r="A107" s="2"/>
       <c r="AP107" s="1"/>
       <c r="AQ107" s="1"/>
       <c r="FV107" s="1"/>
     </row>
-    <row r="108" spans="42:178" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:178" x14ac:dyDescent="0.25">
+      <c r="A108" s="2"/>
       <c r="AP108" s="1"/>
       <c r="AQ108" s="1"/>
       <c r="FV108" s="1"/>
     </row>
-    <row r="109" spans="42:178" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:178" x14ac:dyDescent="0.25">
+      <c r="A109" s="2"/>
       <c r="AP109" s="1"/>
       <c r="AQ109" s="1"/>
       <c r="FV109" s="1"/>
     </row>
-    <row r="110" spans="42:178" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:178" x14ac:dyDescent="0.25">
+      <c r="A110" s="2"/>
       <c r="AP110" s="1"/>
       <c r="AQ110" s="1"/>
       <c r="FV110" s="1"/>
     </row>
-    <row r="111" spans="42:178" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:178" x14ac:dyDescent="0.25">
+      <c r="A111" s="2"/>
       <c r="AP111" s="1"/>
       <c r="AQ111" s="1"/>
       <c r="FV111" s="1"/>
     </row>
-    <row r="112" spans="42:178" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:178" x14ac:dyDescent="0.25">
+      <c r="A112" s="2"/>
       <c r="AP112" s="1"/>
       <c r="AQ112" s="1"/>
       <c r="FV112" s="1"/>
     </row>
-    <row r="113" spans="42:178" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:178" x14ac:dyDescent="0.25">
+      <c r="A113" s="2"/>
       <c r="AP113" s="1"/>
       <c r="AQ113" s="1"/>
       <c r="FV113" s="1"/>
     </row>
-    <row r="114" spans="42:178" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:178" x14ac:dyDescent="0.25">
+      <c r="A114" s="2"/>
       <c r="AP114" s="1"/>
       <c r="AQ114" s="1"/>
       <c r="FV114" s="1"/>
     </row>
-    <row r="115" spans="42:178" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:178" x14ac:dyDescent="0.25">
+      <c r="A115" s="2"/>
       <c r="AP115" s="1"/>
       <c r="AQ115" s="1"/>
       <c r="FV115" s="1"/>
     </row>
-    <row r="116" spans="42:178" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:178" x14ac:dyDescent="0.25">
+      <c r="A116" s="2"/>
       <c r="AP116" s="1"/>
       <c r="AQ116" s="1"/>
       <c r="FV116" s="1"/>
     </row>
-    <row r="117" spans="42:178" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:178" x14ac:dyDescent="0.25">
+      <c r="A117" s="2"/>
       <c r="AP117" s="1"/>
       <c r="AQ117" s="1"/>
       <c r="FV117" s="1"/>
     </row>
-    <row r="118" spans="42:178" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:178" x14ac:dyDescent="0.25">
+      <c r="A118" s="2"/>
       <c r="AP118" s="1"/>
       <c r="AQ118" s="1"/>
       <c r="FV118" s="1"/>
     </row>
-    <row r="119" spans="42:178" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:178" x14ac:dyDescent="0.25">
+      <c r="A119" s="2"/>
       <c r="AP119" s="1"/>
       <c r="AQ119" s="1"/>
       <c r="FV119" s="1"/>
     </row>
-    <row r="120" spans="42:178" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:178" x14ac:dyDescent="0.25">
+      <c r="A120" s="2"/>
       <c r="AP120" s="1"/>
       <c r="AQ120" s="1"/>
       <c r="FV120" s="1"/>
     </row>
-    <row r="121" spans="42:178" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:178" x14ac:dyDescent="0.25">
+      <c r="A121" s="2"/>
       <c r="AP121" s="1"/>
       <c r="AQ121" s="1"/>
       <c r="FV121" s="1"/>
     </row>
-    <row r="122" spans="42:178" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:178" x14ac:dyDescent="0.25">
+      <c r="A122" s="2"/>
       <c r="AP122" s="1"/>
       <c r="AQ122" s="1"/>
       <c r="FV122" s="1"/>
     </row>
-    <row r="123" spans="42:178" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:178" x14ac:dyDescent="0.25">
+      <c r="A123" s="2"/>
       <c r="AP123" s="1"/>
       <c r="AQ123" s="1"/>
       <c r="FV123" s="1"/>
     </row>
-    <row r="124" spans="42:178" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:178" x14ac:dyDescent="0.25">
+      <c r="A124" s="2"/>
       <c r="AP124" s="1"/>
       <c r="AQ124" s="1"/>
       <c r="FV124" s="1"/>
     </row>
-    <row r="125" spans="42:178" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:178" x14ac:dyDescent="0.25">
+      <c r="A125" s="2"/>
       <c r="AP125" s="1"/>
       <c r="AQ125" s="1"/>
       <c r="FV125" s="1"/>
     </row>
-    <row r="126" spans="42:178" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:178" x14ac:dyDescent="0.25">
+      <c r="A126" s="2"/>
       <c r="AP126" s="1"/>
       <c r="AQ126" s="1"/>
       <c r="FV126" s="1"/>
     </row>
-    <row r="127" spans="42:178" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:178" x14ac:dyDescent="0.25">
+      <c r="A127" s="2"/>
       <c r="AP127" s="1"/>
       <c r="AQ127" s="1"/>
       <c r="FV127" s="1"/>
     </row>
-    <row r="128" spans="42:178" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:178" x14ac:dyDescent="0.25">
+      <c r="A128" s="2"/>
       <c r="AP128" s="1"/>
       <c r="AQ128" s="1"/>
       <c r="FV128" s="1"/>
     </row>
-    <row r="129" spans="42:178" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:178" x14ac:dyDescent="0.25">
+      <c r="A129" s="2"/>
       <c r="AP129" s="1"/>
       <c r="AQ129" s="1"/>
       <c r="FV129" s="1"/>
     </row>
-    <row r="130" spans="42:178" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:178" x14ac:dyDescent="0.25">
+      <c r="A130" s="2"/>
       <c r="AP130" s="1"/>
       <c r="AQ130" s="1"/>
       <c r="FV130" s="1"/>
     </row>
-    <row r="131" spans="42:178" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:178" x14ac:dyDescent="0.25">
+      <c r="A131" s="2"/>
       <c r="AP131" s="1"/>
       <c r="AQ131" s="1"/>
       <c r="FV131" s="1"/>
     </row>
-    <row r="132" spans="42:178" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:178" x14ac:dyDescent="0.25">
+      <c r="A132" s="2"/>
       <c r="AP132" s="1"/>
       <c r="AQ132" s="1"/>
       <c r="FV132" s="1"/>
     </row>
-    <row r="133" spans="42:178" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:178" x14ac:dyDescent="0.25">
+      <c r="A133" s="2"/>
       <c r="AP133" s="1"/>
       <c r="AQ133" s="1"/>
       <c r="FV133" s="1"/>
     </row>
-    <row r="134" spans="42:178" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:178" x14ac:dyDescent="0.25">
+      <c r="A134" s="2"/>
       <c r="AP134" s="1"/>
       <c r="AQ134" s="1"/>
       <c r="FV134" s="1"/>
     </row>
-    <row r="135" spans="42:178" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:178" x14ac:dyDescent="0.25">
+      <c r="A135" s="2"/>
       <c r="AP135" s="1"/>
       <c r="AQ135" s="1"/>
       <c r="FV135" s="1"/>
     </row>
-    <row r="136" spans="42:178" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:178" x14ac:dyDescent="0.25">
+      <c r="A136" s="2"/>
       <c r="AP136" s="1"/>
       <c r="AQ136" s="1"/>
       <c r="FV136" s="1"/>
     </row>
-    <row r="137" spans="42:178" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:178" x14ac:dyDescent="0.25">
+      <c r="A137" s="2"/>
       <c r="AP137" s="1"/>
       <c r="AQ137" s="1"/>
       <c r="FV137" s="1"/>
     </row>
-    <row r="138" spans="42:178" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:178" x14ac:dyDescent="0.25">
+      <c r="A138" s="2"/>
       <c r="AP138" s="1"/>
       <c r="AQ138" s="1"/>
       <c r="FV138" s="1"/>
     </row>
-    <row r="139" spans="42:178" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:178" x14ac:dyDescent="0.25">
+      <c r="A139" s="2"/>
       <c r="AP139" s="1"/>
       <c r="AQ139" s="1"/>
       <c r="FV139" s="1"/>
     </row>
-    <row r="140" spans="42:178" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:178" x14ac:dyDescent="0.25">
+      <c r="A140" s="2"/>
       <c r="AP140" s="1"/>
       <c r="AQ140" s="1"/>
       <c r="FV140" s="1"/>
     </row>
-    <row r="141" spans="42:178" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:178" x14ac:dyDescent="0.25">
+      <c r="A141" s="2"/>
       <c r="AP141" s="1"/>
       <c r="AQ141" s="1"/>
       <c r="FV141" s="1"/>
     </row>
-    <row r="142" spans="42:178" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:178" x14ac:dyDescent="0.25">
+      <c r="A142" s="2"/>
       <c r="AP142" s="1"/>
       <c r="AQ142" s="1"/>
       <c r="FV142" s="1"/>
     </row>
-    <row r="143" spans="42:178" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:178" x14ac:dyDescent="0.25">
+      <c r="A143" s="2"/>
       <c r="AP143" s="1"/>
       <c r="AQ143" s="1"/>
       <c r="FV143" s="1"/>
     </row>
-    <row r="144" spans="42:178" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:178" x14ac:dyDescent="0.25">
+      <c r="A144" s="2"/>
       <c r="AP144" s="1"/>
       <c r="AQ144" s="1"/>
       <c r="FV144" s="1"/>
     </row>
-    <row r="145" spans="42:178" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:178" x14ac:dyDescent="0.25">
+      <c r="A145" s="2"/>
       <c r="AP145" s="1"/>
       <c r="AQ145" s="1"/>
       <c r="FV145" s="1"/>
     </row>
-    <row r="146" spans="42:178" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:178" x14ac:dyDescent="0.25">
+      <c r="A146" s="2"/>
       <c r="AP146" s="1"/>
       <c r="AQ146" s="1"/>
       <c r="FV146" s="1"/>
     </row>
-    <row r="147" spans="42:178" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:178" x14ac:dyDescent="0.25">
+      <c r="A147" s="2"/>
       <c r="AP147" s="1"/>
       <c r="AQ147" s="1"/>
       <c r="FV147" s="1"/>
     </row>
-    <row r="148" spans="42:178" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:178" x14ac:dyDescent="0.25">
+      <c r="A148" s="2"/>
       <c r="AP148" s="1"/>
       <c r="AQ148" s="1"/>
       <c r="FV148" s="1"/>
     </row>
-    <row r="149" spans="42:178" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:178" x14ac:dyDescent="0.25">
+      <c r="A149" s="2"/>
       <c r="AP149" s="1"/>
       <c r="AQ149" s="1"/>
       <c r="FV149" s="1"/>
     </row>
-    <row r="150" spans="42:178" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:178" x14ac:dyDescent="0.25">
+      <c r="A150" s="2"/>
       <c r="AP150" s="1"/>
       <c r="AQ150" s="1"/>
       <c r="FV150" s="1"/>
     </row>
-    <row r="151" spans="42:178" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:178" x14ac:dyDescent="0.25">
+      <c r="A151" s="2"/>
       <c r="AP151" s="1"/>
       <c r="AQ151" s="1"/>
       <c r="FV151" s="1"/>
     </row>
-    <row r="152" spans="42:178" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:178" x14ac:dyDescent="0.25">
+      <c r="A152" s="2"/>
       <c r="AP152" s="1"/>
       <c r="AQ152" s="1"/>
       <c r="FV152" s="1"/>
     </row>
-    <row r="153" spans="42:178" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:178" x14ac:dyDescent="0.25">
+      <c r="A153" s="2"/>
       <c r="AP153" s="1"/>
       <c r="AQ153" s="1"/>
       <c r="FV153" s="1"/>
     </row>
-    <row r="154" spans="42:178" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:178" x14ac:dyDescent="0.25">
+      <c r="A154" s="2"/>
       <c r="AP154" s="1"/>
       <c r="AQ154" s="1"/>
       <c r="FV154" s="1"/>
     </row>
-    <row r="155" spans="42:178" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:178" x14ac:dyDescent="0.25">
+      <c r="A155" s="2"/>
       <c r="AP155" s="1"/>
       <c r="AQ155" s="1"/>
       <c r="FV155" s="1"/>
     </row>
-    <row r="156" spans="42:178" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:178" x14ac:dyDescent="0.25">
+      <c r="A156" s="2"/>
       <c r="AP156" s="1"/>
       <c r="AQ156" s="1"/>
       <c r="FV156" s="1"/>
     </row>
-    <row r="157" spans="42:178" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:178" x14ac:dyDescent="0.25">
+      <c r="A157" s="2"/>
       <c r="AP157" s="1"/>
       <c r="AQ157" s="1"/>
       <c r="FV157" s="1"/>
     </row>
-    <row r="158" spans="42:178" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:178" x14ac:dyDescent="0.25">
+      <c r="A158" s="2"/>
       <c r="AP158" s="1"/>
       <c r="AQ158" s="1"/>
       <c r="FV158" s="1"/>
     </row>
-    <row r="159" spans="42:178" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:178" x14ac:dyDescent="0.25">
+      <c r="A159" s="2"/>
       <c r="AP159" s="1"/>
       <c r="AQ159" s="1"/>
       <c r="FV159" s="1"/>
     </row>
-    <row r="160" spans="42:178" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:178" x14ac:dyDescent="0.25">
+      <c r="A160" s="2"/>
       <c r="AP160" s="1"/>
       <c r="AQ160" s="1"/>
       <c r="FV160" s="1"/>
     </row>
-    <row r="161" spans="42:178" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:178" x14ac:dyDescent="0.25">
+      <c r="A161" s="2"/>
       <c r="AP161" s="1"/>
       <c r="AQ161" s="1"/>
       <c r="FV161" s="1"/>
     </row>
-    <row r="162" spans="42:178" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:178" x14ac:dyDescent="0.25">
       <c r="AP162" s="1"/>
       <c r="AQ162" s="1"/>
       <c r="FV162" s="1"/>

</xml_diff>

<commit_message>
Tentando encontrar o erro que apareceu no ValueOfBacklog
</commit_message>
<xml_diff>
--- a/models/dissertation-model/modelo-ithink/dados_ithink_excel_checks.xlsx
+++ b/models/dissertation-model/modelo-ithink/dados_ithink_excel_checks.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Months</t>
   </si>
@@ -76,6 +76,15 @@
   </si>
   <si>
     <t>checkUnitVariableCost</t>
+  </si>
+  <si>
+    <t>checkIndustryDemand</t>
+  </si>
+  <si>
+    <t>checkRevenue1</t>
+  </si>
+  <si>
+    <t>checkValueOfNewOrders1</t>
   </si>
 </sst>
 </file>
@@ -446,6 +455,15 @@
       <c r="J1" t="s">
         <v>18</v>
       </c>
+      <c r="K1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M1" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="2" spans="1:178" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -477,6 +495,15 @@
       </c>
       <c r="J2">
         <v>606.06060600000001</v>
+      </c>
+      <c r="K2">
+        <v>60000000</v>
+      </c>
+      <c r="L2">
+        <v>4</v>
+      </c>
+      <c r="M2">
+        <v>50952000</v>
       </c>
       <c r="AP2" s="1"/>
       <c r="AQ2" s="1"/>
@@ -515,6 +542,15 @@
       <c r="J3">
         <v>605.862077</v>
       </c>
+      <c r="K3">
+        <v>100000000</v>
+      </c>
+      <c r="L3">
+        <v>25476002</v>
+      </c>
+      <c r="M3">
+        <v>91853717.780000001</v>
+      </c>
       <c r="AP3" s="1"/>
       <c r="AQ3" s="1"/>
       <c r="FV3" s="1"/>
@@ -550,6 +586,15 @@
       <c r="J4">
         <v>605.66373799999997</v>
       </c>
+      <c r="K4">
+        <v>100000000</v>
+      </c>
+      <c r="L4">
+        <v>42554350.590000004</v>
+      </c>
+      <c r="M4">
+        <v>105277711.3</v>
+      </c>
       <c r="AP4" s="1"/>
       <c r="AQ4" s="1"/>
       <c r="FV4" s="1"/>
@@ -585,6 +630,15 @@
       <c r="J5">
         <v>605.46559100000002</v>
       </c>
+      <c r="K5">
+        <v>100000000</v>
+      </c>
+      <c r="L5">
+        <v>50637607.25</v>
+      </c>
+      <c r="M5">
+        <v>126176453.95</v>
+      </c>
       <c r="AP5" s="1"/>
       <c r="AQ5" s="1"/>
       <c r="FV5" s="1"/>
@@ -620,6 +674,15 @@
       <c r="J6">
         <v>605.25759100000005</v>
       </c>
+      <c r="K6">
+        <v>100000000</v>
+      </c>
+      <c r="L6">
+        <v>59624282.600000001</v>
+      </c>
+      <c r="M6">
+        <v>154174849.25999999</v>
+      </c>
       <c r="AP6" s="1"/>
       <c r="AQ6" s="1"/>
       <c r="FV6" s="1"/>
@@ -655,6 +718,15 @@
       <c r="J7">
         <v>605.03098799999998</v>
       </c>
+      <c r="K7">
+        <v>100000000</v>
+      </c>
+      <c r="L7">
+        <v>70628262.670000002</v>
+      </c>
+      <c r="M7">
+        <v>188404290.91</v>
+      </c>
       <c r="AP7" s="1"/>
       <c r="AQ7" s="1"/>
       <c r="FV7" s="1"/>
@@ -690,6 +762,15 @@
       <c r="J8">
         <v>604.78114900000003</v>
       </c>
+      <c r="K8">
+        <v>100000000</v>
+      </c>
+      <c r="L8">
+        <v>83081579.450000003</v>
+      </c>
+      <c r="M8">
+        <v>228667136.09999999</v>
+      </c>
       <c r="AP8" s="1"/>
       <c r="AQ8" s="1"/>
       <c r="FV8" s="1"/>
@@ -725,6 +806,15 @@
       <c r="J9">
         <v>604.50717999999995</v>
       </c>
+      <c r="K9">
+        <v>100000000</v>
+      </c>
+      <c r="L9">
+        <v>96190307.099999994</v>
+      </c>
+      <c r="M9">
+        <v>275981434.35000002</v>
+      </c>
       <c r="AP9" s="1"/>
       <c r="AQ9" s="1"/>
       <c r="FV9" s="1"/>
@@ -760,6 +850,15 @@
       <c r="J10">
         <v>604.21070299999997</v>
       </c>
+      <c r="K10">
+        <v>100000000</v>
+      </c>
+      <c r="L10">
+        <v>109380588.37</v>
+      </c>
+      <c r="M10">
+        <v>332128915.06</v>
+      </c>
       <c r="AP10" s="1"/>
       <c r="AQ10" s="1"/>
       <c r="FV10" s="1"/>
@@ -795,6 +894,15 @@
       <c r="J11">
         <v>603.89467200000001</v>
       </c>
+      <c r="K11">
+        <v>100000000</v>
+      </c>
+      <c r="L11">
+        <v>122359003.98</v>
+      </c>
+      <c r="M11">
+        <v>399809478.5</v>
+      </c>
       <c r="AP11" s="1"/>
       <c r="AQ11" s="1"/>
       <c r="FV11" s="1"/>
@@ -830,6 +938,15 @@
       <c r="J12">
         <v>603.562501</v>
       </c>
+      <c r="K12">
+        <v>100000000</v>
+      </c>
+      <c r="L12">
+        <v>135871292.59</v>
+      </c>
+      <c r="M12">
+        <v>484968925.88999999</v>
+      </c>
       <c r="AP12" s="1"/>
       <c r="AQ12" s="1"/>
       <c r="FV12" s="1"/>
@@ -865,6 +982,15 @@
       <c r="J13">
         <v>603.215552</v>
       </c>
+      <c r="K13">
+        <v>100000000</v>
+      </c>
+      <c r="L13">
+        <v>153119011.09999999</v>
+      </c>
+      <c r="M13">
+        <v>591964848.95000005</v>
+      </c>
       <c r="AP13" s="1"/>
       <c r="AQ13" s="1"/>
       <c r="FV13" s="1"/>
@@ -900,6 +1026,15 @@
       <c r="J14">
         <v>602.84842000000003</v>
       </c>
+      <c r="K14">
+        <v>100000000</v>
+      </c>
+      <c r="L14">
+        <v>176267336.34999999</v>
+      </c>
+      <c r="M14">
+        <v>721440060.87</v>
+      </c>
       <c r="AP14" s="1"/>
       <c r="AQ14" s="1"/>
       <c r="FV14" s="1"/>
@@ -935,6 +1070,15 @@
       <c r="J15">
         <v>602.45282599999996</v>
       </c>
+      <c r="K15">
+        <v>100000000</v>
+      </c>
+      <c r="L15">
+        <v>206262043.15000001</v>
+      </c>
+      <c r="M15">
+        <v>872153107.40999997</v>
+      </c>
       <c r="AP15" s="1"/>
       <c r="AQ15" s="1"/>
       <c r="FV15" s="1"/>
@@ -970,6 +1114,15 @@
       <c r="J16">
         <v>602.02038900000002</v>
       </c>
+      <c r="K16">
+        <v>100000000</v>
+      </c>
+      <c r="L16">
+        <v>243160651.03999999</v>
+      </c>
+      <c r="M16">
+        <v>1042845716.73</v>
+      </c>
       <c r="AP16" s="1"/>
       <c r="AQ16" s="1"/>
       <c r="FV16" s="1"/>
@@ -1005,6 +1158,15 @@
       <c r="J17">
         <v>601.54394600000001</v>
       </c>
+      <c r="K17">
+        <v>100000000</v>
+      </c>
+      <c r="L17">
+        <v>286162237.63999999</v>
+      </c>
+      <c r="M17">
+        <v>1234003420.02</v>
+      </c>
       <c r="AP17" s="1"/>
       <c r="AQ17" s="1"/>
       <c r="FV17" s="1"/>
@@ -1040,6 +1202,15 @@
       <c r="J18">
         <v>601.01849900000002</v>
       </c>
+      <c r="K18">
+        <v>100000000</v>
+      </c>
+      <c r="L18">
+        <v>334253714.24000001</v>
+      </c>
+      <c r="M18">
+        <v>1449245928.1900001</v>
+      </c>
       <c r="AP18" s="1"/>
       <c r="AQ18" s="1"/>
       <c r="FV18" s="1"/>
@@ -1075,6 +1246,15 @@
       <c r="J19">
         <v>600.44096300000001</v>
       </c>
+      <c r="K19">
+        <v>100000000</v>
+      </c>
+      <c r="L19">
+        <v>387161841.04000002</v>
+      </c>
+      <c r="M19">
+        <v>1695056058.8199999</v>
+      </c>
       <c r="AP19" s="1"/>
       <c r="AQ19" s="1"/>
       <c r="FV19" s="1"/>
@@ -1110,6 +1290,15 @@
       <c r="J20">
         <v>599.80872099999999</v>
       </c>
+      <c r="K20">
+        <v>100000000</v>
+      </c>
+      <c r="L20">
+        <v>445948432.60000002</v>
+      </c>
+      <c r="M20">
+        <v>1978904820.53</v>
+      </c>
       <c r="AP20" s="1"/>
       <c r="AQ20" s="1"/>
       <c r="FV20" s="1"/>
@@ -1145,6 +1334,15 @@
       <c r="J21">
         <v>599.11781299999996</v>
       </c>
+      <c r="K21">
+        <v>100000000</v>
+      </c>
+      <c r="L21">
+        <v>512913968.92000002</v>
+      </c>
+      <c r="M21">
+        <v>2306994020.0999999</v>
+      </c>
       <c r="AP21" s="1"/>
       <c r="AQ21" s="1"/>
       <c r="FV21" s="1"/>
@@ -1180,6 +1378,15 @@
       <c r="J22">
         <v>598.36168699999996</v>
       </c>
+      <c r="K22">
+        <v>100000000</v>
+      </c>
+      <c r="L22">
+        <v>591111360.98000002</v>
+      </c>
+      <c r="M22">
+        <v>2682990910.0599999</v>
+      </c>
       <c r="AP22" s="1"/>
       <c r="AQ22" s="1"/>
       <c r="FV22" s="1"/>
@@ -1215,6 +1422,15 @@
       <c r="J23">
         <v>597.53070700000001</v>
       </c>
+      <c r="K23">
+        <v>100000000</v>
+      </c>
+      <c r="L23">
+        <v>683988887.33000004</v>
+      </c>
+      <c r="M23">
+        <v>3108112686.0500002</v>
+      </c>
       <c r="AP23" s="1"/>
       <c r="AQ23" s="1"/>
       <c r="FV23" s="1"/>
@@ -1250,6 +1466,15 @@
       <c r="J24">
         <v>596.61205500000005</v>
       </c>
+      <c r="K24">
+        <v>100000000</v>
+      </c>
+      <c r="L24">
+        <v>795107519.40999997</v>
+      </c>
+      <c r="M24">
+        <v>3580776921.1399999</v>
+      </c>
       <c r="AP24" s="1"/>
       <c r="AQ24" s="1"/>
       <c r="FV24" s="1"/>
@@ -1285,6 +1510,15 @@
       <c r="J25">
         <v>595.58986800000002</v>
       </c>
+      <c r="K25">
+        <v>100000000</v>
+      </c>
+      <c r="L25">
+        <v>927090754.75999999</v>
+      </c>
+      <c r="M25">
+        <v>4097366261.52</v>
+      </c>
       <c r="AP25" s="1"/>
       <c r="AQ25" s="1"/>
       <c r="FV25" s="1"/>
@@ -1320,6 +1554,15 @@
       <c r="J26">
         <v>594.44651499999998</v>
       </c>
+      <c r="K26">
+        <v>100000000</v>
+      </c>
+      <c r="L26">
+        <v>1081196372.4200001</v>
+      </c>
+      <c r="M26">
+        <v>4655232335.7399998</v>
+      </c>
       <c r="AP26" s="1"/>
       <c r="AQ26" s="1"/>
       <c r="FV26" s="1"/>
@@ -1355,6 +1598,15 @@
       <c r="J27">
         <v>593.16401199999996</v>
       </c>
+      <c r="K27">
+        <v>100000000</v>
+      </c>
+      <c r="L27">
+        <v>1258023896.1900001</v>
+      </c>
+      <c r="M27">
+        <v>5255279807.6899996</v>
+      </c>
       <c r="AP27" s="1"/>
       <c r="AQ27" s="1"/>
       <c r="FV27" s="1"/>
@@ -1390,6 +1642,15 @@
       <c r="J28">
         <v>591.72443499999997</v>
       </c>
+      <c r="K28">
+        <v>100000000</v>
+      </c>
+      <c r="L28">
+        <v>1458984519.5899999</v>
+      </c>
+      <c r="M28">
+        <v>5901842419.0799999</v>
+      </c>
       <c r="AP28" s="1"/>
       <c r="AQ28" s="1"/>
       <c r="FV28" s="1"/>
@@ -1425,6 +1686,15 @@
       <c r="J29">
         <v>590.10883999999999</v>
       </c>
+      <c r="K29">
+        <v>100000000</v>
+      </c>
+      <c r="L29">
+        <v>1687667307.0699999</v>
+      </c>
+      <c r="M29">
+        <v>6599795664.8400002</v>
+      </c>
       <c r="AP29" s="1"/>
       <c r="AQ29" s="1"/>
       <c r="FV29" s="1"/>
@@ -1460,6 +1730,15 @@
       <c r="J30">
         <v>588.29511200000002</v>
       </c>
+      <c r="K30">
+        <v>100000000</v>
+      </c>
+      <c r="L30">
+        <v>1950285811.0599999</v>
+      </c>
+      <c r="M30">
+        <v>7350709875.0799999</v>
+      </c>
       <c r="AP30" s="1"/>
       <c r="AQ30" s="1"/>
       <c r="FV30" s="1"/>
@@ -1495,6 +1774,15 @@
       <c r="J31">
         <v>586.255717</v>
       </c>
+      <c r="K31">
+        <v>100000000</v>
+      </c>
+      <c r="L31">
+        <v>2255029994.4099998</v>
+      </c>
+      <c r="M31">
+        <v>8150294630.4799995</v>
+      </c>
       <c r="AP31" s="1"/>
       <c r="AQ31" s="1"/>
       <c r="FV31" s="1"/>
@@ -1529,6 +1817,15 @@
       </c>
       <c r="J32">
         <v>583.95628199999999</v>
+      </c>
+      <c r="K32">
+        <v>100000000</v>
+      </c>
+      <c r="L32">
+        <v>2610838315.8800001</v>
+      </c>
+      <c r="M32">
+        <v>8988441431.7800007</v>
       </c>
       <c r="AP32" s="1"/>
       <c r="AQ32" s="1"/>
@@ -1567,6 +1864,15 @@
       <c r="J33">
         <v>581.35534700000005</v>
       </c>
+      <c r="K33">
+        <v>100000000</v>
+      </c>
+      <c r="L33">
+        <v>3026403755.5100002</v>
+      </c>
+      <c r="M33">
+        <v>9851511360.2199993</v>
+      </c>
       <c r="AP33" s="1"/>
       <c r="AQ33" s="1"/>
       <c r="CA33" s="1"/>
@@ -1604,6 +1910,15 @@
       <c r="J34">
         <v>578.40489700000001</v>
       </c>
+      <c r="K34">
+        <v>100000000</v>
+      </c>
+      <c r="L34">
+        <v>3509966737.9499998</v>
+      </c>
+      <c r="M34">
+        <v>10725087810.48</v>
+      </c>
       <c r="AP34" s="1"/>
       <c r="AQ34" s="1"/>
       <c r="CA34" s="1"/>
@@ -1641,6 +1956,15 @@
       <c r="J35">
         <v>575.05098199999998</v>
       </c>
+      <c r="K35">
+        <v>100000000</v>
+      </c>
+      <c r="L35">
+        <v>4069798993.4099998</v>
+      </c>
+      <c r="M35">
+        <v>11595342482.940001</v>
+      </c>
       <c r="AP35" s="1"/>
       <c r="AQ35" s="1"/>
       <c r="CA35" s="1"/>
@@ -1678,6 +2002,15 @@
       <c r="J36">
         <v>571.23393799999997</v>
       </c>
+      <c r="K36">
+        <v>100000000</v>
+      </c>
+      <c r="L36">
+        <v>4714879747.2799997</v>
+      </c>
+      <c r="M36">
+        <v>12448873756.389999</v>
+      </c>
       <c r="AP36" s="1"/>
       <c r="AQ36" s="1"/>
       <c r="CA36" s="1"/>
@@ -1715,6 +2048,15 @@
       <c r="J37">
         <v>566.88822100000004</v>
       </c>
+      <c r="K37">
+        <v>100000000</v>
+      </c>
+      <c r="L37">
+        <v>5455789892.9799995</v>
+      </c>
+      <c r="M37">
+        <v>13271865909.690001</v>
+      </c>
       <c r="AP37" s="1"/>
       <c r="AQ37" s="1"/>
       <c r="CA37" s="1"/>
@@ -1751,6 +2093,15 @@
       </c>
       <c r="J38">
         <v>561.94180400000005</v>
+      </c>
+      <c r="K38">
+        <v>100000000</v>
+      </c>
+      <c r="L38">
+        <v>6305861723.46</v>
+      </c>
+      <c r="M38">
+        <v>14048987033.35</v>
       </c>
       <c r="W38" s="1"/>
       <c r="X38" s="1"/>
@@ -1791,6 +2142,15 @@
       <c r="J39">
         <v>556.31504199999995</v>
       </c>
+      <c r="K39">
+        <v>100000000</v>
+      </c>
+      <c r="L39">
+        <v>7282175958.6400003</v>
+      </c>
+      <c r="M39">
+        <v>14762246746.98</v>
+      </c>
       <c r="W39" s="1"/>
       <c r="X39" s="1"/>
       <c r="AP39" s="1"/>
@@ -1829,6 +2189,15 @@
       </c>
       <c r="J40">
         <v>549.91931299999999</v>
+      </c>
+      <c r="K40">
+        <v>100000000</v>
+      </c>
+      <c r="L40">
+        <v>8405671348.04</v>
+      </c>
+      <c r="M40">
+        <v>15390406471.200001</v>
       </c>
       <c r="S40" s="1"/>
       <c r="T40" s="1"/>
@@ -1873,6 +2242,15 @@
       <c r="J41">
         <v>542.65634599999998</v>
       </c>
+      <c r="K41">
+        <v>100000000</v>
+      </c>
+      <c r="L41">
+        <v>9699963020.6100006</v>
+      </c>
+      <c r="M41">
+        <v>15909722086.68</v>
+      </c>
       <c r="S41" s="1"/>
       <c r="T41" s="1"/>
       <c r="W41" s="1"/>
@@ -1916,6 +2294,15 @@
       <c r="J42">
         <v>534.41943700000002</v>
       </c>
+      <c r="K42">
+        <v>100000000</v>
+      </c>
+      <c r="L42">
+        <v>11189299509.83</v>
+      </c>
+      <c r="M42">
+        <v>16296203282.110001</v>
+      </c>
       <c r="S42" s="1"/>
       <c r="T42" s="1"/>
       <c r="W42" s="1"/>
@@ -1959,6 +2346,15 @@
       <c r="J43">
         <v>525.09724200000005</v>
       </c>
+      <c r="K43">
+        <v>100000000</v>
+      </c>
+      <c r="L43">
+        <v>12896715582.389999</v>
+      </c>
+      <c r="M43">
+        <v>16528580598.549999</v>
+      </c>
       <c r="S43" s="1"/>
       <c r="T43" s="1"/>
       <c r="W43" s="1"/>
@@ -2002,6 +2398,15 @@
       <c r="J44">
         <v>514.57980299999997</v>
       </c>
+      <c r="K44">
+        <v>100000000</v>
+      </c>
+      <c r="L44">
+        <v>14843197267.65</v>
+      </c>
+      <c r="M44">
+        <v>16590706532.77</v>
+      </c>
       <c r="S44" s="1"/>
       <c r="T44" s="1"/>
       <c r="W44" s="1"/>
@@ -2045,6 +2450,15 @@
       <c r="J45">
         <v>502.76568500000002</v>
       </c>
+      <c r="K45">
+        <v>100000000</v>
+      </c>
+      <c r="L45">
+        <v>17047506687.879999</v>
+      </c>
+      <c r="M45">
+        <v>16472656283.639999</v>
+      </c>
       <c r="S45" s="1"/>
       <c r="T45" s="1"/>
       <c r="W45" s="1"/>
@@ -2088,6 +2502,15 @@
       <c r="J46">
         <v>489.56912599999998</v>
       </c>
+      <c r="K46">
+        <v>100000000</v>
+      </c>
+      <c r="L46">
+        <v>19524924568.869999</v>
+      </c>
+      <c r="M46">
+        <v>16170843858.459999</v>
+      </c>
       <c r="S46" s="1"/>
       <c r="T46" s="1"/>
       <c r="W46" s="1"/>
@@ -2131,6 +2554,15 @@
       <c r="J47">
         <v>474.926987</v>
       </c>
+      <c r="K47">
+        <v>100000000</v>
+      </c>
+      <c r="L47">
+        <v>22282441189.599998</v>
+      </c>
+      <c r="M47">
+        <v>15688046942.43</v>
+      </c>
       <c r="S47" s="1"/>
       <c r="T47" s="1"/>
       <c r="W47" s="1"/>
@@ -2174,6 +2606,15 @@
       <c r="J48">
         <v>458.80602900000002</v>
       </c>
+      <c r="K48">
+        <v>100000000</v>
+      </c>
+      <c r="L48">
+        <v>25307731265.889999</v>
+      </c>
+      <c r="M48">
+        <v>15033847069.17</v>
+      </c>
       <c r="S48" s="1"/>
       <c r="T48" s="1"/>
       <c r="W48" s="1"/>
@@ -2217,6 +2658,15 @@
       <c r="J49">
         <v>441.21081600000002</v>
       </c>
+      <c r="K49">
+        <v>100000000</v>
+      </c>
+      <c r="L49">
+        <v>28547593909.310001</v>
+      </c>
+      <c r="M49">
+        <v>14225209334.67</v>
+      </c>
       <c r="S49" s="1"/>
       <c r="T49" s="1"/>
       <c r="W49" s="1"/>
@@ -2260,6 +2710,15 @@
       <c r="J50">
         <v>422.19157200000001</v>
       </c>
+      <c r="K50">
+        <v>100000000</v>
+      </c>
+      <c r="L50">
+        <v>31865095770.950001</v>
+      </c>
+      <c r="M50">
+        <v>13286567434.83</v>
+      </c>
       <c r="S50" s="1"/>
       <c r="T50" s="1"/>
       <c r="W50" s="1"/>
@@ -2303,6 +2762,15 @@
       <c r="J51">
         <v>401.85050200000001</v>
       </c>
+      <c r="K51">
+        <v>0</v>
+      </c>
+      <c r="L51">
+        <v>34944651661.370003</v>
+      </c>
+      <c r="M51">
+        <v>1127869869.3599999</v>
+      </c>
       <c r="S51" s="1"/>
       <c r="T51" s="1"/>
       <c r="W51" s="1"/>
@@ -2346,6 +2814,15 @@
       <c r="J52">
         <v>380.34487100000001</v>
       </c>
+      <c r="K52">
+        <v>0</v>
+      </c>
+      <c r="L52">
+        <v>22183187431.349998</v>
+      </c>
+      <c r="M52">
+        <v>1177838930.25</v>
+      </c>
       <c r="S52" s="1"/>
       <c r="T52" s="1"/>
       <c r="AP52" s="1"/>
@@ -2387,6 +2864,15 @@
       <c r="J53">
         <v>368.11017700000002</v>
       </c>
+      <c r="K53">
+        <v>0</v>
+      </c>
+      <c r="L53">
+        <v>11680513180.799999</v>
+      </c>
+      <c r="M53">
+        <v>1082714958.9000001</v>
+      </c>
       <c r="S53" s="1"/>
       <c r="T53" s="1"/>
       <c r="AP53" s="1"/>
@@ -2428,6 +2914,15 @@
       <c r="J54">
         <v>361.822091</v>
       </c>
+      <c r="K54">
+        <v>0</v>
+      </c>
+      <c r="L54">
+        <v>6381614069.8500004</v>
+      </c>
+      <c r="M54">
+        <v>964617641.27999997</v>
+      </c>
       <c r="S54" s="1"/>
       <c r="T54" s="1"/>
       <c r="AP54" s="1"/>
@@ -2469,6 +2964,15 @@
       <c r="J55">
         <v>358.16148199999998</v>
       </c>
+      <c r="K55">
+        <v>0</v>
+      </c>
+      <c r="L55">
+        <v>3673115855.5599999</v>
+      </c>
+      <c r="M55">
+        <v>874360350.02999997</v>
+      </c>
       <c r="S55" s="1"/>
       <c r="T55" s="1"/>
       <c r="AP55" s="1"/>
@@ -2510,6 +3014,15 @@
       <c r="J56">
         <v>355.72246999999999</v>
       </c>
+      <c r="K56">
+        <v>0</v>
+      </c>
+      <c r="L56">
+        <v>2273738102.8000002</v>
+      </c>
+      <c r="M56">
+        <v>815549899.60000002</v>
+      </c>
       <c r="S56" s="1"/>
       <c r="T56" s="1"/>
       <c r="AP56" s="1"/>
@@ -2543,13 +3056,22 @@
         <v>3306446.54819</v>
       </c>
       <c r="H57">
-        <v>443.74280599999997</v>
+        <v>443.87916300000001</v>
       </c>
       <c r="I57">
         <v>106.16043000000001</v>
       </c>
       <c r="J57">
         <v>353.86810100000002</v>
+      </c>
+      <c r="K57">
+        <v>0</v>
+      </c>
+      <c r="L57">
+        <v>1544644001.2</v>
+      </c>
+      <c r="M57">
+        <v>779840231.51999998</v>
       </c>
       <c r="S57" s="1"/>
       <c r="T57" s="1"/>
@@ -2584,13 +3106,22 @@
         <v>3314431.7955049998</v>
       </c>
       <c r="H58">
-        <v>441.04642200000001</v>
+        <v>441.53733299999999</v>
       </c>
       <c r="I58">
         <v>105.690088</v>
       </c>
       <c r="J58">
         <v>352.30029500000001</v>
+      </c>
+      <c r="K58">
+        <v>0</v>
+      </c>
+      <c r="L58">
+        <v>1162242116.3599999</v>
+      </c>
+      <c r="M58">
+        <v>758663597.02999997</v>
       </c>
       <c r="AP58" s="1"/>
       <c r="AQ58" s="1"/>
@@ -2623,13 +3154,22 @@
         <v>3318324.603571</v>
       </c>
       <c r="H59">
-        <v>438.90472399999999</v>
+        <v>439.98733700000003</v>
       </c>
       <c r="I59">
         <v>105.26319100000001</v>
       </c>
       <c r="J59">
         <v>350.87730399999998</v>
+      </c>
+      <c r="K59">
+        <v>0</v>
+      </c>
+      <c r="L59">
+        <v>960452856.69000006</v>
+      </c>
+      <c r="M59">
+        <v>746068373.23000002</v>
       </c>
       <c r="AP59" s="1"/>
       <c r="AQ59" s="1"/>
@@ -2662,13 +3202,22 @@
         <v>3320222.3475029999</v>
       </c>
       <c r="H60">
-        <v>437.03547600000002</v>
+        <v>439.00052899999997</v>
       </c>
       <c r="I60">
         <v>104.859345</v>
       </c>
       <c r="J60">
         <v>349.53114799999997</v>
+      </c>
+      <c r="K60">
+        <v>0</v>
+      </c>
+      <c r="L60">
+        <v>853260614.96000004</v>
+      </c>
+      <c r="M60">
+        <v>738461471.50999999</v>
       </c>
       <c r="AP60" s="1"/>
       <c r="AQ60" s="1"/>
@@ -2701,13 +3250,22 @@
         <v>3321147.49767</v>
       </c>
       <c r="H61">
-        <v>435.30893300000002</v>
+        <v>438.53511099999997</v>
       </c>
       <c r="I61">
         <v>104.468712</v>
       </c>
       <c r="J61">
         <v>348.229039</v>
+      </c>
+      <c r="K61">
+        <v>0</v>
+      </c>
+      <c r="L61">
+        <v>795861043.23000002</v>
+      </c>
+      <c r="M61">
+        <v>733829995.60000002</v>
       </c>
       <c r="AP61" s="1"/>
       <c r="AQ61" s="1"/>
@@ -2740,13 +3298,22 @@
         <v>3321598.5083770002</v>
       </c>
       <c r="H62">
-        <v>433.66275300000001</v>
+        <v>438.65764100000001</v>
       </c>
       <c r="I62">
         <v>104.086521</v>
       </c>
       <c r="J62">
         <v>346.95507099999998</v>
+      </c>
+      <c r="K62">
+        <v>0</v>
+      </c>
+      <c r="L62">
+        <v>764845519.41999996</v>
+      </c>
+      <c r="M62">
+        <v>731124217.20000005</v>
       </c>
       <c r="AP62" s="1"/>
       <c r="AQ62" s="1"/>
@@ -2779,13 +3346,22 @@
         <v>3321818.376096</v>
       </c>
       <c r="H63">
-        <v>432.06600100000003</v>
+        <v>439.522268</v>
       </c>
       <c r="I63">
         <v>103.710438</v>
       </c>
       <c r="J63">
         <v>345.70146099999999</v>
+      </c>
+      <c r="K63">
+        <v>0</v>
+      </c>
+      <c r="L63">
+        <v>747984868.30999994</v>
+      </c>
+      <c r="M63">
+        <v>729871559.44000006</v>
       </c>
       <c r="AP63" s="1"/>
       <c r="AQ63" s="1"/>
@@ -2818,13 +3394,22 @@
         <v>3321925.561609</v>
       </c>
       <c r="H64">
-        <v>427.56534699999997</v>
+        <v>438.36289399999998</v>
       </c>
       <c r="I64">
         <v>103.339302</v>
       </c>
       <c r="J64">
         <v>344.464339</v>
+      </c>
+      <c r="K64">
+        <v>0</v>
+      </c>
+      <c r="L64">
+        <v>738928213.87</v>
+      </c>
+      <c r="M64">
+        <v>729962619.17999995</v>
       </c>
       <c r="AP64" s="1"/>
       <c r="AQ64" s="1"/>
@@ -2857,13 +3442,22 @@
         <v>3321977.814547</v>
       </c>
       <c r="H65">
-        <v>423.142944</v>
+        <v>438.535933</v>
       </c>
       <c r="I65">
         <v>102.97251799999999</v>
       </c>
       <c r="J65">
         <v>343.24172600000003</v>
+      </c>
+      <c r="K65">
+        <v>0</v>
+      </c>
+      <c r="L65">
+        <v>734445416.52999997</v>
+      </c>
+      <c r="M65">
+        <v>729045003.13999999</v>
       </c>
       <c r="AP65" s="1"/>
       <c r="AQ65" s="1"/>
@@ -2896,13 +3490,22 @@
         <v>3322003.287854</v>
       </c>
       <c r="H66">
-        <v>422.44028400000002</v>
+        <v>444.32574599999998</v>
       </c>
       <c r="I66">
         <v>102.60976599999999</v>
       </c>
       <c r="J66">
         <v>342.032555</v>
+      </c>
+      <c r="K66">
+        <v>0</v>
+      </c>
+      <c r="L66">
+        <v>731745209.84000003</v>
+      </c>
+      <c r="M66">
+        <v>728729749.82000005</v>
       </c>
       <c r="AP66" s="1"/>
       <c r="AQ66" s="1"/>
@@ -2933,13 +3536,22 @@
         <v>3322015.7060909998</v>
       </c>
       <c r="H67">
-        <v>422.05759999999998</v>
+        <v>452.859193</v>
       </c>
       <c r="I67">
         <v>102.25086</v>
       </c>
       <c r="J67">
         <v>340.83620000000002</v>
+      </c>
+      <c r="K67">
+        <v>0</v>
+      </c>
+      <c r="L67">
+        <v>730237479.83000004</v>
+      </c>
+      <c r="M67">
+        <v>733380513.87</v>
       </c>
       <c r="AP67" s="1"/>
       <c r="AQ67" s="1"/>
@@ -2970,13 +3582,22 @@
         <v>3322021.7599820001</v>
       </c>
       <c r="H68">
-        <v>421.727395</v>
+        <v>464.42307099999999</v>
       </c>
       <c r="I68">
         <v>101.89567700000001</v>
       </c>
       <c r="J68">
         <v>339.65225600000002</v>
+      </c>
+      <c r="K68">
+        <v>0</v>
+      </c>
+      <c r="L68">
+        <v>731808996.85000002</v>
+      </c>
+      <c r="M68">
+        <v>742792948.88</v>
       </c>
       <c r="AP68" s="1"/>
       <c r="AQ68" s="1"/>
@@ -3007,13 +3628,22 @@
         <v>3322024.711253</v>
       </c>
       <c r="H69">
-        <v>421.23266100000001</v>
+        <v>478.99254500000001</v>
       </c>
       <c r="I69">
         <v>101.54412600000001</v>
       </c>
       <c r="J69">
         <v>338.48041999999998</v>
+      </c>
+      <c r="K69">
+        <v>0</v>
+      </c>
+      <c r="L69">
+        <v>737300972.86000001</v>
+      </c>
+      <c r="M69">
+        <v>757103033.99000001</v>
       </c>
       <c r="AP69" s="1"/>
       <c r="AQ69" s="1"/>
@@ -3044,13 +3674,22 @@
         <v>3322026.1499979999</v>
       </c>
       <c r="H70">
-        <v>420.48403500000001</v>
+        <v>495.82500199999998</v>
       </c>
       <c r="I70">
         <v>101.196134</v>
       </c>
       <c r="J70">
         <v>337.320446</v>
+      </c>
+      <c r="K70">
+        <v>0</v>
+      </c>
+      <c r="L70">
+        <v>747202003.42999995</v>
+      </c>
+      <c r="M70">
+        <v>776358120.73000002</v>
       </c>
       <c r="AP70" s="1"/>
       <c r="AQ70" s="1"/>
@@ -3081,13 +3720,22 @@
         <v>3322026.8513870002</v>
       </c>
       <c r="H71">
-        <v>419.502298</v>
+        <v>513.14817600000003</v>
       </c>
       <c r="I71">
         <v>100.851635</v>
       </c>
       <c r="J71">
         <v>336.17211500000002</v>
+      </c>
+      <c r="K71">
+        <v>0</v>
+      </c>
+      <c r="L71">
+        <v>761780062.08000004</v>
+      </c>
+      <c r="M71">
+        <v>799965135.17999995</v>
       </c>
       <c r="AP71" s="1"/>
       <c r="AQ71" s="1"/>
@@ -3118,13 +3766,22 @@
         <v>3322027.1933129998</v>
       </c>
       <c r="H72">
-        <v>418.35349300000001</v>
+        <v>528.53807400000005</v>
       </c>
       <c r="I72">
         <v>100.51056699999999</v>
       </c>
       <c r="J72">
         <v>335.03522400000003</v>
+      </c>
+      <c r="K72">
+        <v>0</v>
+      </c>
+      <c r="L72">
+        <v>780872598.63</v>
+      </c>
+      <c r="M72">
+        <v>826155657.14999998</v>
       </c>
       <c r="AP72" s="1"/>
       <c r="AQ72" s="1"/>
@@ -3155,13 +3812,22 @@
         <v>3322027.3600030001</v>
       </c>
       <c r="H73">
-        <v>417.10222599999997</v>
+        <v>540.02608299999997</v>
       </c>
       <c r="I73">
         <v>100.17287399999999</v>
       </c>
       <c r="J73">
         <v>333.909581</v>
+      </c>
+      <c r="K73">
+        <v>0</v>
+      </c>
+      <c r="L73">
+        <v>803514127.88999999</v>
+      </c>
+      <c r="M73">
+        <v>852032335.25999999</v>
       </c>
       <c r="AP73" s="1"/>
       <c r="AQ73" s="1"/>
@@ -3190,13 +3856,22 @@
         <v>3322027.4412639998</v>
       </c>
       <c r="H74">
-        <v>415.79549200000002</v>
+        <v>546.98412499999995</v>
       </c>
       <c r="I74">
         <v>99.838499999999996</v>
       </c>
       <c r="J74">
         <v>332.79499900000002</v>
+      </c>
+      <c r="K74">
+        <v>0</v>
+      </c>
+      <c r="L74">
+        <v>827773231.57000005</v>
+      </c>
+      <c r="M74">
+        <v>874511544.86000001</v>
       </c>
       <c r="AP74" s="1"/>
       <c r="AQ74" s="1"/>
@@ -3225,13 +3900,22 @@
         <v>3322027.4808780001</v>
       </c>
       <c r="H75">
-        <v>414.46301599999998</v>
+        <v>550.03313900000001</v>
       </c>
       <c r="I75">
         <v>99.507389000000003</v>
       </c>
       <c r="J75">
         <v>331.69129800000002</v>
+      </c>
+      <c r="K75">
+        <v>0</v>
+      </c>
+      <c r="L75">
+        <v>851142388.21000004</v>
+      </c>
+      <c r="M75">
+        <v>891529851.72000003</v>
       </c>
       <c r="AP75" s="1"/>
       <c r="AQ75" s="1"/>
@@ -3260,13 +3944,22 @@
         <v>3322027.5001909998</v>
       </c>
       <c r="H76">
-        <v>413.122208</v>
+        <v>550.338525</v>
       </c>
       <c r="I76">
         <v>99.179490999999999</v>
       </c>
       <c r="J76">
         <v>330.59830199999999</v>
+      </c>
+      <c r="K76">
+        <v>0</v>
+      </c>
+      <c r="L76">
+        <v>871336119.97000003</v>
+      </c>
+      <c r="M76">
+        <v>902571231.80999994</v>
       </c>
       <c r="AP76" s="1"/>
       <c r="AQ76" s="1"/>
@@ -3295,13 +3988,22 @@
         <v>3322027.5096049998</v>
       </c>
       <c r="H77">
-        <v>411.78279600000002</v>
+        <v>549.00853199999995</v>
       </c>
       <c r="I77">
         <v>98.854752000000005</v>
       </c>
       <c r="J77">
         <v>329.51584100000002</v>
+      </c>
+      <c r="K77">
+        <v>0</v>
+      </c>
+      <c r="L77">
+        <v>886953675.88999999</v>
+      </c>
+      <c r="M77">
+        <v>908345546.88</v>
       </c>
       <c r="AP77" s="1"/>
       <c r="AQ77" s="1"/>
@@ -3330,13 +4032,22 @@
         <v>3322027.5141949998</v>
       </c>
       <c r="H78">
-        <v>410.45003800000001</v>
+        <v>546.84892300000001</v>
       </c>
       <c r="I78">
         <v>98.533124000000001</v>
       </c>
       <c r="J78">
         <v>328.44374499999998</v>
+      </c>
+      <c r="K78">
+        <v>0</v>
+      </c>
+      <c r="L78">
+        <v>897649611.38999999</v>
+      </c>
+      <c r="M78">
+        <v>910128136.02999997</v>
       </c>
       <c r="AP78" s="1"/>
       <c r="AQ78" s="1"/>
@@ -3365,13 +4076,22 @@
         <v>3322027.5164319999</v>
       </c>
       <c r="H79">
-        <v>409.12668300000001</v>
+        <v>544.35939800000006</v>
       </c>
       <c r="I79">
         <v>98.214556000000002</v>
       </c>
       <c r="J79">
         <v>327.38185199999998</v>
+      </c>
+      <c r="K79">
+        <v>0</v>
+      </c>
+      <c r="L79">
+        <v>903888873.71000004</v>
+      </c>
+      <c r="M79">
+        <v>909225860.66999996</v>
       </c>
       <c r="AP79" s="1"/>
       <c r="AQ79" s="1"/>
@@ -3400,13 +4120,22 @@
         <v>3322027.517523</v>
       </c>
       <c r="H80">
-        <v>407.81411400000002</v>
+        <v>541.81470100000001</v>
       </c>
       <c r="I80">
         <v>97.899000000000001</v>
       </c>
       <c r="J80">
         <v>326.33000099999998</v>
+      </c>
+      <c r="K80">
+        <v>0</v>
+      </c>
+      <c r="L80">
+        <v>906557367.19000006</v>
+      </c>
+      <c r="M80">
+        <v>906707155.01999998</v>
       </c>
       <c r="AP80" s="1"/>
       <c r="AQ80" s="1"/>
@@ -3435,13 +4164,22 @@
         <v>3322027.5180549999</v>
       </c>
       <c r="H81">
-        <v>406.51297099999999</v>
+        <v>539.34782600000005</v>
       </c>
       <c r="I81">
         <v>97.586410999999998</v>
       </c>
       <c r="J81">
         <v>325.28803499999998</v>
+      </c>
+      <c r="K81">
+        <v>0</v>
+      </c>
+      <c r="L81">
+        <v>906632261.11000001</v>
+      </c>
+      <c r="M81">
+        <v>903334413.79999995</v>
       </c>
       <c r="AP81" s="1"/>
       <c r="AQ81" s="1"/>
@@ -3461,7 +4199,7 @@
         <v>3303973.130835</v>
       </c>
       <c r="H82">
-        <v>405.22350699999998</v>
+        <v>537.01084400000002</v>
       </c>
       <c r="I82">
         <v>97.276741000000001</v>

</xml_diff>

<commit_message>
antes implementar check global
</commit_message>
<xml_diff>
--- a/models/dissertation-model/modelo-ithink/dados_ithink_excel_checks.xlsx
+++ b/models/dissertation-model/modelo-ithink/dados_ithink_excel_checks.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>Months</t>
   </si>
@@ -112,6 +112,12 @@
   </si>
   <si>
     <t>,9375</t>
+  </si>
+  <si>
+    <t>checkPerformance</t>
+  </si>
+  <si>
+    <t>checkNPVProfitChange1</t>
   </si>
 </sst>
 </file>
@@ -434,8 +440,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:FV641"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -454,6 +460,7 @@
     <col min="12" max="12" width="15" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="24.85546875" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="17.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:178" x14ac:dyDescent="0.25">
@@ -499,6 +506,12 @@
       <c r="N1" t="s">
         <v>14</v>
       </c>
+      <c r="O1" t="s">
+        <v>31</v>
+      </c>
+      <c r="P1" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="2" spans="1:178" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -542,6 +555,12 @@
       </c>
       <c r="N2">
         <v>47233.947368000001</v>
+      </c>
+      <c r="O2">
+        <v>7.3333329999999997</v>
+      </c>
+      <c r="P2">
+        <v>33320873.026248001</v>
       </c>
       <c r="AP2" s="1"/>
       <c r="AQ2" s="1"/>
@@ -592,6 +611,12 @@
       <c r="N3">
         <v>47165.669455000003</v>
       </c>
+      <c r="O3">
+        <v>7.2990789999999999</v>
+      </c>
+      <c r="P3">
+        <v>33291373.917149998</v>
+      </c>
       <c r="AP3" s="1"/>
       <c r="AQ3" s="1"/>
       <c r="FV3" s="1"/>
@@ -639,6 +664,12 @@
       <c r="N4">
         <v>47095.880051</v>
       </c>
+      <c r="O4">
+        <v>7.2662509999999996</v>
+      </c>
+      <c r="P4">
+        <v>33382641.492642</v>
+      </c>
       <c r="AP4" s="1"/>
       <c r="AQ4" s="1"/>
       <c r="FV4" s="1"/>
@@ -686,6 +717,12 @@
       <c r="N5">
         <v>47024.550516000003</v>
       </c>
+      <c r="O5">
+        <v>7.2347970000000004</v>
+      </c>
+      <c r="P5">
+        <v>33583747.247557998</v>
+      </c>
       <c r="AP5" s="1"/>
       <c r="AQ5" s="1"/>
       <c r="FV5" s="1"/>
@@ -733,6 +770,12 @@
       <c r="N6">
         <v>46951.651895000003</v>
       </c>
+      <c r="O6">
+        <v>7.2046679999999999</v>
+      </c>
+      <c r="P6">
+        <v>34156256.013777003</v>
+      </c>
       <c r="AP6" s="1"/>
       <c r="AQ6" s="1"/>
       <c r="FV6" s="1"/>
@@ -780,6 +823,12 @@
       <c r="N7">
         <v>46877.154927000003</v>
       </c>
+      <c r="O7">
+        <v>7.1758160000000002</v>
+      </c>
+      <c r="P7">
+        <v>35387174.667952999</v>
+      </c>
       <c r="AP7" s="1"/>
       <c r="AQ7" s="1"/>
       <c r="FV7" s="1"/>
@@ -827,6 +876,12 @@
       <c r="N8">
         <v>46801.030058999997</v>
       </c>
+      <c r="O8">
+        <v>7.1481960000000004</v>
+      </c>
+      <c r="P8">
+        <v>37447834.451920003</v>
+      </c>
       <c r="AP8" s="1"/>
       <c r="AQ8" s="1"/>
       <c r="FV8" s="1"/>
@@ -874,6 +929,12 @@
       <c r="N9">
         <v>46723.247450000003</v>
       </c>
+      <c r="O9">
+        <v>7.1217639999999998</v>
+      </c>
+      <c r="P9">
+        <v>40338875.448019996</v>
+      </c>
       <c r="AP9" s="1"/>
       <c r="AQ9" s="1"/>
       <c r="FV9" s="1"/>
@@ -921,6 +982,12 @@
       <c r="N10">
         <v>46643.776986999997</v>
       </c>
+      <c r="O10">
+        <v>7.096476</v>
+      </c>
+      <c r="P10">
+        <v>43900405.734217003</v>
+      </c>
       <c r="AP10" s="1"/>
       <c r="AQ10" s="1"/>
       <c r="FV10" s="1"/>
@@ -968,6 +1035,12 @@
       <c r="N11">
         <v>46562.588292</v>
       </c>
+      <c r="O11">
+        <v>7.0722930000000002</v>
+      </c>
+      <c r="P11">
+        <v>47863176.510031</v>
+      </c>
       <c r="AP11" s="1"/>
       <c r="AQ11" s="1"/>
       <c r="FV11" s="1"/>
@@ -1015,6 +1088,12 @@
       <c r="N12">
         <v>46479.650737000004</v>
       </c>
+      <c r="O12">
+        <v>7.049175</v>
+      </c>
+      <c r="P12">
+        <v>51916581.784474999</v>
+      </c>
       <c r="AP12" s="1"/>
       <c r="AQ12" s="1"/>
       <c r="FV12" s="1"/>
@@ -1062,6 +1141,12 @@
       <c r="N13">
         <v>46394.933456999999</v>
       </c>
+      <c r="O13">
+        <v>7.0270840000000003</v>
+      </c>
+      <c r="P13">
+        <v>55773344.03413</v>
+      </c>
       <c r="AP13" s="1"/>
       <c r="AQ13" s="1"/>
       <c r="FV13" s="1"/>
@@ -1109,6 +1194,12 @@
       <c r="N14">
         <v>46308.405361999998</v>
       </c>
+      <c r="O14">
+        <v>7.0059820000000004</v>
+      </c>
+      <c r="P14">
+        <v>59217294.143532</v>
+      </c>
       <c r="AP14" s="1"/>
       <c r="AQ14" s="1"/>
       <c r="FV14" s="1"/>
@@ -1156,6 +1247,12 @@
       <c r="N15">
         <v>46220.035156999998</v>
       </c>
+      <c r="O15">
+        <v>6.9858339999999997</v>
+      </c>
+      <c r="P15">
+        <v>62127491.137295999</v>
+      </c>
       <c r="AP15" s="1"/>
       <c r="AQ15" s="1"/>
       <c r="FV15" s="1"/>
@@ -1203,6 +1300,12 @@
       <c r="N16">
         <v>46129.79135</v>
       </c>
+      <c r="O16">
+        <v>6.9666069999999998</v>
+      </c>
+      <c r="P16">
+        <v>64477976.300902002</v>
+      </c>
       <c r="AP16" s="1"/>
       <c r="AQ16" s="1"/>
       <c r="FV16" s="1"/>
@@ -1250,6 +1353,12 @@
       <c r="N17">
         <v>46037.64228</v>
       </c>
+      <c r="O17">
+        <v>6.9482670000000004</v>
+      </c>
+      <c r="P17">
+        <v>66317591.463987999</v>
+      </c>
       <c r="AP17" s="1"/>
       <c r="AQ17" s="1"/>
       <c r="FV17" s="1"/>
@@ -1297,6 +1406,12 @@
       <c r="N18">
         <v>45943.556123000002</v>
       </c>
+      <c r="O18">
+        <v>6.9307829999999999</v>
+      </c>
+      <c r="P18">
+        <v>67738069.834040001</v>
+      </c>
       <c r="AP18" s="1"/>
       <c r="AQ18" s="1"/>
       <c r="FV18" s="1"/>
@@ -1344,6 +1459,12 @@
       <c r="N19">
         <v>45847.500923</v>
       </c>
+      <c r="O19">
+        <v>6.9141219999999999</v>
+      </c>
+      <c r="P19">
+        <v>68840085.443843007</v>
+      </c>
       <c r="AP19" s="1"/>
       <c r="AQ19" s="1"/>
       <c r="FV19" s="1"/>
@@ -1391,6 +1512,12 @@
       <c r="N20">
         <v>45749.444601000003</v>
       </c>
+      <c r="O20">
+        <v>6.8982559999999999</v>
+      </c>
+      <c r="P20">
+        <v>69705686.867737994</v>
+      </c>
       <c r="AP20" s="1"/>
       <c r="AQ20" s="1"/>
       <c r="FV20" s="1"/>
@@ -1438,6 +1565,12 @@
       <c r="N21">
         <v>45649.354986999999</v>
       </c>
+      <c r="O21">
+        <v>6.8831569999999997</v>
+      </c>
+      <c r="P21">
+        <v>70382235.157865003</v>
+      </c>
       <c r="AP21" s="1"/>
       <c r="AQ21" s="1"/>
       <c r="FV21" s="1"/>
@@ -1485,6 +1618,12 @@
       <c r="N22">
         <v>45547.199832999999</v>
       </c>
+      <c r="O22">
+        <v>6.8687950000000004</v>
+      </c>
+      <c r="P22">
+        <v>70862345.921941996</v>
+      </c>
       <c r="AP22" s="1"/>
       <c r="AQ22" s="1"/>
       <c r="FV22" s="1"/>
@@ -1532,6 +1671,12 @@
       <c r="N23">
         <v>45442.946842999998</v>
       </c>
+      <c r="O23">
+        <v>6.8551450000000003</v>
+      </c>
+      <c r="P23">
+        <v>71124703.409424007</v>
+      </c>
       <c r="AP23" s="1"/>
       <c r="AQ23" s="1"/>
       <c r="FV23" s="1"/>
@@ -1579,6 +1724,12 @@
       <c r="N24">
         <v>45336.563696999998</v>
       </c>
+      <c r="O24">
+        <v>6.8421810000000001</v>
+      </c>
+      <c r="P24">
+        <v>71158329.349359006</v>
+      </c>
       <c r="AP24" s="1"/>
       <c r="AQ24" s="1"/>
       <c r="FV24" s="1"/>
@@ -1626,6 +1777,12 @@
       <c r="N25">
         <v>45228.018072999999</v>
       </c>
+      <c r="O25">
+        <v>6.8298769999999998</v>
+      </c>
+      <c r="P25">
+        <v>70973342.972271994</v>
+      </c>
       <c r="AP25" s="1"/>
       <c r="AQ25" s="1"/>
       <c r="FV25" s="1"/>
@@ -1673,6 +1830,12 @@
       <c r="N26">
         <v>45117.277679999999</v>
       </c>
+      <c r="O26">
+        <v>6.8182090000000004</v>
+      </c>
+      <c r="P26">
+        <v>70601362.260073006</v>
+      </c>
       <c r="AP26" s="1"/>
       <c r="AQ26" s="1"/>
       <c r="FV26" s="1"/>
@@ -1720,6 +1883,12 @@
       <c r="N27">
         <v>45004.310279999998</v>
       </c>
+      <c r="O27">
+        <v>6.8071549999999998</v>
+      </c>
+      <c r="P27">
+        <v>70089286.551767007</v>
+      </c>
       <c r="AP27" s="1"/>
       <c r="AQ27" s="1"/>
       <c r="FV27" s="1"/>
@@ -1767,6 +1936,12 @@
       <c r="N28">
         <v>44889.083725999997</v>
       </c>
+      <c r="O28">
+        <v>6.796691</v>
+      </c>
+      <c r="P28">
+        <v>69490322.338899001</v>
+      </c>
       <c r="AP28" s="1"/>
       <c r="AQ28" s="1"/>
       <c r="FV28" s="1"/>
@@ -1814,6 +1989,12 @@
       <c r="N29">
         <v>44771.565984000001</v>
       </c>
+      <c r="O29">
+        <v>6.7867949999999997</v>
+      </c>
+      <c r="P29">
+        <v>68855474.227477998</v>
+      </c>
       <c r="AP29" s="1"/>
       <c r="AQ29" s="1"/>
       <c r="FV29" s="1"/>
@@ -1861,6 +2042,12 @@
       <c r="N30">
         <v>44651.725171999999</v>
       </c>
+      <c r="O30">
+        <v>6.7774479999999997</v>
+      </c>
+      <c r="P30">
+        <v>68227531.341561005</v>
+      </c>
       <c r="AP30" s="1"/>
       <c r="AQ30" s="1"/>
       <c r="FV30" s="1"/>
@@ -1908,6 +2095,12 @@
       <c r="N31">
         <v>44529.529589999998</v>
       </c>
+      <c r="O31">
+        <v>6.7686270000000004</v>
+      </c>
+      <c r="P31">
+        <v>67638265.206053004</v>
+      </c>
       <c r="AP31" s="1"/>
       <c r="AQ31" s="1"/>
       <c r="FV31" s="1"/>
@@ -1954,6 +2147,12 @@
       </c>
       <c r="N32">
         <v>44404.947757000002</v>
+      </c>
+      <c r="O32">
+        <v>6.7603150000000003</v>
+      </c>
+      <c r="P32">
+        <v>67108499.174576998</v>
       </c>
       <c r="AP32" s="1"/>
       <c r="AQ32" s="1"/>
@@ -2004,6 +2203,12 @@
       <c r="N33">
         <v>44277.948447000002</v>
       </c>
+      <c r="O33">
+        <v>6.752491</v>
+      </c>
+      <c r="P33">
+        <v>66650104.6219</v>
+      </c>
       <c r="AP33" s="1"/>
       <c r="AQ33" s="1"/>
       <c r="CA33" s="1"/>
@@ -2053,6 +2258,12 @@
       <c r="N34">
         <v>44148.500722999997</v>
       </c>
+      <c r="O34">
+        <v>6.7451369999999997</v>
+      </c>
+      <c r="P34">
+        <v>66268825.539052002</v>
+      </c>
       <c r="AP34" s="1"/>
       <c r="AQ34" s="1"/>
       <c r="CA34" s="1"/>
@@ -2102,6 +2313,12 @@
       <c r="N35">
         <v>44016.573982000002</v>
       </c>
+      <c r="O35">
+        <v>6.7382359999999997</v>
+      </c>
+      <c r="P35">
+        <v>65967008.348159999</v>
+      </c>
       <c r="AP35" s="1"/>
       <c r="AQ35" s="1"/>
       <c r="CA35" s="1"/>
@@ -2151,6 +2368,12 @@
       <c r="N36">
         <v>43882.137989000003</v>
       </c>
+      <c r="O36">
+        <v>6.73177</v>
+      </c>
+      <c r="P36">
+        <v>65745654.852486998</v>
+      </c>
       <c r="AP36" s="1"/>
       <c r="AQ36" s="1"/>
       <c r="CA36" s="1"/>
@@ -2200,6 +2423,12 @@
       <c r="N37">
         <v>43745.162923000004</v>
       </c>
+      <c r="O37">
+        <v>6.7257230000000003</v>
+      </c>
+      <c r="P37">
+        <v>65605579.714488</v>
+      </c>
       <c r="AP37" s="1"/>
       <c r="AQ37" s="1"/>
       <c r="CA37" s="1"/>
@@ -2248,6 +2477,12 @@
       </c>
       <c r="N38">
         <v>43605.619417000002</v>
+      </c>
+      <c r="O38">
+        <v>6.7200800000000003</v>
+      </c>
+      <c r="P38">
+        <v>65547744.290321998</v>
       </c>
       <c r="W38" s="1"/>
       <c r="X38" s="1"/>
@@ -2300,6 +2535,12 @@
       <c r="N39">
         <v>43463.478602000003</v>
       </c>
+      <c r="O39">
+        <v>6.7148240000000001</v>
+      </c>
+      <c r="P39">
+        <v>65573013.037061997</v>
+      </c>
       <c r="W39" s="1"/>
       <c r="X39" s="1"/>
       <c r="AP39" s="1"/>
@@ -2350,6 +2591,12 @@
       </c>
       <c r="N40">
         <v>43318.712156000001</v>
+      </c>
+      <c r="O40">
+        <v>6.7099419999999999</v>
+      </c>
+      <c r="P40">
+        <v>65681636.417563997</v>
       </c>
       <c r="S40" s="1"/>
       <c r="T40" s="1"/>
@@ -2406,6 +2653,12 @@
       <c r="N41">
         <v>43171.292344000001</v>
       </c>
+      <c r="O41">
+        <v>6.705419</v>
+      </c>
+      <c r="P41">
+        <v>65872731.367953002</v>
+      </c>
       <c r="S41" s="1"/>
       <c r="T41" s="1"/>
       <c r="W41" s="1"/>
@@ -2461,6 +2714,12 @@
       <c r="N42">
         <v>43021.192070999998</v>
       </c>
+      <c r="O42">
+        <v>6.7012409999999996</v>
+      </c>
+      <c r="P42">
+        <v>66143944.387457997</v>
+      </c>
       <c r="S42" s="1"/>
       <c r="T42" s="1"/>
       <c r="W42" s="1"/>
@@ -2516,6 +2775,12 @@
       <c r="N43">
         <v>42868.384927999999</v>
       </c>
+      <c r="O43">
+        <v>6.6973950000000002</v>
+      </c>
+      <c r="P43">
+        <v>66491379.805575997</v>
+      </c>
       <c r="S43" s="1"/>
       <c r="T43" s="1"/>
       <c r="W43" s="1"/>
@@ -2571,6 +2836,12 @@
       <c r="N44">
         <v>42712.845243999996</v>
       </c>
+      <c r="O44">
+        <v>6.6938700000000004</v>
+      </c>
+      <c r="P44">
+        <v>66909785.064098999</v>
+      </c>
       <c r="S44" s="1"/>
       <c r="T44" s="1"/>
       <c r="W44" s="1"/>
@@ -2626,6 +2897,12 @@
       <c r="N45">
         <v>42554.548134999997</v>
       </c>
+      <c r="O45">
+        <v>6.690652</v>
+      </c>
+      <c r="P45">
+        <v>67392922.626682997</v>
+      </c>
       <c r="S45" s="1"/>
       <c r="T45" s="1"/>
       <c r="W45" s="1"/>
@@ -2681,6 +2958,12 @@
       <c r="N46">
         <v>42393.469555999996</v>
       </c>
+      <c r="O46">
+        <v>6.687729</v>
+      </c>
+      <c r="P46">
+        <v>67934029.740020007</v>
+      </c>
       <c r="S46" s="1"/>
       <c r="T46" s="1"/>
       <c r="W46" s="1"/>
@@ -2736,6 +3019,12 @@
       <c r="N47">
         <v>42229.586354999999</v>
       </c>
+      <c r="O47">
+        <v>6.685092</v>
+      </c>
+      <c r="P47">
+        <v>68526269.138306007</v>
+      </c>
       <c r="S47" s="1"/>
       <c r="T47" s="1"/>
       <c r="W47" s="1"/>
@@ -2791,6 +3080,12 @@
       <c r="N48">
         <v>42062.876328999999</v>
       </c>
+      <c r="O48">
+        <v>6.6827290000000001</v>
+      </c>
+      <c r="P48">
+        <v>69163096.865693003</v>
+      </c>
       <c r="S48" s="1"/>
       <c r="T48" s="1"/>
       <c r="W48" s="1"/>
@@ -2846,6 +3141,12 @@
       <c r="N49">
         <v>41893.318273999997</v>
       </c>
+      <c r="O49">
+        <v>6.6806299999999998</v>
+      </c>
+      <c r="P49">
+        <v>69838506.696700007</v>
+      </c>
       <c r="S49" s="1"/>
       <c r="T49" s="1"/>
       <c r="W49" s="1"/>
@@ -2901,6 +3202,12 @@
       <c r="N50">
         <v>41720.892043</v>
       </c>
+      <c r="O50">
+        <v>6.6787850000000004</v>
+      </c>
+      <c r="P50">
+        <v>70547144.091484994</v>
+      </c>
       <c r="S50" s="1"/>
       <c r="T50" s="1"/>
       <c r="W50" s="1"/>
@@ -2956,6 +3263,12 @@
       <c r="N51">
         <v>41545.578602000001</v>
       </c>
+      <c r="O51">
+        <v>6.6771839999999996</v>
+      </c>
+      <c r="P51">
+        <v>71284308.948645994</v>
+      </c>
       <c r="S51" s="1"/>
       <c r="T51" s="1"/>
       <c r="W51" s="1"/>
@@ -3011,6 +3324,12 @@
       <c r="N52">
         <v>41367.360089000002</v>
       </c>
+      <c r="O52">
+        <v>6.6758189999999997</v>
+      </c>
+      <c r="P52">
+        <v>72045881.885014996</v>
+      </c>
       <c r="S52" s="1"/>
       <c r="T52" s="1"/>
       <c r="AP52" s="1"/>
@@ -3064,6 +3383,12 @@
       <c r="N53">
         <v>41186.219867</v>
       </c>
+      <c r="O53">
+        <v>6.6746800000000004</v>
+      </c>
+      <c r="P53">
+        <v>72828213.017018005</v>
+      </c>
       <c r="S53" s="1"/>
       <c r="T53" s="1"/>
       <c r="AP53" s="1"/>
@@ -3117,6 +3442,12 @@
       <c r="N54">
         <v>41002.142585000001</v>
       </c>
+      <c r="O54">
+        <v>6.6737599999999997</v>
+      </c>
+      <c r="P54">
+        <v>73628007.393234</v>
+      </c>
       <c r="S54" s="1"/>
       <c r="T54" s="1"/>
       <c r="AP54" s="1"/>
@@ -3170,6 +3501,12 @@
       <c r="N55">
         <v>40815.114235000001</v>
       </c>
+      <c r="O55">
+        <v>6.6730499999999999</v>
+      </c>
+      <c r="P55">
+        <v>74442230.842821002</v>
+      </c>
       <c r="S55" s="1"/>
       <c r="T55" s="1"/>
       <c r="AP55" s="1"/>
@@ -3223,6 +3560,12 @@
       <c r="N56">
         <v>40625.122210000001</v>
       </c>
+      <c r="O56">
+        <v>6.6725440000000003</v>
+      </c>
+      <c r="P56">
+        <v>75268047.795515001</v>
+      </c>
       <c r="S56" s="1"/>
       <c r="T56" s="1"/>
       <c r="AP56" s="1"/>
@@ -3276,6 +3619,12 @@
       <c r="N57">
         <v>40432.155360999997</v>
       </c>
+      <c r="O57">
+        <v>6.6722320000000002</v>
+      </c>
+      <c r="P57">
+        <v>76102791.688314006</v>
+      </c>
       <c r="S57" s="1"/>
       <c r="T57" s="1"/>
       <c r="AP57" s="1"/>
@@ -3329,6 +3678,12 @@
       <c r="N58">
         <v>40236.204060999997</v>
       </c>
+      <c r="O58">
+        <v>6.6721089999999998</v>
+      </c>
+      <c r="P58">
+        <v>76943960.859136999</v>
+      </c>
       <c r="AP58" s="1"/>
       <c r="AQ58" s="1"/>
       <c r="CA58" s="1"/>
@@ -3380,6 +3735,12 @@
       <c r="N59">
         <v>40037.260256000001</v>
       </c>
+      <c r="O59">
+        <v>6.6721680000000001</v>
+      </c>
+      <c r="P59">
+        <v>77789229.053147003</v>
+      </c>
       <c r="AP59" s="1"/>
       <c r="AQ59" s="1"/>
       <c r="CA59" s="1"/>
@@ -3431,6 +3792,12 @@
       <c r="N60">
         <v>39835.317524999999</v>
       </c>
+      <c r="O60">
+        <v>6.6724019999999999</v>
+      </c>
+      <c r="P60">
+        <v>78636459.496381</v>
+      </c>
       <c r="AP60" s="1"/>
       <c r="AQ60" s="1"/>
       <c r="CA60" s="1"/>
@@ -3482,6 +3849,12 @@
       <c r="N61">
         <v>39630.371141000003</v>
       </c>
+      <c r="O61">
+        <v>6.6728059999999996</v>
+      </c>
+      <c r="P61">
+        <v>79483713.904179007</v>
+      </c>
       <c r="AP61" s="1"/>
       <c r="AQ61" s="1"/>
       <c r="CA61" s="1"/>
@@ -3533,6 +3906,12 @@
       <c r="N62">
         <v>39422.418122000003</v>
       </c>
+      <c r="O62">
+        <v>6.6733719999999996</v>
+      </c>
+      <c r="P62">
+        <v>80329251.499308005</v>
+      </c>
       <c r="AP62" s="1"/>
       <c r="AQ62" s="1"/>
       <c r="CA62" s="1"/>
@@ -3584,6 +3963,12 @@
       <c r="N63">
         <v>39211.457292999999</v>
       </c>
+      <c r="O63">
+        <v>6.6740969999999997</v>
+      </c>
+      <c r="P63">
+        <v>81171516.915062994</v>
+      </c>
       <c r="AP63" s="1"/>
       <c r="AQ63" s="1"/>
       <c r="CA63" s="1"/>
@@ -3635,6 +4020,12 @@
       <c r="N64">
         <v>38997.489335999999</v>
       </c>
+      <c r="O64">
+        <v>6.6749729999999996</v>
+      </c>
+      <c r="P64">
+        <v>82009118.874816</v>
+      </c>
       <c r="AP64" s="1"/>
       <c r="AQ64" s="1"/>
       <c r="CA64" s="1"/>
@@ -3686,6 +4077,12 @@
       <c r="N65">
         <v>38780.516846999999</v>
       </c>
+      <c r="O65">
+        <v>6.6759969999999997</v>
+      </c>
+      <c r="P65">
+        <v>82840803.318476006</v>
+      </c>
       <c r="AP65" s="1"/>
       <c r="AQ65" s="1"/>
       <c r="CA65" s="1"/>
@@ -3737,6 +4134,12 @@
       <c r="N66">
         <v>38560.544387000002</v>
       </c>
+      <c r="O66">
+        <v>6.6771640000000003</v>
+      </c>
+      <c r="P66">
+        <v>83665425.137450993</v>
+      </c>
       <c r="AP66" s="1"/>
       <c r="AQ66" s="1"/>
       <c r="CE66" s="1"/>
@@ -3786,6 +4189,12 @@
       <c r="N67">
         <v>38337.578535000001</v>
       </c>
+      <c r="O67">
+        <v>6.6784670000000004</v>
+      </c>
+      <c r="P67">
+        <v>84481922.130888</v>
+      </c>
       <c r="AP67" s="1"/>
       <c r="AQ67" s="1"/>
       <c r="CE67" s="1"/>
@@ -3835,6 +4244,12 @@
       <c r="N68">
         <v>38111.627936999997</v>
       </c>
+      <c r="O68">
+        <v>6.6799049999999998</v>
+      </c>
+      <c r="P68">
+        <v>85289293.614041001</v>
+      </c>
       <c r="AP68" s="1"/>
       <c r="AQ68" s="1"/>
       <c r="CE68" s="1"/>
@@ -3884,6 +4299,12 @@
       <c r="N69">
         <v>37882.703353999997</v>
       </c>
+      <c r="O69">
+        <v>6.6814710000000002</v>
+      </c>
+      <c r="P69">
+        <v>86086584.725652993</v>
+      </c>
       <c r="AP69" s="1"/>
       <c r="AQ69" s="1"/>
       <c r="CE69" s="1"/>
@@ -3933,6 +4354,12 @@
       <c r="N70">
         <v>37650.817708000002</v>
       </c>
+      <c r="O70">
+        <v>6.6831620000000003</v>
+      </c>
+      <c r="P70">
+        <v>86872876.248839006</v>
+      </c>
       <c r="AP70" s="1"/>
       <c r="AQ70" s="1"/>
       <c r="CE70" s="1"/>
@@ -3982,6 +4409,12 @@
       <c r="N71">
         <v>37415.986126000003</v>
       </c>
+      <c r="O71">
+        <v>6.6849740000000004</v>
+      </c>
+      <c r="P71">
+        <v>87647278.900149003</v>
+      </c>
       <c r="AP71" s="1"/>
       <c r="AQ71" s="1"/>
       <c r="CE71" s="1"/>
@@ -4031,6 +4464,12 @@
       <c r="N72">
         <v>37178.225982999997</v>
       </c>
+      <c r="O72">
+        <v>6.686903</v>
+      </c>
+      <c r="P72">
+        <v>88408930.631889999</v>
+      </c>
       <c r="AP72" s="1"/>
       <c r="AQ72" s="1"/>
       <c r="CE72" s="1"/>
@@ -4080,6 +4519,12 @@
       <c r="N73">
         <v>36937.556938000002</v>
       </c>
+      <c r="O73">
+        <v>6.6889459999999996</v>
+      </c>
+      <c r="P73">
+        <v>89156995.491971001</v>
+      </c>
       <c r="AP73" s="1"/>
       <c r="AQ73" s="1"/>
       <c r="FV73" s="1"/>
@@ -4127,6 +4572,12 @@
       <c r="N74">
         <v>36694.000973000002</v>
       </c>
+      <c r="O74">
+        <v>6.6910999999999996</v>
+      </c>
+      <c r="P74">
+        <v>89890662.875899002</v>
+      </c>
       <c r="AP74" s="1"/>
       <c r="AQ74" s="1"/>
       <c r="FV74" s="1"/>
@@ -4174,6 +4625,12 @@
       <c r="N75">
         <v>36447.582427000001</v>
       </c>
+      <c r="O75">
+        <v>6.6933610000000003</v>
+      </c>
+      <c r="P75">
+        <v>90609146.440864995</v>
+      </c>
       <c r="AP75" s="1"/>
       <c r="AQ75" s="1"/>
       <c r="FV75" s="1"/>
@@ -4221,6 +4678,12 @@
       <c r="N76">
         <v>36198.328025000003</v>
       </c>
+      <c r="O76">
+        <v>6.6957259999999996</v>
+      </c>
+      <c r="P76">
+        <v>91311682.397202998</v>
+      </c>
       <c r="AP76" s="1"/>
       <c r="AQ76" s="1"/>
       <c r="FV76" s="1"/>
@@ -4268,6 +4731,12 @@
       <c r="N77">
         <v>35946.266904999997</v>
       </c>
+      <c r="O77">
+        <v>6.6981929999999998</v>
+      </c>
+      <c r="P77">
+        <v>91997527.250020996</v>
+      </c>
       <c r="AP77" s="1"/>
       <c r="AQ77" s="1"/>
       <c r="FV77" s="1"/>
@@ -4315,6 +4784,12 @@
       <c r="N78">
         <v>35691.430643</v>
       </c>
+      <c r="O78">
+        <v>6.7007580000000004</v>
+      </c>
+      <c r="P78">
+        <v>92665955.283508003</v>
+      </c>
       <c r="AP78" s="1"/>
       <c r="AQ78" s="1"/>
       <c r="FV78" s="1"/>
@@ -4362,6 +4837,12 @@
       <c r="N79">
         <v>35433.853273000001</v>
       </c>
+      <c r="O79">
+        <v>6.7034200000000004</v>
+      </c>
+      <c r="P79">
+        <v>93316256.156391993</v>
+      </c>
       <c r="AP79" s="1"/>
       <c r="AQ79" s="1"/>
       <c r="FV79" s="1"/>
@@ -4409,6 +4890,12 @@
       <c r="N80">
         <v>35173.571303999997</v>
       </c>
+      <c r="O80">
+        <v>6.706175</v>
+      </c>
+      <c r="P80">
+        <v>93947732.936560005</v>
+      </c>
       <c r="AP80" s="1"/>
       <c r="AQ80" s="1"/>
       <c r="FV80" s="1"/>
@@ -4456,6 +4943,12 @@
       <c r="N81">
         <v>34910.623733</v>
       </c>
+      <c r="O81">
+        <v>6.709022</v>
+      </c>
+      <c r="P81">
+        <v>94559700.790041</v>
+      </c>
       <c r="AP81" s="1"/>
       <c r="AQ81" s="1"/>
       <c r="FV81" s="1"/>
@@ -4503,6 +4996,12 @@
       <c r="N82">
         <v>34645.052049999998</v>
       </c>
+      <c r="O82">
+        <v>6.7119580000000001</v>
+      </c>
+      <c r="P82">
+        <v>95151486.401362002</v>
+      </c>
       <c r="AP82" s="1"/>
       <c r="AQ82" s="1"/>
       <c r="FV82" s="1"/>
@@ -4550,6 +5049,12 @@
       <c r="N83">
         <v>34376.900248999998</v>
       </c>
+      <c r="O83">
+        <v>6.7149799999999997</v>
+      </c>
+      <c r="P83">
+        <v>95722428.077230006</v>
+      </c>
       <c r="AP83" s="1"/>
       <c r="AQ83" s="1"/>
       <c r="FV83" s="1"/>
@@ -4597,6 +5102,12 @@
       <c r="N84">
         <v>34106.214822000002</v>
       </c>
+      <c r="O84">
+        <v>6.7180879999999998</v>
+      </c>
+      <c r="P84">
+        <v>96271876.397734001</v>
+      </c>
       <c r="AP84" s="1"/>
       <c r="AQ84" s="1"/>
       <c r="FV84" s="1"/>
@@ -4644,6 +5155,12 @@
       <c r="N85">
         <v>33833.044757000003</v>
       </c>
+      <c r="O85">
+        <v>6.7212779999999999</v>
+      </c>
+      <c r="P85">
+        <v>96799195.237954006</v>
+      </c>
       <c r="AP85" s="1"/>
       <c r="AQ85" s="1"/>
       <c r="FV85" s="1"/>
@@ -4691,6 +5208,12 @@
       <c r="N86">
         <v>33557.441531999997</v>
       </c>
+      <c r="O86">
+        <v>6.7245499999999998</v>
+      </c>
+      <c r="P86">
+        <v>97303762.984086007</v>
+      </c>
       <c r="AP86" s="1"/>
       <c r="AQ86" s="1"/>
       <c r="FV86" s="1"/>
@@ -4738,6 +5261,12 @@
       <c r="N87">
         <v>33279.459094999998</v>
       </c>
+      <c r="O87">
+        <v>6.7279010000000001</v>
+      </c>
+      <c r="P87">
+        <v>97784973.800134003</v>
+      </c>
       <c r="AP87" s="1"/>
       <c r="AQ87" s="1"/>
       <c r="FV87" s="1"/>
@@ -4785,6 +5314,12 @@
       <c r="N88">
         <v>32999.153850000002</v>
       </c>
+      <c r="O88">
+        <v>6.731331</v>
+      </c>
+      <c r="P88">
+        <v>98242238.848814994</v>
+      </c>
       <c r="AP88" s="1"/>
       <c r="AQ88" s="1"/>
       <c r="FV88" s="1"/>
@@ -4832,6 +5367,12 @@
       <c r="N89">
         <v>32716.584633999999</v>
       </c>
+      <c r="O89">
+        <v>6.7348359999999996</v>
+      </c>
+      <c r="P89">
+        <v>98674987.419439003</v>
+      </c>
       <c r="AP89" s="1"/>
       <c r="AQ89" s="1"/>
       <c r="FV89" s="1"/>
@@ -4879,6 +5420,12 @@
       <c r="N90">
         <v>32431.812687000001</v>
       </c>
+      <c r="O90">
+        <v>6.738416</v>
+      </c>
+      <c r="P90">
+        <v>99082667.955914006</v>
+      </c>
       <c r="AP90" s="1"/>
       <c r="AQ90" s="1"/>
       <c r="FV90" s="1"/>
@@ -4926,6 +5473,12 @@
       <c r="N91">
         <v>32144.901618</v>
       </c>
+      <c r="O91">
+        <v>6.74207</v>
+      </c>
+      <c r="P91">
+        <v>99464749.004245996</v>
+      </c>
       <c r="AP91" s="1"/>
       <c r="AQ91" s="1"/>
       <c r="FV91" s="1"/>
@@ -4973,6 +5526,12 @@
       <c r="N92">
         <v>31855.917372</v>
       </c>
+      <c r="O92">
+        <v>6.7457960000000003</v>
+      </c>
+      <c r="P92">
+        <v>99820720.110009</v>
+      </c>
       <c r="AP92" s="1"/>
       <c r="AQ92" s="1"/>
       <c r="FV92" s="1"/>
@@ -5020,6 +5579,12 @@
       <c r="N93">
         <v>31564.928177999998</v>
       </c>
+      <c r="O93">
+        <v>6.749593</v>
+      </c>
+      <c r="P93">
+        <v>100150092.694903</v>
+      </c>
       <c r="AP93" s="1"/>
       <c r="AQ93" s="1"/>
       <c r="FV93" s="1"/>
@@ -5067,6 +5632,12 @@
       <c r="N94">
         <v>31272.004510999999</v>
       </c>
+      <c r="O94">
+        <v>6.7534590000000003</v>
+      </c>
+      <c r="P94">
+        <v>100452400.931989</v>
+      </c>
       <c r="AP94" s="1"/>
       <c r="AQ94" s="1"/>
       <c r="FV94" s="1"/>
@@ -5114,6 +5685,12 @@
       <c r="N95">
         <v>30977.219031000001</v>
       </c>
+      <c r="O95">
+        <v>6.7573939999999997</v>
+      </c>
+      <c r="P95">
+        <v>100727202.62637</v>
+      </c>
       <c r="AP95" s="1"/>
       <c r="AQ95" s="1"/>
       <c r="FV95" s="1"/>
@@ -5161,6 +5738,12 @@
       <c r="N96">
         <v>30680.646529000001</v>
       </c>
+      <c r="O96">
+        <v>6.7613960000000004</v>
+      </c>
+      <c r="P96">
+        <v>100974080.09583201</v>
+      </c>
       <c r="AP96" s="1"/>
       <c r="AQ96" s="1"/>
       <c r="FV96" s="1"/>
@@ -5208,6 +5791,12 @@
       <c r="N97">
         <v>30382.363861000002</v>
       </c>
+      <c r="O97">
+        <v>6.7654639999999997</v>
+      </c>
+      <c r="P97">
+        <v>101192641.03707699</v>
+      </c>
       <c r="AP97" s="1"/>
       <c r="AQ97" s="1"/>
       <c r="FV97" s="1"/>
@@ -5255,6 +5844,12 @@
       <c r="N98">
         <v>30082.449883000001</v>
       </c>
+      <c r="O98">
+        <v>6.7695980000000002</v>
+      </c>
+      <c r="P98">
+        <v>101382519.35861</v>
+      </c>
       <c r="AP98" s="1"/>
       <c r="AQ98" s="1"/>
       <c r="FV98" s="1"/>
@@ -5302,6 +5897,12 @@
       <c r="N99">
         <v>29780.985379000002</v>
       </c>
+      <c r="O99">
+        <v>6.7737959999999999</v>
+      </c>
+      <c r="P99">
+        <v>101543375.961037</v>
+      </c>
       <c r="AP99" s="1"/>
       <c r="AQ99" s="1"/>
       <c r="FV99" s="1"/>
@@ -5349,6 +5950,12 @@
       <c r="N100">
         <v>29478.052978</v>
       </c>
+      <c r="O100">
+        <v>6.7780570000000004</v>
+      </c>
+      <c r="P100">
+        <v>101674899.448379</v>
+      </c>
       <c r="AP100" s="1"/>
       <c r="AQ100" s="1"/>
       <c r="FV100" s="1"/>
@@ -5396,6 +6003,12 @@
       <c r="N101">
         <v>29173.737078999999</v>
       </c>
+      <c r="O101">
+        <v>6.782381</v>
+      </c>
+      <c r="P101">
+        <v>101776806.758644</v>
+      </c>
       <c r="AP101" s="1"/>
       <c r="AQ101" s="1"/>
       <c r="FV101" s="1"/>
@@ -5443,6 +6056,12 @@
       <c r="N102">
         <v>28868.123760999999</v>
       </c>
+      <c r="O102">
+        <v>6.7867670000000002</v>
+      </c>
+      <c r="P102">
+        <v>101848843.706908</v>
+      </c>
       <c r="AP102" s="1"/>
       <c r="AQ102" s="1"/>
       <c r="FV102" s="1"/>
@@ -5490,6 +6109,12 @@
       <c r="N103">
         <v>28561.300694000001</v>
       </c>
+      <c r="O103">
+        <v>6.7912129999999999</v>
+      </c>
+      <c r="P103">
+        <v>101890785.438538</v>
+      </c>
       <c r="AP103" s="1"/>
       <c r="AQ103" s="1"/>
       <c r="FV103" s="1"/>
@@ -5537,6 +6162,12 @@
       <c r="N104">
         <v>28253.357044</v>
       </c>
+      <c r="O104">
+        <v>6.7957200000000002</v>
+      </c>
+      <c r="P104">
+        <v>101902436.79333401</v>
+      </c>
       <c r="AP104" s="1"/>
       <c r="AQ104" s="1"/>
       <c r="FV104" s="1"/>
@@ -5584,6 +6215,12 @@
       <c r="N105">
         <v>27944.383375000001</v>
       </c>
+      <c r="O105">
+        <v>6.8002849999999997</v>
+      </c>
+      <c r="P105">
+        <v>101883632.583055</v>
+      </c>
       <c r="AP105" s="1"/>
       <c r="AQ105" s="1"/>
       <c r="FV105" s="1"/>
@@ -5631,6 +6268,12 @@
       <c r="N106">
         <v>27634.471548000001</v>
       </c>
+      <c r="O106">
+        <v>6.8049090000000003</v>
+      </c>
+      <c r="P106">
+        <v>101834237.78532501</v>
+      </c>
       <c r="AP106" s="1"/>
       <c r="AQ106" s="1"/>
       <c r="FV106" s="1"/>
@@ -5678,6 +6321,12 @@
       <c r="N107">
         <v>27323.714613</v>
       </c>
+      <c r="O107">
+        <v>6.8095910000000002</v>
+      </c>
+      <c r="P107">
+        <v>101754147.656532</v>
+      </c>
       <c r="AP107" s="1"/>
       <c r="AQ107" s="1"/>
       <c r="FV107" s="1"/>
@@ -5725,6 +6374,12 @@
       <c r="N108">
         <v>27012.206706000001</v>
       </c>
+      <c r="O108">
+        <v>6.81433</v>
+      </c>
+      <c r="P108">
+        <v>101643287.76554</v>
+      </c>
       <c r="AP108" s="1"/>
       <c r="AQ108" s="1"/>
       <c r="FV108" s="1"/>
@@ -5772,6 +6427,12 @@
       <c r="N109">
         <v>26700.042931</v>
       </c>
+      <c r="O109">
+        <v>6.8191249999999997</v>
+      </c>
+      <c r="P109">
+        <v>101501613.949265</v>
+      </c>
       <c r="AP109" s="1"/>
       <c r="AQ109" s="1"/>
       <c r="FV109" s="1"/>
@@ -5819,6 +6480,12 @@
       <c r="N110">
         <v>26387.319251000001</v>
       </c>
+      <c r="O110">
+        <v>6.823976</v>
+      </c>
+      <c r="P110">
+        <v>101329112.19053601</v>
+      </c>
       <c r="AP110" s="1"/>
       <c r="AQ110" s="1"/>
       <c r="FV110" s="1"/>
@@ -5866,6 +6533,12 @@
       <c r="N111">
         <v>26074.132371</v>
       </c>
+      <c r="O111">
+        <v>6.828881</v>
+      </c>
+      <c r="P111">
+        <v>101125798.41851801</v>
+      </c>
       <c r="AP111" s="1"/>
       <c r="AQ111" s="1"/>
       <c r="FV111" s="1"/>
@@ -5913,6 +6586,12 @@
       <c r="N112">
         <v>25760.579618</v>
       </c>
+      <c r="O112">
+        <v>6.8338409999999996</v>
+      </c>
+      <c r="P112">
+        <v>100891718.232095</v>
+      </c>
       <c r="AP112" s="1"/>
       <c r="AQ112" s="1"/>
       <c r="FV112" s="1"/>
@@ -5960,6 +6639,12 @@
       <c r="N113">
         <v>25446.758823</v>
       </c>
+      <c r="O113">
+        <v>6.8388540000000004</v>
+      </c>
+      <c r="P113">
+        <v>100626946.547124</v>
+      </c>
       <c r="AP113" s="1"/>
       <c r="AQ113" s="1"/>
       <c r="FV113" s="1"/>
@@ -6007,6 +6692,12 @@
       <c r="N114">
         <v>25132.768197000001</v>
       </c>
+      <c r="O114">
+        <v>6.8439199999999998</v>
+      </c>
+      <c r="P114">
+        <v>100331587.16914199</v>
+      </c>
       <c r="AP114" s="1"/>
       <c r="AQ114" s="1"/>
       <c r="FV114" s="1"/>
@@ -6054,6 +6745,12 @@
       <c r="N115">
         <v>24818.706212000001</v>
       </c>
+      <c r="O115">
+        <v>6.8490380000000002</v>
+      </c>
+      <c r="P115">
+        <v>100005772.293795</v>
+      </c>
       <c r="AP115" s="1"/>
       <c r="AQ115" s="1"/>
       <c r="FV115" s="1"/>
@@ -6101,6 +6798,12 @@
       <c r="N116">
         <v>24504.671477</v>
       </c>
+      <c r="O116">
+        <v>6.8542079999999999</v>
+      </c>
+      <c r="P116">
+        <v>99649661.937995002</v>
+      </c>
       <c r="AP116" s="1"/>
       <c r="AQ116" s="1"/>
       <c r="FV116" s="1"/>
@@ -6148,6 +6851,12 @@
       <c r="N117">
         <v>24190.762610000002</v>
       </c>
+      <c r="O117">
+        <v>6.8594290000000004</v>
+      </c>
+      <c r="P117">
+        <v>99263443.305324003</v>
+      </c>
       <c r="AP117" s="1"/>
       <c r="AQ117" s="1"/>
       <c r="FV117" s="1"/>
@@ -6195,6 +6904,12 @@
       <c r="N118">
         <v>23877.078119999998</v>
       </c>
+      <c r="O118">
+        <v>6.8646989999999999</v>
+      </c>
+      <c r="P118">
+        <v>98847330.089675993</v>
+      </c>
       <c r="AP118" s="1"/>
       <c r="AQ118" s="1"/>
       <c r="FV118" s="1"/>
@@ -6242,6 +6957,12 @@
       <c r="N119">
         <v>23563.716280000001</v>
       </c>
+      <c r="O119">
+        <v>6.8700200000000002</v>
+      </c>
+      <c r="P119">
+        <v>98401561.721385002</v>
+      </c>
       <c r="AP119" s="1"/>
       <c r="AQ119" s="1"/>
       <c r="FV119" s="1"/>
@@ -6289,6 +7010,12 @@
       <c r="N120">
         <v>23250.775002999999</v>
       </c>
+      <c r="O120">
+        <v>6.8753890000000002</v>
+      </c>
+      <c r="P120">
+        <v>97926402.560293004</v>
+      </c>
       <c r="AP120" s="1"/>
       <c r="AQ120" s="1"/>
       <c r="FV120" s="1"/>
@@ -6336,6 +7063,12 @@
       <c r="N121">
         <v>22938.351723</v>
       </c>
+      <c r="O121">
+        <v>6.8808059999999998</v>
+      </c>
+      <c r="P121">
+        <v>97422141.040292993</v>
+      </c>
       <c r="AP121" s="1"/>
       <c r="AQ121" s="1"/>
       <c r="FV121" s="1"/>
@@ -6383,6 +7116,12 @@
       <c r="N122">
         <v>22626.543272999999</v>
       </c>
+      <c r="O122">
+        <v>6.8862709999999998</v>
+      </c>
+      <c r="P122">
+        <v>96889088.769942001</v>
+      </c>
       <c r="AP122" s="1"/>
       <c r="AQ122" s="1"/>
       <c r="FV122" s="1"/>
@@ -6430,6 +7169,12 @@
       <c r="N123">
         <v>22315.445763</v>
       </c>
+      <c r="O123">
+        <v>6.8917820000000001</v>
+      </c>
+      <c r="P123">
+        <v>96327579.593776003</v>
+      </c>
       <c r="AP123" s="1"/>
       <c r="AQ123" s="1"/>
       <c r="FV123" s="1"/>
@@ -6477,6 +7222,12 @@
       <c r="N124">
         <v>22005.154462999999</v>
       </c>
+      <c r="O124">
+        <v>6.8973389999999997</v>
+      </c>
+      <c r="P124">
+        <v>95737968.618974999</v>
+      </c>
       <c r="AP124" s="1"/>
       <c r="AQ124" s="1"/>
       <c r="FV124" s="1"/>
@@ -6524,6 +7275,12 @@
       <c r="N125">
         <v>21695.763691</v>
       </c>
+      <c r="O125">
+        <v>6.9029420000000004</v>
+      </c>
+      <c r="P125">
+        <v>95120631.212064996</v>
+      </c>
       <c r="AP125" s="1"/>
       <c r="AQ125" s="1"/>
       <c r="FV125" s="1"/>
@@ -6571,6 +7328,12 @@
       <c r="N126">
         <v>21387.366694</v>
       </c>
+      <c r="O126">
+        <v>6.9085900000000002</v>
+      </c>
+      <c r="P126">
+        <v>94475961.970367</v>
+      </c>
       <c r="AP126" s="1"/>
       <c r="AQ126" s="1"/>
       <c r="FV126" s="1"/>
@@ -6618,6 +7381,12 @@
       <c r="N127">
         <v>21080.055543999999</v>
       </c>
+      <c r="O127">
+        <v>6.9142809999999999</v>
+      </c>
+      <c r="P127">
+        <v>93804373.672895998</v>
+      </c>
       <c r="AP127" s="1"/>
       <c r="AQ127" s="1"/>
       <c r="FV127" s="1"/>
@@ -6665,6 +7434,12 @@
       <c r="N128">
         <v>20773.921021999999</v>
       </c>
+      <c r="O128">
+        <v>6.9200150000000002</v>
+      </c>
+      <c r="P128">
+        <v>93106296.215432003</v>
+      </c>
       <c r="AP128" s="1"/>
       <c r="AQ128" s="1"/>
       <c r="FV128" s="1"/>
@@ -6712,6 +7487,12 @@
       <c r="N129">
         <v>20469.052523999999</v>
       </c>
+      <c r="O129">
+        <v>6.9257920000000004</v>
+      </c>
+      <c r="P129">
+        <v>92382175.534427002</v>
+      </c>
       <c r="AP129" s="1"/>
       <c r="AQ129" s="1"/>
       <c r="FV129" s="1"/>
@@ -6759,6 +7540,12 @@
       <c r="N130">
         <v>20165.537950999998</v>
       </c>
+      <c r="O130">
+        <v>6.9316110000000002</v>
+      </c>
+      <c r="P130">
+        <v>91632472.524350002</v>
+      </c>
       <c r="AP130" s="1"/>
       <c r="AQ130" s="1"/>
       <c r="FV130" s="1"/>
@@ -6806,6 +7593,12 @@
       <c r="N131">
         <v>19863.463616000001</v>
       </c>
+      <c r="O131">
+        <v>6.9374700000000002</v>
+      </c>
+      <c r="P131">
+        <v>90857661.952960998</v>
+      </c>
       <c r="AP131" s="1"/>
       <c r="AQ131" s="1"/>
       <c r="FV131" s="1"/>
@@ -6853,6 +7646,12 @@
       <c r="N132">
         <v>19562.914153000002</v>
       </c>
+      <c r="O132">
+        <v>6.9433699999999998</v>
+      </c>
+      <c r="P132">
+        <v>90058231.378874004</v>
+      </c>
       <c r="AP132" s="1"/>
       <c r="AQ132" s="1"/>
       <c r="FV132" s="1"/>
@@ -6900,6 +7699,12 @@
       <c r="N133">
         <v>19263.972421999999</v>
       </c>
+      <c r="O133">
+        <v>6.9493080000000003</v>
+      </c>
+      <c r="P133">
+        <v>89234680.075579002</v>
+      </c>
       <c r="AP133" s="1"/>
       <c r="AQ133" s="1"/>
       <c r="FV133" s="1"/>
@@ -6947,6 +7752,12 @@
       <c r="N134">
         <v>18966.719430000001</v>
       </c>
+      <c r="O134">
+        <v>6.9552860000000001</v>
+      </c>
+      <c r="P134">
+        <v>88387517.965910003</v>
+      </c>
       <c r="AP134" s="1"/>
       <c r="AQ134" s="1"/>
       <c r="FV134" s="1"/>
@@ -6994,6 +7805,12 @@
       <c r="N135">
         <v>18671.234247</v>
       </c>
+      <c r="O135">
+        <v>6.9613009999999997</v>
+      </c>
+      <c r="P135">
+        <v>87517264.570720002</v>
+      </c>
       <c r="AP135" s="1"/>
       <c r="AQ135" s="1"/>
       <c r="FV135" s="1"/>
@@ -7041,6 +7858,12 @@
       <c r="N136">
         <v>18377.593933</v>
       </c>
+      <c r="O136">
+        <v>6.9673530000000001</v>
+      </c>
+      <c r="P136">
+        <v>86624447.975272998</v>
+      </c>
       <c r="AP136" s="1"/>
       <c r="AQ136" s="1"/>
       <c r="FV136" s="1"/>
@@ -7088,6 +7911,12 @@
       <c r="N137">
         <v>18085.873464</v>
       </c>
+      <c r="O137">
+        <v>6.9734410000000002</v>
+      </c>
+      <c r="P137">
+        <v>85709603.816626996</v>
+      </c>
       <c r="AP137" s="1"/>
       <c r="AQ137" s="1"/>
       <c r="FV137" s="1"/>
@@ -7135,6 +7964,12 @@
       <c r="N138">
         <v>17796.145670000002</v>
       </c>
+      <c r="O138">
+        <v>6.9795639999999999</v>
+      </c>
+      <c r="P138">
+        <v>84773274.295013994</v>
+      </c>
       <c r="AP138" s="1"/>
       <c r="AQ138" s="1"/>
       <c r="FV138" s="1"/>
@@ -7182,6 +8017,12 @@
       <c r="N139">
         <v>17508.481169999999</v>
       </c>
+      <c r="O139">
+        <v>6.985722</v>
+      </c>
+      <c r="P139">
+        <v>83816007.211940005</v>
+      </c>
       <c r="AP139" s="1"/>
       <c r="AQ139" s="1"/>
       <c r="FV139" s="1"/>
@@ -7229,6 +8070,12 @@
       <c r="N140">
         <v>17222.948316999998</v>
       </c>
+      <c r="O140">
+        <v>6.9919130000000003</v>
+      </c>
+      <c r="P140">
+        <v>82838355.037488997</v>
+      </c>
       <c r="AP140" s="1"/>
       <c r="AQ140" s="1"/>
       <c r="FV140" s="1"/>
@@ -7276,6 +8123,12 @@
       <c r="N141">
         <v>16939.613149000001</v>
       </c>
+      <c r="O141">
+        <v>6.9981369999999998</v>
+      </c>
+      <c r="P141">
+        <v>81840874.008987993</v>
+      </c>
       <c r="AP141" s="1"/>
       <c r="AQ141" s="1"/>
       <c r="FV141" s="1"/>
@@ -7323,6 +8176,12 @@
       <c r="N142">
         <v>16658.539341</v>
       </c>
+      <c r="O142">
+        <v>7.0043930000000003</v>
+      </c>
+      <c r="P142">
+        <v>80824123.262950003</v>
+      </c>
       <c r="AP142" s="1"/>
       <c r="AQ142" s="1"/>
       <c r="FV142" s="1"/>
@@ -7370,6 +8229,12 @@
       <c r="N143">
         <v>16379.788166</v>
       </c>
+      <c r="O143">
+        <v>7.0106799999999998</v>
+      </c>
+      <c r="P143">
+        <v>79788664.001926005</v>
+      </c>
       <c r="AP143" s="1"/>
       <c r="AQ143" s="1"/>
       <c r="FV143" s="1"/>
@@ -7417,6 +8282,12 @@
       <c r="N144">
         <v>16103.418455000001</v>
       </c>
+      <c r="O144">
+        <v>7.0169959999999998</v>
+      </c>
+      <c r="P144">
+        <v>78735058.697602004</v>
+      </c>
       <c r="AP144" s="1"/>
       <c r="AQ144" s="1"/>
       <c r="FV144" s="1"/>
@@ -7464,6 +8335,12 @@
       <c r="N145">
         <v>15829.486573</v>
       </c>
+      <c r="O145">
+        <v>7.0233420000000004</v>
+      </c>
+      <c r="P145">
+        <v>77663870.33123</v>
+      </c>
       <c r="AP145" s="1"/>
       <c r="AQ145" s="1"/>
       <c r="FV145" s="1"/>
@@ -7511,6 +8388,12 @@
       <c r="N146">
         <v>15558.046388000001</v>
       </c>
+      <c r="O146">
+        <v>7.0297159999999996</v>
+      </c>
+      <c r="P146">
+        <v>76575661.672195002</v>
+      </c>
       <c r="AP146" s="1"/>
       <c r="AQ146" s="1"/>
       <c r="FV146" s="1"/>
@@ -7558,6 +8441,12 @@
       <c r="N147">
         <v>15289.149254</v>
       </c>
+      <c r="O147">
+        <v>7.0361180000000001</v>
+      </c>
+      <c r="P147">
+        <v>75470994.595281005</v>
+      </c>
       <c r="AP147" s="1"/>
       <c r="AQ147" s="1"/>
       <c r="FV147" s="1"/>
@@ -7605,6 +8494,12 @@
       <c r="N148">
         <v>15022.843994000001</v>
       </c>
+      <c r="O148">
+        <v>7.0425449999999996</v>
+      </c>
+      <c r="P148">
+        <v>74350429.436939001</v>
+      </c>
       <c r="AP148" s="1"/>
       <c r="AQ148" s="1"/>
       <c r="FV148" s="1"/>
@@ -7652,6 +8547,12 @@
       <c r="N149">
         <v>14759.176887</v>
       </c>
+      <c r="O149">
+        <v>7.0489990000000002</v>
+      </c>
+      <c r="P149">
+        <v>73214524.390615001</v>
+      </c>
       <c r="AP149" s="1"/>
       <c r="AQ149" s="1"/>
       <c r="FV149" s="1"/>
@@ -7699,6 +8600,12 @@
       <c r="N150">
         <v>14498.191666999999</v>
       </c>
+      <c r="O150">
+        <v>7.0554769999999998</v>
+      </c>
+      <c r="P150">
+        <v>72063834.941009</v>
+      </c>
       <c r="AP150" s="1"/>
       <c r="AQ150" s="1"/>
       <c r="FV150" s="1"/>
@@ -7746,6 +8653,12 @@
       <c r="N151">
         <v>14239.929518999999</v>
       </c>
+      <c r="O151">
+        <v>7.0619779999999999</v>
+      </c>
+      <c r="P151">
+        <v>70898913.336869001</v>
+      </c>
       <c r="AP151" s="1"/>
       <c r="AQ151" s="1"/>
       <c r="FV151" s="1"/>
@@ -7793,6 +8706,12 @@
       <c r="N152">
         <v>13984.429082000001</v>
       </c>
+      <c r="O152">
+        <v>7.0685029999999998</v>
+      </c>
+      <c r="P152">
+        <v>69720308.101795003</v>
+      </c>
       <c r="AP152" s="1"/>
       <c r="AQ152" s="1"/>
       <c r="FV152" s="1"/>
@@ -7840,6 +8759,12 @@
       <c r="N153">
         <v>13731.726457000001</v>
       </c>
+      <c r="O153">
+        <v>7.0750489999999999</v>
+      </c>
+      <c r="P153">
+        <v>68528563.582288995</v>
+      </c>
       <c r="AP153" s="1"/>
       <c r="AQ153" s="1"/>
       <c r="FV153" s="1"/>
@@ -7887,6 +8812,12 @@
       <c r="N154">
         <v>13481.855218000001</v>
       </c>
+      <c r="O154">
+        <v>7.0816160000000004</v>
+      </c>
+      <c r="P154">
+        <v>67324219.532162994</v>
+      </c>
       <c r="AP154" s="1"/>
       <c r="AQ154" s="1"/>
       <c r="FV154" s="1"/>
@@ -7934,6 +8865,12 @@
       <c r="N155">
         <v>13234.846432</v>
       </c>
+      <c r="O155">
+        <v>7.088203</v>
+      </c>
+      <c r="P155">
+        <v>66107810.732262</v>
+      </c>
       <c r="AP155" s="1"/>
       <c r="AQ155" s="1"/>
       <c r="FV155" s="1"/>
@@ -7981,6 +8918,12 @@
       <c r="N156">
         <v>12990.728673</v>
       </c>
+      <c r="O156">
+        <v>7.0948089999999997</v>
+      </c>
+      <c r="P156">
+        <v>64879866.644317001</v>
+      </c>
       <c r="AP156" s="1"/>
       <c r="AQ156" s="1"/>
       <c r="FV156" s="1"/>
@@ -8028,6 +8971,12 @@
       <c r="N157">
         <v>12749.528050999999</v>
       </c>
+      <c r="O157">
+        <v>7.1014330000000001</v>
+      </c>
+      <c r="P157">
+        <v>63640911.097646996</v>
+      </c>
       <c r="AP157" s="1"/>
       <c r="AQ157" s="1"/>
       <c r="FV157" s="1"/>
@@ -8075,6 +9024,12 @@
       <c r="N158">
         <v>12511.268237</v>
       </c>
+      <c r="O158">
+        <v>7.1080740000000002</v>
+      </c>
+      <c r="P158">
+        <v>62391462.007316001</v>
+      </c>
       <c r="AP158" s="1"/>
       <c r="AQ158" s="1"/>
       <c r="FV158" s="1"/>
@@ -8122,6 +9077,12 @@
       <c r="N159">
         <v>12275.970493999999</v>
       </c>
+      <c r="O159">
+        <v>7.1147309999999999</v>
+      </c>
+      <c r="P159">
+        <v>61132031.122290999</v>
+      </c>
       <c r="AP159" s="1"/>
       <c r="AQ159" s="1"/>
       <c r="FV159" s="1"/>
@@ -8169,6 +9130,12 @@
       <c r="N160">
         <v>12043.653709</v>
       </c>
+      <c r="O160">
+        <v>7.1214040000000001</v>
+      </c>
+      <c r="P160">
+        <v>59863123.802061997</v>
+      </c>
       <c r="AP160" s="1"/>
       <c r="AQ160" s="1"/>
       <c r="FV160" s="1"/>
@@ -8216,6 +9183,12 @@
       <c r="N161">
         <v>11814.334435000001</v>
       </c>
+      <c r="O161">
+        <v>7.1280910000000004</v>
+      </c>
+      <c r="P161">
+        <v>58585238.820138998</v>
+      </c>
       <c r="AP161" s="1"/>
       <c r="AQ161" s="1"/>
       <c r="FV161" s="1"/>
@@ -8241,6 +9214,9 @@
       </c>
       <c r="J162">
         <v>29355.635704</v>
+      </c>
+      <c r="O162">
+        <v>7.1347909999999999</v>
       </c>
       <c r="AP162" s="1"/>
       <c r="AQ162" s="1"/>

</xml_diff>

<commit_message>
RESULTADOS FECHANDO COM ITHINK - MÓDULOS DE PATENTES LIGADO!
</commit_message>
<xml_diff>
--- a/models/dissertation-model/modelo-ithink/dados_ithink_excel_checks.xlsx
+++ b/models/dissertation-model/modelo-ithink/dados_ithink_excel_checks.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027" iterateDelta="1E-4"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -560,7 +560,7 @@
         <v>7.3333329999999997</v>
       </c>
       <c r="P2">
-        <v>33320873.026248001</v>
+        <v>33372956.359581001</v>
       </c>
       <c r="AP2" s="1"/>
       <c r="AQ2" s="1"/>
@@ -615,7 +615,7 @@
         <v>7.2990789999999999</v>
       </c>
       <c r="P3">
-        <v>33291373.917149998</v>
+        <v>33343846.022480998</v>
       </c>
       <c r="AP3" s="1"/>
       <c r="AQ3" s="1"/>
@@ -668,7 +668,7 @@
         <v>7.2662509999999996</v>
       </c>
       <c r="P4">
-        <v>33382641.492642</v>
+        <v>33435461.341742001</v>
       </c>
       <c r="AP4" s="1"/>
       <c r="AQ4" s="1"/>
@@ -721,7 +721,7 @@
         <v>7.2347970000000004</v>
       </c>
       <c r="P5">
-        <v>33583747.247557998</v>
+        <v>33636895.176821001</v>
       </c>
       <c r="AP5" s="1"/>
       <c r="AQ5" s="1"/>
@@ -774,7 +774,7 @@
         <v>7.2046679999999999</v>
       </c>
       <c r="P6">
-        <v>34156256.013777003</v>
+        <v>34209621.586962998</v>
       </c>
       <c r="AP6" s="1"/>
       <c r="AQ6" s="1"/>
@@ -827,7 +827,7 @@
         <v>7.1758160000000002</v>
       </c>
       <c r="P7">
-        <v>35387174.667952999</v>
+        <v>35440541.191720001</v>
       </c>
       <c r="AP7" s="1"/>
       <c r="AQ7" s="1"/>
@@ -880,7 +880,7 @@
         <v>7.1481960000000004</v>
       </c>
       <c r="P8">
-        <v>37447834.451920003</v>
+        <v>37500923.477287002</v>
       </c>
       <c r="AP8" s="1"/>
       <c r="AQ8" s="1"/>
@@ -933,7 +933,7 @@
         <v>7.1217639999999998</v>
       </c>
       <c r="P9">
-        <v>40338875.448019996</v>
+        <v>40391416.089759</v>
       </c>
       <c r="AP9" s="1"/>
       <c r="AQ9" s="1"/>
@@ -986,7 +986,7 @@
         <v>7.096476</v>
       </c>
       <c r="P10">
-        <v>43900405.734217003</v>
+        <v>43952197.578226</v>
       </c>
       <c r="AP10" s="1"/>
       <c r="AQ10" s="1"/>
@@ -1039,7 +1039,7 @@
         <v>7.0722930000000002</v>
       </c>
       <c r="P11">
-        <v>47863176.510031</v>
+        <v>47914126.149590001</v>
       </c>
       <c r="AP11" s="1"/>
       <c r="AQ11" s="1"/>
@@ -1092,7 +1092,7 @@
         <v>7.049175</v>
       </c>
       <c r="P12">
-        <v>51916581.784474999</v>
+        <v>51966708.294238001</v>
       </c>
       <c r="AP12" s="1"/>
       <c r="AQ12" s="1"/>
@@ -1145,7 +1145,7 @@
         <v>7.0270840000000003</v>
       </c>
       <c r="P13">
-        <v>55773344.03413</v>
+        <v>55822760.526470996</v>
       </c>
       <c r="AP13" s="1"/>
       <c r="AQ13" s="1"/>
@@ -1198,7 +1198,7 @@
         <v>7.0059820000000004</v>
       </c>
       <c r="P14">
-        <v>59217294.143532</v>
+        <v>59266177.019899003</v>
       </c>
       <c r="AP14" s="1"/>
       <c r="AQ14" s="1"/>
@@ -1251,7 +1251,7 @@
         <v>6.9858339999999997</v>
       </c>
       <c r="P15">
-        <v>62127491.137295999</v>
+        <v>62176047.288144998</v>
       </c>
       <c r="AP15" s="1"/>
       <c r="AQ15" s="1"/>
@@ -1304,7 +1304,7 @@
         <v>6.9666069999999998</v>
       </c>
       <c r="P16">
-        <v>64477976.300902002</v>
+        <v>64526414.963812999</v>
       </c>
       <c r="AP16" s="1"/>
       <c r="AQ16" s="1"/>
@@ -1357,7 +1357,7 @@
         <v>6.9482670000000004</v>
       </c>
       <c r="P17">
-        <v>66317591.463987999</v>
+        <v>66366104.195997998</v>
       </c>
       <c r="AP17" s="1"/>
       <c r="AQ17" s="1"/>
@@ -1410,7 +1410,7 @@
         <v>6.9307829999999999</v>
       </c>
       <c r="P18">
-        <v>67738069.834040001</v>
+        <v>67786819.747245997</v>
       </c>
       <c r="AP18" s="1"/>
       <c r="AQ18" s="1"/>
@@ -1463,7 +1463,7 @@
         <v>6.9141219999999999</v>
       </c>
       <c r="P19">
-        <v>68840085.443843007</v>
+        <v>68889205.207337007</v>
       </c>
       <c r="AP19" s="1"/>
       <c r="AQ19" s="1"/>
@@ -1516,7 +1516,7 @@
         <v>6.8982559999999999</v>
       </c>
       <c r="P20">
-        <v>69705686.867737994</v>
+        <v>69755283.664789006</v>
       </c>
       <c r="AP20" s="1"/>
       <c r="AQ20" s="1"/>
@@ -1569,7 +1569,7 @@
         <v>6.8831569999999997</v>
       </c>
       <c r="P21">
-        <v>70382235.157865003</v>
+        <v>70432399.808457002</v>
       </c>
       <c r="AP21" s="1"/>
       <c r="AQ21" s="1"/>
@@ -1622,7 +1622,7 @@
         <v>6.8687950000000004</v>
       </c>
       <c r="P22">
-        <v>70862345.921941996</v>
+        <v>70913168.647002995</v>
       </c>
       <c r="AP22" s="1"/>
       <c r="AQ22" s="1"/>
@@ -1675,7 +1675,7 @@
         <v>6.8551450000000003</v>
       </c>
       <c r="P23">
-        <v>71124703.409424007</v>
+        <v>71176275.166672006</v>
       </c>
       <c r="AP23" s="1"/>
       <c r="AQ23" s="1"/>
@@ -1728,7 +1728,7 @@
         <v>6.8421810000000001</v>
       </c>
       <c r="P24">
-        <v>71158329.349359006</v>
+        <v>71210736.024608999</v>
       </c>
       <c r="AP24" s="1"/>
       <c r="AQ24" s="1"/>
@@ -1781,7 +1781,7 @@
         <v>6.8298769999999998</v>
       </c>
       <c r="P25">
-        <v>70973342.972271994</v>
+        <v>71026657.589027002</v>
       </c>
       <c r="AP25" s="1"/>
       <c r="AQ25" s="1"/>
@@ -1834,7 +1834,7 @@
         <v>6.8182090000000004</v>
       </c>
       <c r="P26">
-        <v>70601362.260073006</v>
+        <v>70655638.545504004</v>
       </c>
       <c r="AP26" s="1"/>
       <c r="AQ26" s="1"/>
@@ -1887,7 +1887,7 @@
         <v>6.8071549999999998</v>
       </c>
       <c r="P27">
-        <v>70089286.551767007</v>
+        <v>70144555.587386996</v>
       </c>
       <c r="AP27" s="1"/>
       <c r="AQ27" s="1"/>
@@ -1940,7 +1940,7 @@
         <v>6.796691</v>
       </c>
       <c r="P28">
-        <v>69490322.338899001</v>
+        <v>69546592.701141998</v>
       </c>
       <c r="AP28" s="1"/>
       <c r="AQ28" s="1"/>
@@ -1993,7 +1993,7 @@
         <v>6.7867949999999997</v>
       </c>
       <c r="P29">
-        <v>68855474.227477998</v>
+        <v>68912735.068173006</v>
       </c>
       <c r="AP29" s="1"/>
       <c r="AQ29" s="1"/>
@@ -2046,7 +2046,7 @@
         <v>6.7774479999999997</v>
       </c>
       <c r="P30">
-        <v>68227531.341561005</v>
+        <v>68285757.315986007</v>
       </c>
       <c r="AP30" s="1"/>
       <c r="AQ30" s="1"/>
@@ -2099,7 +2099,7 @@
         <v>6.7686270000000004</v>
       </c>
       <c r="P31">
-        <v>67638265.206053004</v>
+        <v>67697422.014929995</v>
       </c>
       <c r="AP31" s="1"/>
       <c r="AQ31" s="1"/>
@@ -2152,7 +2152,7 @@
         <v>6.7603150000000003</v>
       </c>
       <c r="P32">
-        <v>67108499.174576998</v>
+        <v>67168548.667181998</v>
       </c>
       <c r="AP32" s="1"/>
       <c r="AQ32" s="1"/>
@@ -2207,7 +2207,7 @@
         <v>6.752491</v>
       </c>
       <c r="P33">
-        <v>66650104.6219</v>
+        <v>66711008.779812999</v>
       </c>
       <c r="AP33" s="1"/>
       <c r="AQ33" s="1"/>
@@ -2262,7 +2262,7 @@
         <v>6.7451369999999997</v>
       </c>
       <c r="P34">
-        <v>66268825.539052002</v>
+        <v>66330549.079334997</v>
       </c>
       <c r="AP34" s="1"/>
       <c r="AQ34" s="1"/>
@@ -2317,7 +2317,7 @@
         <v>6.7382359999999997</v>
       </c>
       <c r="P35">
-        <v>65967008.348159999</v>
+        <v>66029520.034904003</v>
       </c>
       <c r="AP35" s="1"/>
       <c r="AQ35" s="1"/>
@@ -2372,7 +2372,7 @@
         <v>6.73177</v>
       </c>
       <c r="P36">
-        <v>65745654.852486998</v>
+        <v>65808927.824181996</v>
       </c>
       <c r="AP36" s="1"/>
       <c r="AQ36" s="1"/>
@@ -2427,7 +2427,7 @@
         <v>6.7257230000000003</v>
       </c>
       <c r="P37">
-        <v>65605579.714488</v>
+        <v>65669591.213155001</v>
       </c>
       <c r="AP37" s="1"/>
       <c r="AQ37" s="1"/>
@@ -2482,7 +2482,7 @@
         <v>6.7200800000000003</v>
       </c>
       <c r="P38">
-        <v>65547744.290321998</v>
+        <v>65612475.146135002</v>
       </c>
       <c r="W38" s="1"/>
       <c r="X38" s="1"/>
@@ -2539,7 +2539,7 @@
         <v>6.7148240000000001</v>
       </c>
       <c r="P39">
-        <v>65573013.037061997</v>
+        <v>65638447.164852999</v>
       </c>
       <c r="W39" s="1"/>
       <c r="X39" s="1"/>
@@ -2596,7 +2596,7 @@
         <v>6.7099419999999999</v>
       </c>
       <c r="P40">
-        <v>65681636.417563997</v>
+        <v>65747760.463538997</v>
       </c>
       <c r="S40" s="1"/>
       <c r="T40" s="1"/>
@@ -2657,7 +2657,7 @@
         <v>6.705419</v>
       </c>
       <c r="P41">
-        <v>65872731.367953002</v>
+        <v>65939534.539774999</v>
       </c>
       <c r="S41" s="1"/>
       <c r="T41" s="1"/>
@@ -2718,7 +2718,7 @@
         <v>6.7012409999999996</v>
       </c>
       <c r="P42">
-        <v>66143944.387457997</v>
+        <v>66211418.427576996</v>
       </c>
       <c r="S42" s="1"/>
       <c r="T42" s="1"/>
@@ -2779,7 +2779,7 @@
         <v>6.6973950000000002</v>
       </c>
       <c r="P43">
-        <v>66491379.805575997</v>
+        <v>66559519.032063</v>
       </c>
       <c r="S43" s="1"/>
       <c r="T43" s="1"/>
@@ -2840,7 +2840,7 @@
         <v>6.6938700000000004</v>
       </c>
       <c r="P44">
-        <v>66909785.064098999</v>
+        <v>66978586.400716998</v>
       </c>
       <c r="S44" s="1"/>
       <c r="T44" s="1"/>
@@ -2901,7 +2901,7 @@
         <v>6.690652</v>
       </c>
       <c r="P45">
-        <v>67392922.626682997</v>
+        <v>67462385.564109996</v>
       </c>
       <c r="S45" s="1"/>
       <c r="T45" s="1"/>
@@ -2962,7 +2962,7 @@
         <v>6.687729</v>
       </c>
       <c r="P46">
-        <v>67934029.740020007</v>
+        <v>68004156.200709</v>
       </c>
       <c r="S46" s="1"/>
       <c r="T46" s="1"/>
@@ -3023,7 +3023,7 @@
         <v>6.685092</v>
       </c>
       <c r="P47">
-        <v>68526269.138306007</v>
+        <v>68597063.247696996</v>
       </c>
       <c r="S47" s="1"/>
       <c r="T47" s="1"/>
@@ -3084,7 +3084,7 @@
         <v>6.6827290000000001</v>
       </c>
       <c r="P48">
-        <v>69163096.865693003</v>
+        <v>69234564.654938996</v>
       </c>
       <c r="S48" s="1"/>
       <c r="T48" s="1"/>
@@ -3145,7 +3145,7 @@
         <v>6.6806299999999998</v>
       </c>
       <c r="P49">
-        <v>69838506.696700007</v>
+        <v>69910655.773525</v>
       </c>
       <c r="S49" s="1"/>
       <c r="T49" s="1"/>
@@ -3206,7 +3206,7 @@
         <v>6.6787850000000004</v>
       </c>
       <c r="P50">
-        <v>70547144.091484994</v>
+        <v>70619983.316396996</v>
       </c>
       <c r="S50" s="1"/>
       <c r="T50" s="1"/>
@@ -3267,7 +3267,7 @@
         <v>6.6771839999999996</v>
       </c>
       <c r="P51">
-        <v>71284308.948645994</v>
+        <v>71357848.146308005</v>
       </c>
       <c r="S51" s="1"/>
       <c r="T51" s="1"/>
@@ -3328,7 +3328,7 @@
         <v>6.6758189999999997</v>
       </c>
       <c r="P52">
-        <v>72045881.885014996</v>
+        <v>72120131.608759999</v>
       </c>
       <c r="S52" s="1"/>
       <c r="T52" s="1"/>
@@ -3387,7 +3387,7 @@
         <v>6.6746800000000004</v>
       </c>
       <c r="P53">
-        <v>72828213.017018005</v>
+        <v>72903184.371996</v>
       </c>
       <c r="S53" s="1"/>
       <c r="T53" s="1"/>
@@ -3446,7 +3446,7 @@
         <v>6.6737599999999997</v>
       </c>
       <c r="P54">
-        <v>73628007.393234</v>
+        <v>73703711.913380995</v>
       </c>
       <c r="S54" s="1"/>
       <c r="T54" s="1"/>
@@ -3505,7 +3505,7 @@
         <v>6.6730499999999999</v>
       </c>
       <c r="P55">
-        <v>74442230.842821002</v>
+        <v>74518680.410169005</v>
       </c>
       <c r="S55" s="1"/>
       <c r="T55" s="1"/>
@@ -3564,7 +3564,7 @@
         <v>6.6725440000000003</v>
       </c>
       <c r="P56">
-        <v>75268047.795515001</v>
+        <v>75345254.587752998</v>
       </c>
       <c r="S56" s="1"/>
       <c r="T56" s="1"/>
@@ -3623,7 +3623,7 @@
         <v>6.6722320000000002</v>
       </c>
       <c r="P57">
-        <v>76102791.688314006</v>
+        <v>76180768.141354993</v>
       </c>
       <c r="S57" s="1"/>
       <c r="T57" s="1"/>
@@ -3682,7 +3682,7 @@
         <v>6.6721089999999998</v>
       </c>
       <c r="P58">
-        <v>76943960.859136999</v>
+        <v>77022719.634525999</v>
       </c>
       <c r="AP58" s="1"/>
       <c r="AQ58" s="1"/>
@@ -3739,7 +3739,7 @@
         <v>6.6721680000000001</v>
       </c>
       <c r="P59">
-        <v>77789229.053147003</v>
+        <v>77868783.004203007</v>
       </c>
       <c r="AP59" s="1"/>
       <c r="AQ59" s="1"/>
@@ -3796,7 +3796,7 @@
         <v>6.6724019999999999</v>
       </c>
       <c r="P60">
-        <v>78636459.496381</v>
+        <v>78716821.63087</v>
       </c>
       <c r="AP60" s="1"/>
       <c r="AQ60" s="1"/>
@@ -3853,7 +3853,7 @@
         <v>6.6728059999999996</v>
       </c>
       <c r="P61">
-        <v>79483713.904179007</v>
+        <v>79564897.344260007</v>
       </c>
       <c r="AP61" s="1"/>
       <c r="AQ61" s="1"/>
@@ -3910,7 +3910,7 @@
         <v>6.6733719999999996</v>
       </c>
       <c r="P62">
-        <v>80329251.499308005</v>
+        <v>80411269.441192001</v>
       </c>
       <c r="AP62" s="1"/>
       <c r="AQ62" s="1"/>
@@ -3967,7 +3967,7 @@
         <v>6.6740969999999997</v>
       </c>
       <c r="P63">
-        <v>81171516.915062994</v>
+        <v>81254382.591279</v>
       </c>
       <c r="AP63" s="1"/>
       <c r="AQ63" s="1"/>
@@ -4024,7 +4024,7 @@
         <v>6.6749729999999996</v>
       </c>
       <c r="P64">
-        <v>82009118.874816</v>
+        <v>82092845.521477997</v>
       </c>
       <c r="AP64" s="1"/>
       <c r="AQ64" s="1"/>
@@ -4081,7 +4081,7 @@
         <v>6.6759969999999997</v>
       </c>
       <c r="P65">
-        <v>82840803.318476006</v>
+        <v>82925404.148910001</v>
       </c>
       <c r="AP65" s="1"/>
       <c r="AQ65" s="1"/>
@@ -4138,7 +4138,7 @@
         <v>6.6771640000000003</v>
       </c>
       <c r="P66">
-        <v>83665425.137450993</v>
+        <v>83750913.322385997</v>
       </c>
       <c r="AP66" s="1"/>
       <c r="AQ66" s="1"/>
@@ -4193,7 +4193,7 @@
         <v>6.6784670000000004</v>
       </c>
       <c r="P67">
-        <v>84481922.130888</v>
+        <v>84568310.784402996</v>
       </c>
       <c r="AP67" s="1"/>
       <c r="AQ67" s="1"/>
@@ -4248,7 +4248,7 @@
         <v>6.6799049999999998</v>
       </c>
       <c r="P68">
-        <v>85289293.614041001</v>
+        <v>85376595.783842996</v>
       </c>
       <c r="AP68" s="1"/>
       <c r="AQ68" s="1"/>
@@ -4303,7 +4303,7 @@
         <v>6.6814710000000002</v>
       </c>
       <c r="P69">
-        <v>86086584.725652993</v>
+        <v>86174813.386032</v>
       </c>
       <c r="AP69" s="1"/>
       <c r="AQ69" s="1"/>
@@ -4358,7 +4358,7 @@
         <v>6.6831620000000003</v>
       </c>
       <c r="P70">
-        <v>86872876.248839006</v>
+        <v>86962044.294775993</v>
       </c>
       <c r="AP70" s="1"/>
       <c r="AQ70" s="1"/>
@@ -4413,7 +4413,7 @@
         <v>6.6849740000000004</v>
       </c>
       <c r="P71">
-        <v>87647278.900149003</v>
+        <v>87737399.141404003</v>
       </c>
       <c r="AP71" s="1"/>
       <c r="AQ71" s="1"/>
@@ -4468,7 +4468,7 @@
         <v>6.686903</v>
       </c>
       <c r="P72">
-        <v>88408930.631889999</v>
+        <v>88500015.786390007</v>
       </c>
       <c r="AP72" s="1"/>
       <c r="AQ72" s="1"/>
@@ -4523,7 +4523,7 @@
         <v>6.6889459999999996</v>
       </c>
       <c r="P73">
-        <v>89156995.491971001</v>
+        <v>89249058.178223997</v>
       </c>
       <c r="AP73" s="1"/>
       <c r="AQ73" s="1"/>
@@ -4576,7 +4576,7 @@
         <v>6.6910999999999996</v>
       </c>
       <c r="P74">
-        <v>89890662.875899002</v>
+        <v>89983715.604534</v>
       </c>
       <c r="AP74" s="1"/>
       <c r="AQ74" s="1"/>
@@ -4629,7 +4629,7 @@
         <v>6.6933610000000003</v>
       </c>
       <c r="P75">
-        <v>90609146.440864995</v>
+        <v>90703201.605596006</v>
       </c>
       <c r="AP75" s="1"/>
       <c r="AQ75" s="1"/>
@@ -4682,7 +4682,7 @@
         <v>6.6957259999999996</v>
       </c>
       <c r="P76">
-        <v>91311682.397202998</v>
+        <v>91406752.265554994</v>
       </c>
       <c r="AP76" s="1"/>
       <c r="AQ76" s="1"/>
@@ -4735,7 +4735,7 @@
         <v>6.6981929999999998</v>
       </c>
       <c r="P77">
-        <v>91997527.250020996</v>
+        <v>92093623.954166993</v>
       </c>
       <c r="AP77" s="1"/>
       <c r="AQ77" s="1"/>
@@ -4788,7 +4788,7 @@
         <v>6.7007580000000004</v>
       </c>
       <c r="P78">
-        <v>92665955.283508003</v>
+        <v>92763090.811416999</v>
       </c>
       <c r="AP78" s="1"/>
       <c r="AQ78" s="1"/>
@@ -4841,7 +4841,7 @@
         <v>6.7034200000000004</v>
       </c>
       <c r="P79">
-        <v>93316256.156391993</v>
+        <v>93414442.343383998</v>
       </c>
       <c r="AP79" s="1"/>
       <c r="AQ79" s="1"/>
@@ -4894,7 +4894,7 @@
         <v>6.706175</v>
       </c>
       <c r="P80">
-        <v>93947732.936560005</v>
+        <v>94046981.457251996</v>
       </c>
       <c r="AP80" s="1"/>
       <c r="AQ80" s="1"/>
@@ -4947,7 +4947,7 @@
         <v>6.709022</v>
       </c>
       <c r="P81">
-        <v>94559700.790041</v>
+        <v>94660023.150591001</v>
       </c>
       <c r="AP81" s="1"/>
       <c r="AQ81" s="1"/>
@@ -5000,7 +5000,7 @@
         <v>6.7119580000000001</v>
       </c>
       <c r="P82">
-        <v>95151486.401362002</v>
+        <v>95252893.931888998</v>
       </c>
       <c r="AP82" s="1"/>
       <c r="AQ82" s="1"/>
@@ -5053,7 +5053,7 @@
         <v>6.7149799999999997</v>
       </c>
       <c r="P83">
-        <v>95722428.077230006</v>
+        <v>95824931.924281999</v>
       </c>
       <c r="AP83" s="1"/>
       <c r="AQ83" s="1"/>
@@ -5106,7 +5106,7 @@
         <v>6.7180879999999998</v>
       </c>
       <c r="P84">
-        <v>96271876.397734001</v>
+        <v>96375487.516725004</v>
       </c>
       <c r="AP84" s="1"/>
       <c r="AQ84" s="1"/>
@@ -5159,7 +5159,7 @@
         <v>6.7212779999999999</v>
       </c>
       <c r="P85">
-        <v>96799195.237954006</v>
+        <v>96903924.385521993</v>
       </c>
       <c r="AP85" s="1"/>
       <c r="AQ85" s="1"/>
@@ -5212,7 +5212,7 @@
         <v>6.7245499999999998</v>
       </c>
       <c r="P86">
-        <v>97303762.984086007</v>
+        <v>97409620.710366994</v>
       </c>
       <c r="AP86" s="1"/>
       <c r="AQ86" s="1"/>
@@ -5265,7 +5265,7 @@
         <v>6.7279010000000001</v>
       </c>
       <c r="P87">
-        <v>97784973.800134003</v>
+        <v>97891970.441001996</v>
       </c>
       <c r="AP87" s="1"/>
       <c r="AQ87" s="1"/>
@@ -5318,7 +5318,7 @@
         <v>6.731331</v>
       </c>
       <c r="P88">
-        <v>98242238.848814994</v>
+        <v>98350384.518135995</v>
       </c>
       <c r="AP88" s="1"/>
       <c r="AQ88" s="1"/>
@@ -5371,7 +5371,7 @@
         <v>6.7348359999999996</v>
       </c>
       <c r="P89">
-        <v>98674987.419439003</v>
+        <v>98784292.001402006</v>
       </c>
       <c r="AP89" s="1"/>
       <c r="AQ89" s="1"/>
@@ -5424,7 +5424,7 @@
         <v>6.738416</v>
       </c>
       <c r="P90">
-        <v>99082667.955914006</v>
+        <v>99193141.097519994</v>
       </c>
       <c r="AP90" s="1"/>
       <c r="AQ90" s="1"/>
@@ -5477,7 +5477,7 @@
         <v>6.74207</v>
       </c>
       <c r="P91">
-        <v>99464749.004245996</v>
+        <v>99576400.107986003</v>
       </c>
       <c r="AP91" s="1"/>
       <c r="AQ91" s="1"/>
@@ -5530,7 +5530,7 @@
         <v>6.7457960000000003</v>
       </c>
       <c r="P92">
-        <v>99820720.110009</v>
+        <v>99933558.326784</v>
       </c>
       <c r="AP92" s="1"/>
       <c r="AQ92" s="1"/>
@@ -5583,7 +5583,7 @@
         <v>6.749593</v>
       </c>
       <c r="P93">
-        <v>100150092.694903</v>
+        <v>100264126.9172</v>
       </c>
       <c r="AP93" s="1"/>
       <c r="AQ93" s="1"/>
@@ -5636,7 +5636,7 @@
         <v>6.7534590000000003</v>
       </c>
       <c r="P94">
-        <v>100452400.931989</v>
+        <v>100567639.78734399</v>
       </c>
       <c r="AP94" s="1"/>
       <c r="AQ94" s="1"/>
@@ -5689,7 +5689,7 @@
         <v>6.7573939999999997</v>
       </c>
       <c r="P95">
-        <v>100727202.62637</v>
+        <v>100843654.471109</v>
       </c>
       <c r="AP95" s="1"/>
       <c r="AQ95" s="1"/>
@@ -5742,7 +5742,7 @@
         <v>6.7613960000000004</v>
       </c>
       <c r="P96">
-        <v>100974080.09583201</v>
+        <v>101091753.009115</v>
       </c>
       <c r="AP96" s="1"/>
       <c r="AQ96" s="1"/>
@@ -5795,7 +5795,7 @@
         <v>6.7654639999999997</v>
       </c>
       <c r="P97">
-        <v>101192641.03707699</v>
+        <v>101311542.815247</v>
       </c>
       <c r="AP97" s="1"/>
       <c r="AQ97" s="1"/>
@@ -5848,7 +5848,7 @@
         <v>6.7695980000000002</v>
       </c>
       <c r="P98">
-        <v>101382519.35861</v>
+        <v>101502657.509858</v>
       </c>
       <c r="AP98" s="1"/>
       <c r="AQ98" s="1"/>
@@ -5901,7 +5901,7 @@
         <v>6.7737959999999999</v>
       </c>
       <c r="P99">
-        <v>101543375.961037</v>
+        <v>101664757.700403</v>
       </c>
       <c r="AP99" s="1"/>
       <c r="AQ99" s="1"/>
@@ -5954,7 +5954,7 @@
         <v>6.7780570000000004</v>
       </c>
       <c r="P100">
-        <v>101674899.448379</v>
+        <v>101797531.693113</v>
       </c>
       <c r="AP100" s="1"/>
       <c r="AQ100" s="1"/>
@@ -6007,7 +6007,7 @@
         <v>6.782381</v>
       </c>
       <c r="P101">
-        <v>101776806.758644</v>
+        <v>101900696.123935</v>
       </c>
       <c r="AP101" s="1"/>
       <c r="AQ101" s="1"/>
@@ -6060,7 +6060,7 @@
         <v>6.7867670000000002</v>
       </c>
       <c r="P102">
-        <v>101848843.706908</v>
+        <v>101973996.502013</v>
       </c>
       <c r="AP102" s="1"/>
       <c r="AQ102" s="1"/>
@@ -6113,7 +6113,7 @@
         <v>6.7912129999999999</v>
       </c>
       <c r="P103">
-        <v>101890785.438538</v>
+        <v>102017207.66332801</v>
       </c>
       <c r="AP103" s="1"/>
       <c r="AQ103" s="1"/>
@@ -6166,7 +6166,7 @@
         <v>6.7957200000000002</v>
       </c>
       <c r="P104">
-        <v>101902436.79333401</v>
+        <v>102030134.135267</v>
       </c>
       <c r="AP104" s="1"/>
       <c r="AQ104" s="1"/>
@@ -6219,7 +6219,7 @@
         <v>6.8002849999999997</v>
       </c>
       <c r="P105">
-        <v>101883632.583055</v>
+        <v>102012610.414601</v>
       </c>
       <c r="AP105" s="1"/>
       <c r="AQ105" s="1"/>
@@ -6272,7 +6272,7 @@
         <v>6.8049090000000003</v>
       </c>
       <c r="P106">
-        <v>101834237.78532501</v>
+        <v>101964501.161854</v>
       </c>
       <c r="AP106" s="1"/>
       <c r="AQ106" s="1"/>
@@ -6325,7 +6325,7 @@
         <v>6.8095910000000002</v>
       </c>
       <c r="P107">
-        <v>101754147.656532</v>
+        <v>101885701.31466299</v>
       </c>
       <c r="AP107" s="1"/>
       <c r="AQ107" s="1"/>
@@ -6378,7 +6378,7 @@
         <v>6.81433</v>
       </c>
       <c r="P108">
-        <v>101643287.76554</v>
+        <v>101776136.121978</v>
       </c>
       <c r="AP108" s="1"/>
       <c r="AQ108" s="1"/>
@@ -6431,7 +6431,7 @@
         <v>6.8191249999999997</v>
       </c>
       <c r="P109">
-        <v>101501613.949265</v>
+        <v>101635761.10010999</v>
       </c>
       <c r="AP109" s="1"/>
       <c r="AQ109" s="1"/>
@@ -6484,7 +6484,7 @@
         <v>6.823976</v>
       </c>
       <c r="P110">
-        <v>101329112.19053601</v>
+        <v>101464561.91109399</v>
       </c>
       <c r="AP110" s="1"/>
       <c r="AQ110" s="1"/>
@@ -6537,7 +6537,7 @@
         <v>6.828881</v>
       </c>
       <c r="P111">
-        <v>101125798.41851801</v>
+        <v>101262554.16359299</v>
       </c>
       <c r="AP111" s="1"/>
       <c r="AQ111" s="1"/>
@@ -6590,7 +6590,7 @@
         <v>6.8338409999999996</v>
       </c>
       <c r="P112">
-        <v>100891718.232095</v>
+        <v>101029783.136774</v>
       </c>
       <c r="AP112" s="1"/>
       <c r="AQ112" s="1"/>
@@ -6643,7 +6643,7 @@
         <v>6.8388540000000004</v>
       </c>
       <c r="P113">
-        <v>100626946.547124</v>
+        <v>100766323.428065</v>
       </c>
       <c r="AP113" s="1"/>
       <c r="AQ113" s="1"/>
@@ -6696,7 +6696,7 @@
         <v>6.8439199999999998</v>
       </c>
       <c r="P114">
-        <v>100331587.16914199</v>
+        <v>100472278.526344</v>
       </c>
       <c r="AP114" s="1"/>
       <c r="AQ114" s="1"/>
@@ -6749,7 +6749,7 @@
         <v>6.8490380000000002</v>
       </c>
       <c r="P115">
-        <v>100005772.293795</v>
+        <v>100147780.312867</v>
       </c>
       <c r="AP115" s="1"/>
       <c r="AQ115" s="1"/>
@@ -6802,7 +6802,7 @@
         <v>6.8542079999999999</v>
       </c>
       <c r="P116">
-        <v>99649661.937995002</v>
+        <v>99792988.492908001</v>
       </c>
       <c r="AP116" s="1"/>
       <c r="AQ116" s="1"/>
@@ -6855,7 +6855,7 @@
         <v>6.8594290000000004</v>
       </c>
       <c r="P117">
-        <v>99263443.305324003</v>
+        <v>99408089.961647004</v>
       </c>
       <c r="AP117" s="1"/>
       <c r="AQ117" s="1"/>
@@ -6908,7 +6908,7 @@
         <v>6.8646989999999999</v>
       </c>
       <c r="P118">
-        <v>98847330.089675993</v>
+        <v>98993298.108280003</v>
       </c>
       <c r="AP118" s="1"/>
       <c r="AQ118" s="1"/>
@@ -6961,7 +6961,7 @@
         <v>6.8700200000000002</v>
       </c>
       <c r="P119">
-        <v>98401561.721385002</v>
+        <v>98548852.062619001</v>
       </c>
       <c r="AP119" s="1"/>
       <c r="AQ119" s="1"/>
@@ -7014,7 +7014,7 @@
         <v>6.8753890000000002</v>
       </c>
       <c r="P120">
-        <v>97926402.560293004</v>
+        <v>98075015.888607994</v>
       </c>
       <c r="AP120" s="1"/>
       <c r="AQ120" s="1"/>
@@ -7067,7 +7067,7 @@
         <v>6.8808059999999998</v>
       </c>
       <c r="P121">
-        <v>97422141.040292993</v>
+        <v>97572077.729305997</v>
       </c>
       <c r="AP121" s="1"/>
       <c r="AQ121" s="1"/>
@@ -7120,7 +7120,7 @@
         <v>6.8862709999999998</v>
       </c>
       <c r="P122">
-        <v>96889088.769942001</v>
+        <v>97040348.907931998</v>
       </c>
       <c r="AP122" s="1"/>
       <c r="AQ122" s="1"/>
@@ -7173,7 +7173,7 @@
         <v>6.8917820000000001</v>
       </c>
       <c r="P123">
-        <v>96327579.593776003</v>
+        <v>96480162.989582002</v>
       </c>
       <c r="AP123" s="1"/>
       <c r="AQ123" s="1"/>
@@ -7226,7 +7226,7 @@
         <v>6.8973389999999997</v>
       </c>
       <c r="P124">
-        <v>95737968.618974999</v>
+        <v>95891874.808292001</v>
       </c>
       <c r="AP124" s="1"/>
       <c r="AQ124" s="1"/>
@@ -7279,7 +7279,7 @@
         <v>6.9029420000000004</v>
       </c>
       <c r="P125">
-        <v>95120631.212064996</v>
+        <v>95275859.464111999</v>
       </c>
       <c r="AP125" s="1"/>
       <c r="AQ125" s="1"/>
@@ -7332,7 +7332,7 @@
         <v>6.9085900000000002</v>
       </c>
       <c r="P126">
-        <v>94475961.970367</v>
+        <v>94632511.294909999</v>
       </c>
       <c r="AP126" s="1"/>
       <c r="AQ126" s="1"/>
@@ -7385,7 +7385,7 @@
         <v>6.9142809999999999</v>
       </c>
       <c r="P127">
-        <v>93804373.672895998</v>
+        <v>93962242.827601999</v>
       </c>
       <c r="AP127" s="1"/>
       <c r="AQ127" s="1"/>
@@ -7438,7 +7438,7 @@
         <v>6.9200150000000002</v>
       </c>
       <c r="P128">
-        <v>93106296.215432003</v>
+        <v>93265483.713533998</v>
       </c>
       <c r="AP128" s="1"/>
       <c r="AQ128" s="1"/>
@@ -7491,7 +7491,7 @@
         <v>6.9257920000000004</v>
       </c>
       <c r="P129">
-        <v>92382175.534427002</v>
+        <v>92542679.652675003</v>
       </c>
       <c r="AP129" s="1"/>
       <c r="AQ129" s="1"/>
@@ -7544,7 +7544,7 @@
         <v>6.9316110000000002</v>
       </c>
       <c r="P130">
-        <v>91632472.524350002</v>
+        <v>91794291.311225995</v>
       </c>
       <c r="AP130" s="1"/>
       <c r="AQ130" s="1"/>
@@ -7597,7 +7597,7 @@
         <v>6.9374700000000002</v>
       </c>
       <c r="P131">
-        <v>90857661.952960998</v>
+        <v>91020793.237129003</v>
       </c>
       <c r="AP131" s="1"/>
       <c r="AQ131" s="1"/>
@@ -7650,7 +7650,7 @@
         <v>6.9433699999999998</v>
       </c>
       <c r="P132">
-        <v>90058231.378874004</v>
+        <v>90222672.777842999</v>
       </c>
       <c r="AP132" s="1"/>
       <c r="AQ132" s="1"/>
@@ -7703,7 +7703,7 @@
         <v>6.9493080000000003</v>
       </c>
       <c r="P133">
-        <v>89234680.075579002</v>
+        <v>89400429.004549995</v>
       </c>
       <c r="AP133" s="1"/>
       <c r="AQ133" s="1"/>
@@ -7756,7 +7756,7 @@
         <v>6.9552860000000001</v>
       </c>
       <c r="P134">
-        <v>88387517.965910003</v>
+        <v>88554571.646781996</v>
       </c>
       <c r="AP134" s="1"/>
       <c r="AQ134" s="1"/>
@@ -7809,7 +7809,7 @@
         <v>6.9613009999999997</v>
       </c>
       <c r="P135">
-        <v>87517264.570720002</v>
+        <v>87685620.041225001</v>
       </c>
       <c r="AP135" s="1"/>
       <c r="AQ135" s="1"/>
@@ -7862,7 +7862,7 @@
         <v>6.9673530000000001</v>
       </c>
       <c r="P136">
-        <v>86624447.975272998</v>
+        <v>86794102.098214</v>
       </c>
       <c r="AP136" s="1"/>
       <c r="AQ136" s="1"/>
@@ -7915,7 +7915,7 @@
         <v>6.9734410000000002</v>
       </c>
       <c r="P137">
-        <v>85709603.816626996</v>
+        <v>85880553.289196</v>
       </c>
       <c r="AP137" s="1"/>
       <c r="AQ137" s="1"/>
@@ -7968,7 +7968,7 @@
         <v>6.9795639999999999</v>
       </c>
       <c r="P138">
-        <v>84773274.295013994</v>
+        <v>84945515.658148006</v>
       </c>
       <c r="AP138" s="1"/>
       <c r="AQ138" s="1"/>
@@ -8021,7 +8021,7 @@
         <v>6.985722</v>
       </c>
       <c r="P139">
-        <v>83816007.211940005</v>
+        <v>83989536.859713003</v>
       </c>
       <c r="AP139" s="1"/>
       <c r="AQ139" s="1"/>
@@ -8074,7 +8074,7 @@
         <v>6.9919130000000003</v>
       </c>
       <c r="P140">
-        <v>82838355.037488997</v>
+        <v>83013169.226481006</v>
       </c>
       <c r="AP140" s="1"/>
       <c r="AQ140" s="1"/>
@@ -8127,7 +8127,7 @@
         <v>6.9981369999999998</v>
       </c>
       <c r="P141">
-        <v>81840874.008987993</v>
+        <v>82016968.867633998</v>
       </c>
       <c r="AP141" s="1"/>
       <c r="AQ141" s="1"/>
@@ -8180,7 +8180,7 @@
         <v>7.0043930000000003</v>
       </c>
       <c r="P142">
-        <v>80824123.262950003</v>
+        <v>81001494.800823003</v>
       </c>
       <c r="AP142" s="1"/>
       <c r="AQ142" s="1"/>
@@ -8233,7 +8233,7 @@
         <v>7.0106799999999998</v>
       </c>
       <c r="P143">
-        <v>79788664.001926005</v>
+        <v>79967308.118939996</v>
       </c>
       <c r="AP143" s="1"/>
       <c r="AQ143" s="1"/>
@@ -8286,7 +8286,7 @@
         <v>7.0169959999999998</v>
       </c>
       <c r="P144">
-        <v>78735058.697602004</v>
+        <v>78914971.193102002</v>
       </c>
       <c r="AP144" s="1"/>
       <c r="AQ144" s="1"/>
@@ -8339,7 +8339,7 @@
         <v>7.0233420000000004</v>
       </c>
       <c r="P145">
-        <v>77663870.33123</v>
+        <v>77845046.912952006</v>
       </c>
       <c r="AP145" s="1"/>
       <c r="AQ145" s="1"/>
@@ -8392,7 +8392,7 @@
         <v>7.0297159999999996</v>
       </c>
       <c r="P146">
-        <v>76575661.672195002</v>
+        <v>76758097.965074003</v>
       </c>
       <c r="AP146" s="1"/>
       <c r="AQ146" s="1"/>
@@ -8445,7 +8445,7 @@
         <v>7.0361180000000001</v>
       </c>
       <c r="P147">
-        <v>75470994.595281005</v>
+        <v>75654686.150074005</v>
       </c>
       <c r="AP147" s="1"/>
       <c r="AQ147" s="1"/>
@@ -8498,7 +8498,7 @@
         <v>7.0425449999999996</v>
       </c>
       <c r="P148">
-        <v>74350429.436939001</v>
+        <v>74535371.738656998</v>
       </c>
       <c r="AP148" s="1"/>
       <c r="AQ148" s="1"/>
@@ -8551,7 +8551,7 @@
         <v>7.0489990000000002</v>
       </c>
       <c r="P149">
-        <v>73214524.390615001</v>
+        <v>73400712.866736993</v>
       </c>
       <c r="AP149" s="1"/>
       <c r="AQ149" s="1"/>
@@ -8604,7 +8604,7 @@
         <v>7.0554769999999998</v>
       </c>
       <c r="P150">
-        <v>72063834.941009</v>
+        <v>72251264.969458997</v>
       </c>
       <c r="AP150" s="1"/>
       <c r="AQ150" s="1"/>
@@ -8657,7 +8657,7 @@
         <v>7.0619779999999999</v>
       </c>
       <c r="P151">
-        <v>70898913.336869001</v>
+        <v>71087580.253748</v>
       </c>
       <c r="AP151" s="1"/>
       <c r="AQ151" s="1"/>
@@ -8710,7 +8710,7 @@
         <v>7.0685029999999998</v>
       </c>
       <c r="P152">
-        <v>69720308.101795003</v>
+        <v>69910207.208836004</v>
       </c>
       <c r="AP152" s="1"/>
       <c r="AQ152" s="1"/>
@@ -8763,7 +8763,7 @@
         <v>7.0750489999999999</v>
       </c>
       <c r="P153">
-        <v>68528563.582288995</v>
+        <v>68719690.154042006</v>
       </c>
       <c r="AP153" s="1"/>
       <c r="AQ153" s="1"/>
@@ -8816,7 +8816,7 @@
         <v>7.0816160000000004</v>
       </c>
       <c r="P154">
-        <v>67324219.532162994</v>
+        <v>67516568.822882995</v>
       </c>
       <c r="AP154" s="1"/>
       <c r="AQ154" s="1"/>
@@ -8869,7 +8869,7 @@
         <v>7.088203</v>
       </c>
       <c r="P155">
-        <v>66107810.732262</v>
+        <v>66301377.982492998</v>
       </c>
       <c r="AP155" s="1"/>
       <c r="AQ155" s="1"/>
@@ -8922,7 +8922,7 @@
         <v>7.0948089999999997</v>
       </c>
       <c r="P156">
-        <v>64879866.644317001</v>
+        <v>65074647.087163001</v>
       </c>
       <c r="AP156" s="1"/>
       <c r="AQ156" s="1"/>
@@ -8975,7 +8975,7 @@
         <v>7.1014330000000001</v>
       </c>
       <c r="P157">
-        <v>63640911.097646996</v>
+        <v>63836899.964726001</v>
       </c>
       <c r="AP157" s="1"/>
       <c r="AQ157" s="1"/>
@@ -9028,7 +9028,7 @@
         <v>7.1080740000000002</v>
       </c>
       <c r="P158">
-        <v>62391462.007316001</v>
+        <v>62588654.534385003</v>
       </c>
       <c r="AP158" s="1"/>
       <c r="AQ158" s="1"/>
@@ -9081,7 +9081,7 @@
         <v>7.1147309999999999</v>
       </c>
       <c r="P159">
-        <v>61132031.122290999</v>
+        <v>61330422.554537997</v>
       </c>
       <c r="AP159" s="1"/>
       <c r="AQ159" s="1"/>
@@ -9134,7 +9134,7 @@
         <v>7.1214040000000001</v>
       </c>
       <c r="P160">
-        <v>59863123.802061997</v>
+        <v>60062709.399065003</v>
       </c>
       <c r="AP160" s="1"/>
       <c r="AQ160" s="1"/>
@@ -9187,7 +9187,7 @@
         <v>7.1280910000000004</v>
       </c>
       <c r="P161">
-        <v>58585238.820138998</v>
+        <v>58786013.860487998</v>
       </c>
       <c r="AP161" s="1"/>
       <c r="AQ161" s="1"/>

</xml_diff>